<commit_message>
Fix issues #16 #26 #29 #27 #28 #21 #15 #36 #35 #34 #13 #18
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpommier/src/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpommier/src/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7DB6656C-4E89-CA41-B2D6-4AA993EC29F6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4468273-A112-1C4C-B668-C6724E3B157D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="480" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="720">
   <si>
     <t>MIAPPE</t>
   </si>
@@ -575,9 +575,6 @@
     <t>License for the reuse of the data associated with this investigation. The Creative Commons licenses cover most use cases and are recommended.</t>
   </si>
   <si>
-    <t>CC BY-SA 4.0 Unreported</t>
-  </si>
-  <si>
     <t>MIAPPE version</t>
   </si>
   <si>
@@ -947,27 +944,12 @@
     <t>Geographic location (altitude)</t>
   </si>
   <si>
-    <t>Altitude of the experimental site, preferably provided in metres (m).</t>
-  </si>
-  <si>
     <t>100m</t>
   </si>
   <si>
-    <t>Description of statistical design</t>
-  </si>
-  <si>
-    <t>Short description of the statistical design.</t>
-  </si>
-  <si>
     <t>Lines were repeated twice at each location using a complete block design. In order to limit competition effects, each block was organized into four sub-blocks corresponding to earliness groups based on a priori information. https://urgi.versailles.inra.fr/files/ephesis/181000503/181000503_plan.xls</t>
   </si>
   <si>
-    <t>Type of statistical design</t>
-  </si>
-  <si>
-    <t>Type of statistical design of the study, in the form of an accession number from the Crop Ontology.</t>
-  </si>
-  <si>
     <t>CO_715:0000145</t>
   </si>
   <si>
@@ -989,16 +971,10 @@
     <t>General description of the observation units in the study.</t>
   </si>
   <si>
-    <t>Observation units consisted in individual plots themselves consisting of a row of 15 plants at a density of approximately six plants per square meter</t>
-  </si>
-  <si>
     <t>Description of growth facility</t>
   </si>
   <si>
     <t>Short description of the facility in which the study was carried out.</t>
-  </si>
-  <si>
-    <t>field environment condition</t>
   </si>
   <si>
     <t>Type of growth facility</t>
@@ -1174,9 +1150,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Species name for  the organism under study, according to standard scientific nomenclature.</t>
-  </si>
-  <si>
     <t>mays; lycosperium x pennellii</t>
   </si>
   <si>
@@ -1201,9 +1174,6 @@
     <t>Biological material altitude</t>
   </si>
   <si>
-    <t>Altitude of the studied biological material, preferably provided in metres (m). [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
     <t>10m</t>
   </si>
   <si>
@@ -1261,9 +1231,6 @@
     <t>Material source altitude</t>
   </si>
   <si>
-    <t>Altitude of the material source, preferably provided in metres (m). [Alternative identifier for in situ material]</t>
-  </si>
-  <si>
     <t>Material source coordinates uncertainty</t>
   </si>
   <si>
@@ -1276,67 +1243,32 @@
     <t>Branches were collected from a 10-year-old tree growing in a progeny trial established in a loamy brown earth soil</t>
   </si>
   <si>
-    <t>An environmental parameters or experimental conditions that was kept constant throughout the study and did not change betweeen observation units or assays.</t>
-  </si>
-  <si>
     <t>0-1 per study</t>
   </si>
   <si>
     <t>Environment parameter</t>
   </si>
   <si>
-    <t>Name of the environment parameter</t>
-  </si>
-  <si>
-    <t>List environmental parameters in attachment to main MIAPPE table.
-Examples: air temperature; rooting medium; medium composition; plot size</t>
-  </si>
-  <si>
     <t>Free text (see Appendix I)</t>
   </si>
   <si>
     <t>Environment parameter value</t>
   </si>
   <si>
-    <t>Value of the environment parameter.</t>
-  </si>
-  <si>
-    <t>Value for each of the above parameters.
-Examples: 22 °C; Ca: 5 mg/L</t>
-  </si>
-  <si>
     <t>1 per parameter</t>
-  </si>
-  <si>
-    <t>Factor</t>
-  </si>
-  <si>
-    <t>The object of a study is to ascertain the impact of one or more factors on the biological material. Thus, a factor is, by definition a condition that varies between observation units, which may be biotic (pest, disease interaction) or abiotic (treatment and cultural practice) in nature.</t>
   </si>
   <si>
     <t>0+ per study;
 0+ per observation unit</t>
   </si>
   <si>
-    <t>Name/Acronym of the factor.</t>
-  </si>
-  <si>
     <t>Watering</t>
   </si>
   <si>
     <t>Free text (see Appendix II)</t>
   </si>
   <si>
-    <t>Factor description</t>
-  </si>
-  <si>
-    <t>Free text description of the factor. This include all relevant treatments planificaito and protocole considered for all the plant targeted by a given factor.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Daily watering 1L per plant. </t>
-  </si>
-  <si>
-    <t>Factor values</t>
   </si>
   <si>
     <t>List of possible values for the factor.</t>
@@ -1532,9 +1464,6 @@
     <t>Observed Variable</t>
   </si>
   <si>
-    <t>An observed variable, typically taking the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement.</t>
-  </si>
-  <si>
     <t>Variable ID</t>
   </si>
   <si>
@@ -2172,6 +2101,110 @@
   </si>
   <si>
     <t>TR-27</t>
+  </si>
+  <si>
+    <t>CC BY-SA 4.0, Unreported</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>DM-44'</t>
+  </si>
+  <si>
+    <t>Infraspecific name</t>
+  </si>
+  <si>
+    <t>Free text, or key value pair list, or MCPD compliant format</t>
+  </si>
+  <si>
+    <t>Name of any subtaxa level, including variety, crossing name, etc....  It can be used to store any additional taxonomic identifier. 
+For Key value pair list format, the Key is the name of the rank)and the valueis the valueof  the rank. Ranks can be among the following terms: subspecies, cultivar, variety, subvariety, convariety, group, subgroup, hybrid, line, form, subform.
+For MCPD compliant format, the following abbreviations are allowed: ‘subsp.’ (subspecies); ‘convar.’ (convariety); ‘var.’ ( variety); ‘f.’ (form); ‘Group’ (cultivar group).).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free text: vinifera Pinot noir | B73
+Key value pair list: subspecies:vinifera ; cultivar:Pinot noir | var:B73
+MCPD: subsp. vinifera var Pinot Noir | var. B73, </t>
+  </si>
+  <si>
+    <t>SSpecies name (formally species epithet) for the organism under study, according to standard scientific nomenclature.</t>
+  </si>
+  <si>
+    <t>Observation units consisted in individual plots themselves consisting of a row of 15 plants at a density of approximately six plants per square meter | NA</t>
+  </si>
+  <si>
+    <t>field environment condition | NA</t>
+  </si>
+  <si>
+    <t>Altitude of the experimental site, provided in metres (m).</t>
+  </si>
+  <si>
+    <t>Numeric + unit abbreviation</t>
+  </si>
+  <si>
+    <t>Altitude of the studied biological material, provided in meters (m). [Alternative identifier for in situ material]</t>
+  </si>
+  <si>
+    <t>Altitude of the material source, provided in metres (m). [Alternative identifier for in situ material]</t>
+  </si>
+  <si>
+    <t>Circular uncertainty of the coordinates, provided in meters (m). [Alternative identifier for in situ material]</t>
+  </si>
+  <si>
+    <t>Type of experimental design</t>
+  </si>
+  <si>
+    <t>Short description of the experimental design, possibly including statistical design. Can be simply 'NA' or 'none' when it doesn't make sense anymore, like for data computed from several studies.</t>
+  </si>
+  <si>
+    <t>Type of esperimental  design of the study, in the form of an accession number from the Crop Ontology.</t>
+  </si>
+  <si>
+    <t>Experimental Factor</t>
+  </si>
+  <si>
+    <t>Experimental Factor type</t>
+  </si>
+  <si>
+    <t>Experimental Factor description</t>
+  </si>
+  <si>
+    <t>Experimental Factor values</t>
+  </si>
+  <si>
+    <t>Name/Acronym of the experimental factor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free text description of the experimental factor. This include all relevant treatments planification and protocol planed for all the plant targeted by a given experimental factor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The object of a study is to ascertain the impact of one or more factors on the biological material. Thus, a factor is, by definition a condition that varies between observation units, which may be biotic (pest, disease interaction) or abiotic (treatment and cultural practice) in nature. Depending on the level of the data, an experimental factor can be either  "what is the factor applied to the plant" (ie Unwatered), or the "environmental characterisation" (ie if no rain on unwatered plant : Drought ;  if rain on unwatered plant: Irrigated) </t>
+  </si>
+  <si>
+    <t>Environmental parameters that was kept constant throughout the study and did not change betweeen observation units or assays. Environment measures that varies over time, ie environmental variables like soil water content, can be recorded as time series of Observed Variables (see below)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the environment parameter, permanent within the experiment. </t>
+  </si>
+  <si>
+    <t>Value of the environment parameter, permanent within the experiment.</t>
+  </si>
+  <si>
+    <t>Value for each of the above parameters.
+Clay 50% plus sand ; Ca: 5 mg/L</t>
+  </si>
+  <si>
+    <t>rooting medium; medium composition; soil reflection</t>
+  </si>
+  <si>
+    <t>An observed variable describe how a measurement has been made. It typically takes the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement.</t>
+  </si>
+  <si>
+    <t>Description of the experimental design</t>
   </si>
 </sst>
 </file>
@@ -2845,11 +2878,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2873,7 +2906,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>539</v>
+        <v>516</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>3</v>
@@ -2893,7 +2926,7 @@
     </row>
     <row r="3" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>11</v>
@@ -2907,9 +2940,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>18</v>
@@ -2927,9 +2960,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A5" s="33" t="s">
-        <v>542</v>
+        <v>519</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>130</v>
@@ -2947,9 +2980,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="84" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="91" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
-        <v>543</v>
+        <v>520</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>136</v>
@@ -2967,9 +3000,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
-        <v>544</v>
+        <v>521</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>153</v>
@@ -2987,9 +3020,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
-        <v>545</v>
+        <v>522</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>173</v>
@@ -3007,9 +3040,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
-        <v>546</v>
+        <v>523</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>180</v>
@@ -3018,7 +3051,7 @@
         <v>181</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>182</v>
+        <v>687</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>44</v>
@@ -3027,74 +3060,74 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
-        <v>547</v>
+        <v>524</v>
       </c>
       <c r="B10" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="15">
-        <v>1.1000000000000001</v>
+      <c r="D10" s="15" t="s">
+        <v>688</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>188</v>
+        <v>689</v>
       </c>
       <c r="F10" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
-        <v>548</v>
+        <v>525</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="F11" s="15" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+      <c r="A12" s="33" t="s">
+        <v>526</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.15">
-      <c r="A12" s="33" t="s">
-        <v>549</v>
-      </c>
-      <c r="B12" s="35" t="s">
+      <c r="C12" s="39" t="s">
         <v>197</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>198</v>
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="41"/>
       <c r="F12" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="33" t="s">
-        <v>550</v>
+        <v>527</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>44</v>
@@ -3103,18 +3136,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="33" t="s">
-        <v>551</v>
+        <v>528</v>
       </c>
       <c r="B14" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>225</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>133</v>
@@ -3123,18 +3156,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A15" s="33" t="s">
-        <v>552</v>
+        <v>529</v>
       </c>
       <c r="B15" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="D15" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>152</v>
@@ -3143,18 +3176,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>553</v>
+        <v>530</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>172</v>
@@ -3163,15 +3196,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="33" t="s">
-        <v>554</v>
+        <v>531</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D17" s="20">
         <v>37587</v>
@@ -3183,18 +3216,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="33" t="s">
-        <v>555</v>
+        <v>532</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>133</v>
@@ -3203,38 +3236,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="33" t="s">
-        <v>556</v>
+        <v>533</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>280</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>281</v>
       </c>
       <c r="F19" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="33" t="s">
-        <v>557</v>
+        <v>534</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>133</v>
@@ -3243,78 +3276,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="33" t="s">
-        <v>558</v>
+        <v>535</v>
       </c>
       <c r="B21" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="11" t="s">
         <v>298</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="F21" s="15" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A22" s="33" t="s">
+        <v>536</v>
+      </c>
+      <c r="B22" s="36" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A22" s="33" t="s">
-        <v>559</v>
-      </c>
-      <c r="B22" s="36" t="s">
+      <c r="C22" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="F22" s="15" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="33" t="s">
+        <v>537</v>
+      </c>
+      <c r="B23" s="36" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="33" t="s">
-        <v>560</v>
-      </c>
-      <c r="B23" s="36" t="s">
+      <c r="C23" s="11" t="s">
+        <v>698</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>307</v>
-      </c>
       <c r="E23" s="11" t="s">
-        <v>99</v>
+        <v>699</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="84" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="91" x14ac:dyDescent="0.15">
       <c r="A24" s="33" t="s">
-        <v>561</v>
+        <v>538</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>308</v>
+        <v>719</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>309</v>
+        <v>704</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>152</v>
@@ -3323,58 +3356,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A25" s="33" t="s">
-        <v>562</v>
+        <v>539</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>311</v>
+        <v>703</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>312</v>
+        <v>705</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="33" t="s">
-        <v>563</v>
+        <v>540</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>537</v>
+        <v>514</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A27" s="33" t="s">
-        <v>564</v>
+        <v>541</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>320</v>
+        <v>696</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>152</v>
@@ -3383,18 +3416,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="33" t="s">
-        <v>565</v>
+        <v>542</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>323</v>
+        <v>697</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>133</v>
@@ -3403,38 +3436,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="33" t="s">
-        <v>566</v>
+        <v>543</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="33" t="s">
-        <v>567</v>
+        <v>544</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>152</v>
@@ -3443,92 +3476,92 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="33" t="s">
-        <v>568</v>
+        <v>545</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="29" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="33" t="s">
-        <v>569</v>
+        <v>546</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="D32" s="40"/>
       <c r="E32" s="41"/>
       <c r="F32" s="6" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A33" s="33" t="s">
-        <v>570</v>
+        <v>547</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="F33" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="33" t="s">
-        <v>571</v>
+        <v>548</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A35" s="33" t="s">
-        <v>572</v>
+        <v>549</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>44</v>
@@ -3537,94 +3570,94 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="33" t="s">
-        <v>573</v>
+        <v>550</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>133</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="33" t="s">
-        <v>574</v>
+        <v>551</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>133</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.15">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A38" s="33" t="s">
-        <v>575</v>
+        <v>552</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D38" s="40"/>
       <c r="E38" s="41"/>
       <c r="F38" s="6" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A39" s="33" t="s">
-        <v>576</v>
+        <v>553</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="F39" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="33" t="s">
-        <v>577</v>
+        <v>554</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>133</v>
@@ -3633,54 +3666,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="33" t="s">
-        <v>578</v>
+        <v>555</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F41" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A42" s="33" t="s">
-        <v>579</v>
+        <v>556</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="D42" s="40"/>
       <c r="E42" s="41"/>
       <c r="F42" s="6" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A43" s="33" t="s">
-        <v>580</v>
+        <v>557</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>44</v>
@@ -3689,18 +3722,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A44" s="33" t="s">
-        <v>581</v>
+        <v>558</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>44</v>
@@ -3709,1039 +3742,1059 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A45" s="33" t="s">
-        <v>582</v>
+        <v>559</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A46" s="33" t="s">
-        <v>583</v>
+        <v>560</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>381</v>
+        <v>695</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" ht="117" x14ac:dyDescent="0.15">
       <c r="A47" s="33" t="s">
-        <v>584</v>
+        <v>690</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>384</v>
+        <v>691</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="D47" s="21" t="s">
-        <v>386</v>
+        <v>693</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>694</v>
       </c>
       <c r="E47" s="11" t="s">
+        <v>692</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A48" s="33" t="s">
+        <v>561</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="F48" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="F47" s="15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A48" s="33" t="s">
-        <v>585</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>387</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="D48" s="15">
+    </row>
+    <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A49" s="33" t="s">
+        <v>562</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="D49" s="15">
         <v>-8.73</v>
       </c>
-      <c r="E48" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A49" s="33" t="s">
-        <v>586</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>389</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>390</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>391</v>
-      </c>
       <c r="E49" s="11" t="s">
-        <v>99</v>
+        <v>298</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>47</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A50" s="33" t="s">
-        <v>587</v>
+        <v>563</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>393</v>
+        <v>700</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>99</v>
+        <v>699</v>
       </c>
       <c r="F50" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" s="33" t="s">
-        <v>588</v>
+        <v>564</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>397</v>
+        <v>383</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>384</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>398</v>
+        <v>99</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="108" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A52" s="33" t="s">
-        <v>589</v>
+        <v>565</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>401</v>
+        <v>386</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>387</v>
       </c>
       <c r="E52" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="117" x14ac:dyDescent="0.15">
+      <c r="A53" s="33" t="s">
+        <v>566</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>389</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="E53" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="33" t="s">
-        <v>590</v>
-      </c>
-      <c r="B53" s="36" t="s">
-        <v>402</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>404</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>195</v>
       </c>
       <c r="F53" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="33" t="s">
-        <v>591</v>
+        <v>567</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="D54" s="21" t="s">
-        <v>386</v>
+        <v>393</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="E54" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A55" s="33" t="s">
+        <v>568</v>
+      </c>
+      <c r="B55" s="36" t="s">
+        <v>395</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="F55" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="F54" s="15" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A55" s="33" t="s">
-        <v>592</v>
-      </c>
-      <c r="B55" s="36" t="s">
-        <v>407</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="D55" s="15">
+    </row>
+    <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A56" s="33" t="s">
+        <v>569</v>
+      </c>
+      <c r="B56" s="36" t="s">
+        <v>397</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="D56" s="15">
         <v>-8.73</v>
       </c>
-      <c r="E55" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A56" s="33" t="s">
-        <v>593</v>
-      </c>
-      <c r="B56" s="36" t="s">
-        <v>409</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>391</v>
-      </c>
       <c r="E56" s="11" t="s">
-        <v>99</v>
+        <v>298</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>47</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A57" s="33" t="s">
-        <v>594</v>
+        <v>570</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>394</v>
+        <v>701</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>381</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>99</v>
+        <v>699</v>
       </c>
       <c r="F57" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A58" s="33" t="s">
-        <v>595</v>
+        <v>571</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>414</v>
+        <v>702</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>384</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>152</v>
+        <v>699</v>
       </c>
       <c r="F58" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A59" s="33" t="s">
-        <v>596</v>
-      </c>
-      <c r="B59" s="35" t="s">
+        <v>572</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>401</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="33" t="s">
+        <v>573</v>
+      </c>
+      <c r="B60" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="39" t="s">
-        <v>415</v>
-      </c>
-      <c r="D59" s="40"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="6" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="48" x14ac:dyDescent="0.15">
-      <c r="A60" s="33" t="s">
-        <v>597</v>
-      </c>
-      <c r="B60" s="36" t="s">
-        <v>417</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="F60" s="11" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="C60" s="39" t="s">
+        <v>713</v>
+      </c>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="33" t="s">
-        <v>598</v>
+        <v>574</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>422</v>
+        <v>714</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>423</v>
+        <v>717</v>
       </c>
       <c r="E61" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A62" s="33" t="s">
+        <v>575</v>
+      </c>
+      <c r="B62" s="36" t="s">
+        <v>407</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>716</v>
+      </c>
+      <c r="E62" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="F61" s="11" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A62" s="33" t="s">
-        <v>599</v>
-      </c>
-      <c r="B62" s="35" t="s">
-        <v>425</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>426</v>
-      </c>
-      <c r="D62" s="40"/>
-      <c r="E62" s="41"/>
-      <c r="F62" s="6" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="F62" s="11" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="33" t="s">
-        <v>600</v>
-      </c>
-      <c r="B63" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>428</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="F63" s="15">
+        <v>576</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>706</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>712</v>
+      </c>
+      <c r="D63" s="40"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A64" s="33" t="s">
+        <v>577</v>
+      </c>
+      <c r="B64" s="36" t="s">
+        <v>707</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="F64" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A64" s="33" t="s">
-        <v>601</v>
-      </c>
-      <c r="B64" s="36" t="s">
-        <v>431</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>432</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>433</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A65" s="33" t="s">
-        <v>602</v>
+        <v>578</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>434</v>
+        <v>708</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>435</v>
+        <v>711</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>152</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="18" x14ac:dyDescent="0.15">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="33" t="s">
-        <v>603</v>
-      </c>
-      <c r="B66" s="35" t="s">
-        <v>438</v>
-      </c>
-      <c r="C66" s="39" t="s">
-        <v>439</v>
-      </c>
-      <c r="D66" s="40"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="6" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+        <v>579</v>
+      </c>
+      <c r="B66" s="36" t="s">
+        <v>709</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="33" t="s">
-        <v>604</v>
-      </c>
-      <c r="B67" s="36" t="s">
-        <v>441</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>443</v>
-      </c>
-      <c r="E67" s="11" t="s">
+        <v>580</v>
+      </c>
+      <c r="B67" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="C67" s="39" t="s">
+        <v>417</v>
+      </c>
+      <c r="D67" s="40"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A68" s="33" t="s">
+        <v>581</v>
+      </c>
+      <c r="B68" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="E68" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="F67" s="15">
+      <c r="F68" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A68" s="33" t="s">
-        <v>605</v>
-      </c>
-      <c r="B68" s="36" t="s">
-        <v>444</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>445</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A69" s="33" t="s">
-        <v>606</v>
+        <v>582</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>448</v>
+        <v>422</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>449</v>
+        <v>423</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>450</v>
+        <v>424</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>152</v>
+        <v>425</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A70" s="33" t="s">
-        <v>607</v>
+        <v>583</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>452</v>
+        <v>427</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>453</v>
+        <v>428</v>
       </c>
       <c r="E70" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A71" s="33" t="s">
+        <v>584</v>
+      </c>
+      <c r="B71" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="E71" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="F70" s="11" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="18" x14ac:dyDescent="0.15">
-      <c r="A71" s="33" t="s">
-        <v>608</v>
-      </c>
-      <c r="B71" s="35" t="s">
-        <v>454</v>
-      </c>
-      <c r="C71" s="39" t="s">
-        <v>455</v>
-      </c>
-      <c r="D71" s="40"/>
-      <c r="E71" s="41"/>
-      <c r="F71" s="6" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+      <c r="F71" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A72" s="33" t="s">
-        <v>609</v>
-      </c>
-      <c r="B72" s="36" t="s">
-        <v>457</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="E72" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="B72" s="35" t="s">
+        <v>432</v>
+      </c>
+      <c r="C72" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="D72" s="40"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A73" s="33" t="s">
+        <v>586</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>435</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="E73" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="F72" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A73" s="33" t="s">
-        <v>610</v>
-      </c>
-      <c r="B73" s="36" t="s">
-        <v>460</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="E73" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="F73" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A74" s="33" t="s">
-        <v>611</v>
+        <v>587</v>
       </c>
       <c r="B74" s="36" t="s">
+        <v>438</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F74" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A75" s="33" t="s">
+        <v>588</v>
+      </c>
+      <c r="B75" s="36" t="s">
+        <v>441</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+      <c r="A76" s="33" t="s">
+        <v>589</v>
+      </c>
+      <c r="B76" s="36" t="s">
+        <v>444</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D76" s="22" t="s">
+        <v>446</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A77" s="33" t="s">
+        <v>590</v>
+      </c>
+      <c r="B77" s="36" t="s">
+        <v>448</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+      <c r="A78" s="33" t="s">
+        <v>591</v>
+      </c>
+      <c r="B78" s="35" t="s">
+        <v>451</v>
+      </c>
+      <c r="C78" s="39" t="s">
+        <v>452</v>
+      </c>
+      <c r="D78" s="40"/>
+      <c r="E78" s="41"/>
+      <c r="F78" s="6" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A79" s="33" t="s">
+        <v>592</v>
+      </c>
+      <c r="B79" s="36" t="s">
+        <v>454</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>455</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F79" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A80" s="33" t="s">
+        <v>593</v>
+      </c>
+      <c r="B80" s="36" t="s">
+        <v>457</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="E80" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="F80" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A81" s="33" t="s">
+        <v>594</v>
+      </c>
+      <c r="B81" s="36" t="s">
+        <v>461</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="D81" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="E81" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="D74" s="11" t="s">
+      <c r="F81" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A82" s="33" t="s">
+        <v>595</v>
+      </c>
+      <c r="B82" s="36" t="s">
         <v>465</v>
       </c>
-      <c r="E74" s="11" t="s">
+      <c r="C82" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="E82" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A83" s="33" t="s">
+        <v>596</v>
+      </c>
+      <c r="B83" s="36" t="s">
+        <v>468</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>470</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="F83" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+      <c r="A84" s="33" t="s">
+        <v>597</v>
+      </c>
+      <c r="B84" s="36" t="s">
+        <v>441</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="E84" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F74" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.15">
-      <c r="A75" s="33" t="s">
-        <v>612</v>
-      </c>
-      <c r="B75" s="36" t="s">
-        <v>466</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>467</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>468</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A76" s="33" t="s">
-        <v>613</v>
-      </c>
-      <c r="B76" s="36" t="s">
-        <v>470</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>471</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="E76" s="11" t="s">
+      <c r="F84" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="33" t="s">
+        <v>598</v>
+      </c>
+      <c r="B85" s="35" t="s">
+        <v>474</v>
+      </c>
+      <c r="C85" s="39" t="s">
+        <v>718</v>
+      </c>
+      <c r="D85" s="40"/>
+      <c r="E85" s="41"/>
+      <c r="F85" s="6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="65" x14ac:dyDescent="0.15">
+      <c r="A86" s="33" t="s">
+        <v>599</v>
+      </c>
+      <c r="B86" s="37" t="s">
+        <v>475</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A87" s="33" t="s">
+        <v>600</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>478</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="E87" s="11" t="s">
         <v>152</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="18" x14ac:dyDescent="0.15">
-      <c r="A77" s="33" t="s">
-        <v>614</v>
-      </c>
-      <c r="B77" s="35" t="s">
-        <v>473</v>
-      </c>
-      <c r="C77" s="39" t="s">
-        <v>474</v>
-      </c>
-      <c r="D77" s="40"/>
-      <c r="E77" s="41"/>
-      <c r="F77" s="6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A78" s="33" t="s">
-        <v>615</v>
-      </c>
-      <c r="B78" s="36" t="s">
-        <v>476</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>477</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>478</v>
-      </c>
-      <c r="E78" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F78" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A79" s="33" t="s">
-        <v>616</v>
-      </c>
-      <c r="B79" s="36" t="s">
-        <v>479</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>480</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>481</v>
-      </c>
-      <c r="E79" s="11" t="s">
-        <v>482</v>
-      </c>
-      <c r="F79" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A80" s="33" t="s">
-        <v>617</v>
-      </c>
-      <c r="B80" s="36" t="s">
-        <v>483</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>485</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>486</v>
-      </c>
-      <c r="F80" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A81" s="33" t="s">
-        <v>618</v>
-      </c>
-      <c r="B81" s="36" t="s">
-        <v>487</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>488</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="F81" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A82" s="33" t="s">
-        <v>619</v>
-      </c>
-      <c r="B82" s="36" t="s">
-        <v>490</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>491</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="F82" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="48" x14ac:dyDescent="0.15">
-      <c r="A83" s="33" t="s">
-        <v>620</v>
-      </c>
-      <c r="B83" s="36" t="s">
-        <v>463</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>494</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>495</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F83" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="33" t="s">
-        <v>621</v>
-      </c>
-      <c r="B84" s="35" t="s">
-        <v>496</v>
-      </c>
-      <c r="C84" s="39" t="s">
-        <v>497</v>
-      </c>
-      <c r="D84" s="40"/>
-      <c r="E84" s="41"/>
-      <c r="F84" s="6" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="60" x14ac:dyDescent="0.15">
-      <c r="A85" s="33" t="s">
-        <v>622</v>
-      </c>
-      <c r="B85" s="37" t="s">
-        <v>498</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>499</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>500</v>
-      </c>
-      <c r="E85" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F85" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A86" s="33" t="s">
-        <v>623</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>501</v>
-      </c>
-      <c r="C86" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="D86" s="22" t="s">
-        <v>503</v>
-      </c>
-      <c r="E86" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="F86" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A87" s="33" t="s">
-        <v>624</v>
-      </c>
-      <c r="B87" s="37" t="s">
-        <v>504</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>506</v>
-      </c>
-      <c r="E87" s="11" t="s">
-        <v>507</v>
       </c>
       <c r="F87" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="33" t="s">
-        <v>625</v>
+        <v>601</v>
       </c>
       <c r="B88" s="37" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="E88" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A89" s="33" t="s">
+        <v>602</v>
+      </c>
+      <c r="B89" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="E89" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="F88" s="15">
+      <c r="F89" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A89" s="33" t="s">
-        <v>626</v>
-      </c>
-      <c r="B89" s="37" t="s">
-        <v>511</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>512</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>513</v>
-      </c>
-      <c r="E89" s="11" t="s">
-        <v>514</v>
-      </c>
-      <c r="F89" s="15" t="s">
+    <row r="90" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A90" s="33" t="s">
+        <v>603</v>
+      </c>
+      <c r="B90" s="37" t="s">
+        <v>488</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="E90" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="F90" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A90" s="33" t="s">
-        <v>627</v>
-      </c>
-      <c r="B90" s="36" t="s">
-        <v>515</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>516</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="E90" s="11" t="s">
+    <row r="91" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A91" s="33" t="s">
+        <v>604</v>
+      </c>
+      <c r="B91" s="36" t="s">
+        <v>492</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="E91" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="F90" s="15">
+      <c r="F91" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="36" x14ac:dyDescent="0.15">
-      <c r="A91" s="33" t="s">
-        <v>628</v>
-      </c>
-      <c r="B91" s="36" t="s">
-        <v>518</v>
-      </c>
-      <c r="C91" s="11" t="s">
-        <v>519</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>520</v>
-      </c>
-      <c r="E91" s="11" t="s">
-        <v>514</v>
-      </c>
-      <c r="F91" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="96" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A92" s="33" t="s">
-        <v>629</v>
-      </c>
-      <c r="B92" s="38" t="s">
-        <v>521</v>
+        <v>605</v>
+      </c>
+      <c r="B92" s="36" t="s">
+        <v>495</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>522</v>
+        <v>496</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>523</v>
+        <v>497</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>152</v>
+        <v>491</v>
       </c>
       <c r="F92" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:6" ht="104" x14ac:dyDescent="0.15">
       <c r="A93" s="33" t="s">
-        <v>630</v>
-      </c>
-      <c r="B93" s="36" t="s">
-        <v>524</v>
+        <v>606</v>
+      </c>
+      <c r="B93" s="38" t="s">
+        <v>498</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>525</v>
-      </c>
-      <c r="D93" s="27" t="s">
-        <v>526</v>
+        <v>499</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>500</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>527</v>
+        <v>152</v>
       </c>
       <c r="F93" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="33" t="s">
-        <v>631</v>
+        <v>607</v>
       </c>
       <c r="B94" s="36" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>529</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>530</v>
+        <v>502</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>503</v>
       </c>
       <c r="E94" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A95" s="33" t="s">
+        <v>608</v>
+      </c>
+      <c r="B95" s="36" t="s">
+        <v>505</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="E95" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F94" s="15">
+      <c r="F95" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A95" s="33" t="s">
-        <v>632</v>
-      </c>
-      <c r="B95" s="36" t="s">
-        <v>531</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>532</v>
-      </c>
-      <c r="D95" s="22" t="s">
-        <v>533</v>
-      </c>
-      <c r="E95" s="11" t="s">
-        <v>507</v>
-      </c>
-      <c r="F95" s="15" t="s">
+    <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A96" s="33" t="s">
+        <v>609</v>
+      </c>
+      <c r="B96" s="36" t="s">
+        <v>508</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>509</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="E96" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="F96" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="24" x14ac:dyDescent="0.15">
-      <c r="A96" s="33" t="s">
-        <v>633</v>
-      </c>
-      <c r="B96" s="36" t="s">
-        <v>534</v>
-      </c>
-      <c r="C96" s="11" t="s">
-        <v>535</v>
-      </c>
-      <c r="D96" s="11" t="s">
-        <v>536</v>
-      </c>
-      <c r="E96" s="11" t="s">
+    <row r="97" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A97" s="33" t="s">
+        <v>610</v>
+      </c>
+      <c r="B97" s="36" t="s">
+        <v>511</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>512</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>513</v>
+      </c>
+      <c r="E97" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="F96" s="15" t="s">
-        <v>196</v>
+      <c r="F97" s="15" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C63:E63"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C38:E38"/>
     <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D93" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D94" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4772,7 +4825,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="33" t="s">
-        <v>634</v>
+        <v>611</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1</v>
@@ -4784,7 +4837,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>635</v>
+        <v>612</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>5</v>
@@ -4796,7 +4849,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
-        <v>636</v>
+        <v>613</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>7</v>
@@ -4814,7 +4867,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
-        <v>637</v>
+        <v>614</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>65</v>
@@ -4823,9 +4876,9 @@
       <c r="D4" s="44"/>
       <c r="E4" s="45"/>
     </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="33" t="s">
-        <v>638</v>
+        <v>615</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>77</v>
@@ -4840,9 +4893,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
-        <v>639</v>
+        <v>616</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>102</v>
@@ -4857,9 +4910,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
-        <v>640</v>
+        <v>617</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>110</v>
@@ -4874,9 +4927,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
-        <v>641</v>
+        <v>618</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>117</v>
@@ -4891,9 +4944,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
-        <v>642</v>
+        <v>619</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>137</v>
@@ -4908,9 +4961,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
-        <v>643</v>
+        <v>620</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>141</v>
@@ -4925,9 +4978,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
-        <v>644</v>
+        <v>621</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>144</v>
@@ -4942,9 +4995,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="33" t="s">
-        <v>645</v>
+        <v>622</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>146</v>
@@ -4959,9 +5012,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="33" t="s">
-        <v>646</v>
+        <v>623</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>149</v>
@@ -4976,9 +5029,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="33" t="s">
-        <v>647</v>
+        <v>624</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>155</v>
@@ -4993,9 +5046,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" s="33" t="s">
-        <v>648</v>
+        <v>625</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>158</v>
@@ -5010,9 +5063,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>649</v>
+        <v>626</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>161</v>
@@ -5027,9 +5080,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="33" t="s">
-        <v>650</v>
+        <v>627</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>163</v>
@@ -5044,9 +5097,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="33" t="s">
-        <v>651</v>
+        <v>628</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>165</v>
@@ -5061,9 +5114,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="33" t="s">
-        <v>652</v>
+        <v>629</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>168</v>
@@ -5078,9 +5131,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="65" x14ac:dyDescent="0.15">
       <c r="A20" s="33" t="s">
-        <v>653</v>
+        <v>630</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>171</v>
@@ -5095,9 +5148,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A21" s="33" t="s">
-        <v>654</v>
+        <v>631</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>178</v>
@@ -5112,32 +5165,32 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A22" s="33" t="s">
-        <v>655</v>
+        <v>632</v>
       </c>
       <c r="B22" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A23" s="33" t="s">
-        <v>656</v>
+        <v>633</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" s="18">
         <v>0.33</v>
@@ -5148,246 +5201,246 @@
     </row>
     <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="33" t="s">
-        <v>657</v>
+        <v>634</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C24" s="44"/>
       <c r="D24" s="44"/>
       <c r="E24" s="45"/>
     </row>
-    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A25" s="33" t="s">
-        <v>658</v>
+        <v>635</v>
       </c>
       <c r="B25" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="E25" s="7" t="s">
+    </row>
+    <row r="26" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+      <c r="A26" s="33" t="s">
+        <v>636</v>
+      </c>
+      <c r="B26" s="32" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.15">
-      <c r="A26" s="33" t="s">
-        <v>659</v>
-      </c>
-      <c r="B26" s="32" t="s">
+      <c r="C26" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>205</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" s="33" t="s">
-        <v>660</v>
+        <v>637</v>
       </c>
       <c r="B27" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="33" t="s">
-        <v>661</v>
+        <v>638</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C28" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="E28" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="33" t="s">
-        <v>662</v>
+        <v>639</v>
       </c>
       <c r="B29" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>214</v>
-      </c>
       <c r="D29" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="33" t="s">
-        <v>663</v>
+        <v>640</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C30" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>220</v>
-      </c>
       <c r="E30" s="19" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.15">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A31" s="33" t="s">
-        <v>664</v>
+        <v>641</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="E31" s="19" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+      <c r="A32" s="33" t="s">
+        <v>642</v>
+      </c>
+      <c r="B32" s="32" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.15">
-      <c r="A32" s="33" t="s">
-        <v>665</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>233</v>
-      </c>
       <c r="C32" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A33" s="33" t="s">
-        <v>666</v>
+        <v>643</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>240</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A34" s="33" t="s">
-        <v>667</v>
+        <v>644</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="33" t="s">
-        <v>668</v>
+        <v>645</v>
       </c>
       <c r="B35" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="48" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A36" s="33" t="s">
-        <v>669</v>
+        <v>646</v>
       </c>
       <c r="B36" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="33" t="s">
-        <v>670</v>
+        <v>647</v>
       </c>
       <c r="B37" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>253</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>254</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="33" t="s">
-        <v>671</v>
+        <v>648</v>
       </c>
       <c r="B38" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>256</v>
-      </c>
       <c r="D38" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>99</v>
@@ -5395,180 +5448,180 @@
     </row>
     <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="33" t="s">
-        <v>672</v>
+        <v>649</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C39" s="44"/>
       <c r="D39" s="44"/>
       <c r="E39" s="45"/>
     </row>
-    <row r="40" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="33" t="s">
-        <v>673</v>
+        <v>650</v>
       </c>
       <c r="B40" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C40" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="D40" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="E40" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="E40" s="10" t="s">
+    </row>
+    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A41" s="33" t="s">
+        <v>651</v>
+      </c>
+      <c r="B41" s="32" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="A41" s="33" t="s">
-        <v>674</v>
-      </c>
-      <c r="B41" s="32" t="s">
+      <c r="C41" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="D41" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="E41" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="E41" s="10" t="s">
+    </row>
+    <row r="42" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A42" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="B42" s="32" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="39" x14ac:dyDescent="0.15">
-      <c r="A42" s="33" t="s">
-        <v>675</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>266</v>
-      </c>
       <c r="C42" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="D42" s="19" t="s">
-        <v>269</v>
-      </c>
       <c r="E42" s="10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.15">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" s="33" t="s">
-        <v>676</v>
+        <v>653</v>
       </c>
       <c r="B43" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="D43" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A44" s="33" t="s">
+        <v>654</v>
+      </c>
+      <c r="B44" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="D43" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="A44" s="33" t="s">
-        <v>677</v>
-      </c>
-      <c r="B44" s="32" t="s">
-        <v>275</v>
-      </c>
       <c r="C44" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D44" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="E44" s="10" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    </row>
+    <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" s="33" t="s">
-        <v>678</v>
+        <v>655</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="33" t="s">
-        <v>679</v>
+        <v>656</v>
       </c>
       <c r="B46" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="D46" s="19" t="s">
         <v>283</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>284</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A47" s="33" t="s">
-        <v>680</v>
+        <v>657</v>
       </c>
       <c r="B47" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C47" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>287</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>288</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A48" s="33" t="s">
-        <v>681</v>
+        <v>658</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C48" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A49" s="33" t="s">
+        <v>659</v>
+      </c>
+      <c r="B49" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="D48" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="A49" s="33" t="s">
-        <v>682</v>
-      </c>
-      <c r="B49" s="32" t="s">
+      <c r="C49" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="D49" s="19" t="s">
         <v>294</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>295</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>99</v>
@@ -5610,7 +5663,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="33" t="s">
-        <v>539</v>
+        <v>516</v>
       </c>
       <c r="B1" s="48" t="s">
         <v>2</v>
@@ -5621,7 +5674,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
-        <v>683</v>
+        <v>660</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>4</v>
@@ -5654,7 +5707,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
-        <v>684</v>
+        <v>661</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>12</v>
@@ -5691,9 +5744,9 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="33" t="s">
-        <v>685</v>
+        <v>662</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>15</v>
@@ -5708,9 +5761,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="33" t="s">
-        <v>686</v>
+        <v>663</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>23</v>
@@ -5725,9 +5778,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
-        <v>687</v>
+        <v>664</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>27</v>
@@ -5742,9 +5795,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
-        <v>688</v>
+        <v>665</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>30</v>
@@ -5759,9 +5812,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
-        <v>689</v>
+        <v>666</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>33</v>
@@ -5776,9 +5829,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
-        <v>690</v>
+        <v>667</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>37</v>
@@ -5793,9 +5846,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="52" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
-        <v>691</v>
+        <v>668</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>41</v>
@@ -5810,9 +5863,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
-        <v>692</v>
+        <v>669</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>48</v>
@@ -5827,9 +5880,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="33" t="s">
-        <v>693</v>
+        <v>670</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>52</v>
@@ -5844,9 +5897,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="33" t="s">
-        <v>694</v>
+        <v>671</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>56</v>
@@ -5861,9 +5914,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A14" s="33" t="s">
-        <v>695</v>
+        <v>672</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>60</v>
@@ -5878,9 +5931,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="52" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A15" s="33" t="s">
-        <v>696</v>
+        <v>673</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>64</v>
@@ -5895,9 +5948,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="39" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>697</v>
+        <v>674</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>69</v>
@@ -5912,9 +5965,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="33" t="s">
-        <v>698</v>
+        <v>675</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>73</v>
@@ -5929,9 +5982,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="52" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A18" s="33" t="s">
-        <v>699</v>
+        <v>676</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>79</v>
@@ -5946,9 +5999,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A19" s="33" t="s">
-        <v>700</v>
+        <v>677</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>83</v>
@@ -5963,9 +6016,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="104" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="112" x14ac:dyDescent="0.15">
       <c r="A20" s="33" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>87</v>
@@ -5980,9 +6033,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="33" t="s">
-        <v>702</v>
+        <v>679</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>91</v>
@@ -5997,9 +6050,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="78" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="84" x14ac:dyDescent="0.15">
       <c r="A22" s="33" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>95</v>
@@ -6014,9 +6067,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="33" t="s">
-        <v>704</v>
+        <v>681</v>
       </c>
       <c r="B23" s="32" t="s">
         <v>101</v>
@@ -6031,9 +6084,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="33" t="s">
-        <v>705</v>
+        <v>682</v>
       </c>
       <c r="B24" s="32" t="s">
         <v>108</v>
@@ -6048,9 +6101,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="52" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A25" s="33" t="s">
-        <v>706</v>
+        <v>683</v>
       </c>
       <c r="B25" s="32" t="s">
         <v>115</v>
@@ -6065,9 +6118,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="33" t="s">
-        <v>707</v>
+        <v>684</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>121</v>
@@ -6082,9 +6135,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="33" t="s">
-        <v>708</v>
+        <v>685</v>
       </c>
       <c r="B27" s="32" t="s">
         <v>125</v>
@@ -6099,9 +6152,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="33" t="s">
-        <v>709</v>
+        <v>686</v>
       </c>
       <c r="B28" s="32" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
close #18 - clean examples for environment
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hania/Code/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7400A4AB-055C-B540-B5BA-9586A2A1205B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D139B24E-9129-BE4A-A468-F1D22FAC8264}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -2149,22 +2149,6 @@
     <t xml:space="preserve">The object of a study is to ascertain the impact of one or more factors on the biological material. Thus, a factor is, by definition a condition that varies between observation units, which may be biotic (pest, disease interaction) or abiotic (treatment and cultural practice) in nature. Depending on the level of the data, an experimental factor can be either  "what is the factor applied to the plant" (ie Unwatered), or the "environmental characterisation" (ie if no rain on unwatered plant : Drought ;  if rain on unwatered plant: Irrigated) </t>
   </si>
   <si>
-    <t>Environmental parameters that was kept constant throughout the study and did not change betweeen observation units or assays. Environment measures that varies over time, ie environmental variables like soil water content, can be recorded as time series of Observed Variables (see below)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of the environment parameter, permanent within the experiment. </t>
-  </si>
-  <si>
-    <t>Value of the environment parameter, permanent within the experiment.</t>
-  </si>
-  <si>
-    <t>Value for each of the above parameters.
-Clay 50% plus sand ; Ca: 5 mg/L</t>
-  </si>
-  <si>
-    <t>rooting medium; medium composition; soil reflection</t>
-  </si>
-  <si>
     <t>An observed variable describe how a measurement has been made. It typically takes the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement.</t>
   </si>
   <si>
@@ -2205,6 +2189,23 @@
   </si>
   <si>
     <t>Potential energy of water per unit mass of water in the soil.XEO:00126</t>
+  </si>
+  <si>
+    <t>Environmental parameters that were kept constant throughout the study and did not change betweeen observation units or assays. Environment characteristics that vary over time, i.e. environmental variables, should be recorded as Observed Variables (see below).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the environment parameter constant within the experiment. </t>
+  </si>
+  <si>
+    <t>Value of the environment parameter (defined above) constant within the experiment.</t>
+  </si>
+  <si>
+    <t>sowing density
+rooting medium composition; pH</t>
+  </si>
+  <si>
+    <t>300 seeds per m2
+Clay 50% plus sand; 6.5</t>
   </si>
 </sst>
 </file>
@@ -2880,9 +2881,9 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1380" topLeftCell="A19" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1380" topLeftCell="A3" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3341,7 +3342,7 @@
         <v>526</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>692</v>
@@ -4050,7 +4051,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>701</v>
+        <v>715</v>
       </c>
       <c r="D60" s="40"/>
       <c r="E60" s="41"/>
@@ -4058,7 +4059,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A61" s="32" t="s">
         <v>562</v>
       </c>
@@ -4066,10 +4067,10 @@
         <v>393</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>702</v>
+        <v>716</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>705</v>
+        <v>718</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>394</v>
@@ -4086,10 +4087,10 @@
         <v>395</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>703</v>
+        <v>717</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>704</v>
+        <v>719</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>149</v>
@@ -4530,7 +4531,7 @@
         <v>462</v>
       </c>
       <c r="C85" s="39" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="D85" s="40"/>
       <c r="E85" s="41"/>
@@ -4810,7 +4811,7 @@
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -4884,7 +4885,7 @@
         <v>77</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>95</v>
@@ -4901,7 +4902,7 @@
         <v>101</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>105</v>
@@ -4935,7 +4936,7 @@
         <v>115</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>131</v>
@@ -5054,7 +5055,7 @@
         <v>155</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>156</v>
@@ -5071,7 +5072,7 @@
         <v>157</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>156</v>
@@ -5088,7 +5089,7 @@
         <v>158</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>156</v>
@@ -5122,7 +5123,7 @@
         <v>162</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>163</v>
@@ -5235,7 +5236,7 @@
         <v>195</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>196</v>
@@ -5252,7 +5253,7 @@
         <v>197</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>198</v>
@@ -5269,7 +5270,7 @@
         <v>199</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>201</v>
@@ -5286,7 +5287,7 @@
         <v>202</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>204</v>
@@ -5420,7 +5421,7 @@
         <v>240</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>241</v>

</xml_diff>

<commit_message>
close #31 - persistant repository
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hania/Code/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D139B24E-9129-BE4A-A468-F1D22FAC8264}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6CE3238-1A14-EE47-A199-6A59D43FE0CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15480" yWindow="460" windowWidth="22920" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -1044,9 +1044,6 @@
     <t>Data file link</t>
   </si>
   <si>
-    <t>Link to the data file (or digital object) in a public database or institutional repository; or identifier of the data file when submitted together with the MIAPPE submission.</t>
-  </si>
-  <si>
     <t>http://www.ebi.ac.uk/arrayexpress/experiments/E-GEOD-32551/</t>
   </si>
   <si>
@@ -2206,6 +2203,9 @@
   <si>
     <t>300 seeds per m2
 Clay 50% plus sand; 6.5</t>
+  </si>
+  <si>
+    <t>Link to the data file (or digital object) in a public database or in a persistant institutional repository; or identifier of the data file when submitted together with the MIAPPE submission.</t>
   </si>
 </sst>
 </file>
@@ -2882,8 +2882,8 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1380" topLeftCell="A3" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1380" topLeftCell="A27" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>3</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="3" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>11</v>
@@ -2943,7 +2943,7 @@
     </row>
     <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B4" s="35" t="s">
         <v>18</v>
@@ -2963,7 +2963,7 @@
     </row>
     <row r="5" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B5" s="35" t="s">
         <v>127</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="6" spans="1:6" ht="91" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>133</v>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>150</v>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>166</v>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>173</v>
@@ -3052,7 +3052,7 @@
         <v>174</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>44</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B10" s="35" t="s">
         <v>175</v>
@@ -3072,10 +3072,10 @@
         <v>176</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>675</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>676</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>677</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B11" s="35" t="s">
         <v>182</v>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>189</v>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>203</v>
@@ -3139,7 +3139,7 @@
     </row>
     <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>211</v>
@@ -3159,7 +3159,7 @@
     </row>
     <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B15" s="35" t="s">
         <v>214</v>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B16" s="35" t="s">
         <v>222</v>
@@ -3199,7 +3199,7 @@
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B17" s="35" t="s">
         <v>229</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>254</v>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B19" s="35" t="s">
         <v>263</v>
@@ -3259,7 +3259,7 @@
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="32" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B20" s="35" t="s">
         <v>273</v>
@@ -3279,7 +3279,7 @@
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B21" s="35" t="s">
         <v>283</v>
@@ -3299,7 +3299,7 @@
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B22" s="35" t="s">
         <v>288</v>
@@ -3319,19 +3319,19 @@
     </row>
     <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B23" s="35" t="s">
         <v>292</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>293</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>47</v>
@@ -3339,13 +3339,13 @@
     </row>
     <row r="24" spans="1:6" ht="91" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>294</v>
@@ -3359,13 +3359,13 @@
     </row>
     <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>295</v>
@@ -3379,10 +3379,10 @@
     </row>
     <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>297</v>
@@ -3399,7 +3399,7 @@
     </row>
     <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B27" s="35" t="s">
         <v>300</v>
@@ -3408,7 +3408,7 @@
         <v>301</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>149</v>
@@ -3419,7 +3419,7 @@
     </row>
     <row r="28" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="32" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B28" s="35" t="s">
         <v>302</v>
@@ -3428,7 +3428,7 @@
         <v>303</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>130</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="32" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B29" s="35" t="s">
         <v>304</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="32" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>308</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="31" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="32" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B31" s="35" t="s">
         <v>311</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="32" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B32" s="34" t="s">
         <v>314</v>
@@ -3508,12 +3508,12 @@
       <c r="D32" s="40"/>
       <c r="E32" s="41"/>
       <c r="F32" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A33" s="32" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B33" s="35" t="s">
         <v>316</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="32" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B34" s="35" t="s">
         <v>320</v>
@@ -3553,7 +3553,7 @@
     </row>
     <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A35" s="32" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B35" s="35" t="s">
         <v>324</v>
@@ -3573,7 +3573,7 @@
     </row>
     <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="32" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B36" s="35" t="s">
         <v>327</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B37" s="35" t="s">
         <v>330</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A38" s="32" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B38" s="34" t="s">
         <v>334</v>
@@ -3629,19 +3629,19 @@
     </row>
     <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A39" s="32" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B39" s="35" t="s">
         <v>337</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>719</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>338</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="E39" s="11" t="s">
         <v>339</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>340</v>
       </c>
       <c r="F39" s="14">
         <v>1</v>
@@ -3649,16 +3649,16 @@
     </row>
     <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="32" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B40" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>341</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="D40" s="21" t="s">
         <v>342</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>343</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>130</v>
@@ -3669,16 +3669,16 @@
     </row>
     <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="32" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B41" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="23" t="s">
         <v>345</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>346</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>180</v>
@@ -3689,32 +3689,32 @@
     </row>
     <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A42" s="32" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B42" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="C42" s="39" t="s">
         <v>347</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>348</v>
       </c>
       <c r="D42" s="40"/>
       <c r="E42" s="41"/>
       <c r="F42" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A43" s="32" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B43" s="35" t="s">
+        <v>349</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>351</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>352</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>44</v>
@@ -3725,16 +3725,16 @@
     </row>
     <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A44" s="32" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B44" s="35" t="s">
+        <v>352</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="21" t="s">
         <v>354</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>355</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>44</v>
@@ -3745,19 +3745,19 @@
     </row>
     <row r="45" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A45" s="32" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B45" s="35" t="s">
+        <v>355</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="E45" s="11" t="s">
         <v>358</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>359</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>47</v>
@@ -3765,19 +3765,19 @@
     </row>
     <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A46" s="32" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B46" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="D46" s="14" t="s">
+      <c r="E46" s="11" t="s">
         <v>361</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>362</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>47</v>
@@ -3785,19 +3785,19 @@
     </row>
     <row r="47" spans="1:6" ht="117" x14ac:dyDescent="0.15">
       <c r="A47" s="32" t="s">
+        <v>677</v>
+      </c>
+      <c r="B47" s="35" t="s">
         <v>678</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="C47" s="11" t="s">
+        <v>680</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>681</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>679</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>681</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>682</v>
-      </c>
-      <c r="E47" s="11" t="s">
-        <v>680</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>47</v>
@@ -3805,16 +3805,16 @@
     </row>
     <row r="48" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A48" s="32" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B48" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="20" t="s">
         <v>364</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>365</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>286</v>
@@ -3825,13 +3825,13 @@
     </row>
     <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A49" s="32" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B49" s="35" t="s">
+        <v>365</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>366</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>367</v>
       </c>
       <c r="D49" s="14">
         <v>-8.73</v>
@@ -3845,19 +3845,19 @@
     </row>
     <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A50" s="32" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B50" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>688</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>369</v>
-      </c>
       <c r="E50" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>47</v>
@@ -3865,16 +3865,16 @@
     </row>
     <row r="51" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" s="32" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B51" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="D51" s="14" t="s">
         <v>371</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>372</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>98</v>
@@ -3885,19 +3885,19 @@
     </row>
     <row r="52" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A52" s="32" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B52" s="35" t="s">
+        <v>372</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="24" t="s">
         <v>374</v>
       </c>
-      <c r="D52" s="24" t="s">
+      <c r="E52" s="11" t="s">
         <v>375</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>376</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>188</v>
@@ -3905,16 +3905,16 @@
     </row>
     <row r="53" spans="1:6" ht="117" x14ac:dyDescent="0.15">
       <c r="A53" s="32" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B53" s="35" t="s">
+        <v>376</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="D53" s="14" t="s">
         <v>378</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>379</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>44</v>
@@ -3925,16 +3925,16 @@
     </row>
     <row r="54" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="32" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B54" s="35" t="s">
+        <v>379</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>382</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>187</v>
@@ -3945,16 +3945,16 @@
     </row>
     <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A55" s="32" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B55" s="35" t="s">
+        <v>382</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>384</v>
-      </c>
       <c r="D55" s="20" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>286</v>
@@ -3965,13 +3965,13 @@
     </row>
     <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A56" s="32" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B56" s="35" t="s">
+        <v>384</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>385</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>386</v>
       </c>
       <c r="D56" s="14">
         <v>-8.73</v>
@@ -3985,19 +3985,19 @@
     </row>
     <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A57" s="32" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B57" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>47</v>
@@ -4005,19 +4005,19 @@
     </row>
     <row r="58" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A58" s="32" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>47</v>
@@ -4025,16 +4025,16 @@
     </row>
     <row r="59" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A59" s="32" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B59" s="35" t="s">
+        <v>388</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="D59" s="21" t="s">
         <v>390</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>391</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>149</v>
@@ -4045,35 +4045,35 @@
     </row>
     <row r="60" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="32" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B60" s="34" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D60" s="40"/>
       <c r="E60" s="41"/>
       <c r="F60" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A61" s="32" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B61" s="35" t="s">
+        <v>392</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>717</v>
+      </c>
+      <c r="E61" s="11" t="s">
         <v>393</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>716</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>718</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>394</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>333</v>
@@ -4081,55 +4081,55 @@
     </row>
     <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A62" s="32" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B62" s="35" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="32" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B63" s="34" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C63" s="39" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D63" s="40"/>
       <c r="E63" s="41"/>
       <c r="F63" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="32" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D64" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="E64" s="11" t="s">
         <v>398</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>399</v>
       </c>
       <c r="F64" s="14">
         <v>1</v>
@@ -4137,16 +4137,16 @@
     </row>
     <row r="65" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A65" s="32" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B65" s="35" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>149</v>
@@ -4157,52 +4157,52 @@
     </row>
     <row r="66" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="32" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B66" s="35" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C66" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="D66" s="11" t="s">
         <v>401</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>402</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="32" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B67" s="34" t="s">
+        <v>403</v>
+      </c>
+      <c r="C67" s="39" t="s">
         <v>404</v>
-      </c>
-      <c r="C67" s="39" t="s">
-        <v>405</v>
       </c>
       <c r="D67" s="40"/>
       <c r="E67" s="41"/>
       <c r="F67" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="32" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B68" s="35" t="s">
+        <v>406</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="D68" s="11" t="s">
         <v>408</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>409</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>130</v>
@@ -4213,19 +4213,19 @@
     </row>
     <row r="69" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A69" s="32" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B69" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="D69" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="E69" s="11" t="s">
         <v>412</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>413</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>47</v>
@@ -4233,16 +4233,16 @@
     </row>
     <row r="70" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A70" s="32" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B70" s="35" t="s">
+        <v>413</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="D70" s="11" t="s">
         <v>415</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>416</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>149</v>
@@ -4253,16 +4253,16 @@
     </row>
     <row r="71" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A71" s="32" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B71" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="D71" s="11" t="s">
         <v>418</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>419</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>165</v>
@@ -4273,32 +4273,32 @@
     </row>
     <row r="72" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A72" s="32" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B72" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="C72" s="39" t="s">
         <v>420</v>
-      </c>
-      <c r="C72" s="39" t="s">
-        <v>421</v>
       </c>
       <c r="D72" s="40"/>
       <c r="E72" s="41"/>
       <c r="F72" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A73" s="32" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B73" s="35" t="s">
+        <v>422</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="D73" s="11" t="s">
         <v>424</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>425</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>44</v>
@@ -4309,16 +4309,16 @@
     </row>
     <row r="74" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A74" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B74" s="35" t="s">
+        <v>425</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>426</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="D74" s="11" t="s">
         <v>427</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>428</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>149</v>
@@ -4329,16 +4329,16 @@
     </row>
     <row r="75" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A75" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B75" s="35" t="s">
+        <v>428</v>
+      </c>
+      <c r="C75" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="D75" s="11" t="s">
         <v>430</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>431</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>44</v>
@@ -4349,19 +4349,19 @@
     </row>
     <row r="76" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A76" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B76" s="35" t="s">
+        <v>431</v>
+      </c>
+      <c r="C76" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="D76" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="D76" s="21" t="s">
+      <c r="E76" s="11" t="s">
         <v>434</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>435</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>188</v>
@@ -4369,16 +4369,16 @@
     </row>
     <row r="77" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B77" s="35" t="s">
+        <v>435</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="D77" s="11" t="s">
         <v>437</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>438</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>149</v>
@@ -4389,32 +4389,32 @@
     </row>
     <row r="78" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A78" s="32" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B78" s="34" t="s">
+        <v>438</v>
+      </c>
+      <c r="C78" s="39" t="s">
         <v>439</v>
-      </c>
-      <c r="C78" s="39" t="s">
-        <v>440</v>
       </c>
       <c r="D78" s="40"/>
       <c r="E78" s="41"/>
       <c r="F78" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A79" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B79" s="35" t="s">
+        <v>441</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="D79" s="11" t="s">
         <v>443</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>444</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>44</v>
@@ -4425,19 +4425,19 @@
     </row>
     <row r="80" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A80" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B80" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="D80" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="E80" s="11" t="s">
         <v>447</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>448</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>47</v>
@@ -4445,19 +4445,19 @@
     </row>
     <row r="81" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A81" s="32" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B81" s="35" t="s">
+        <v>448</v>
+      </c>
+      <c r="C81" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="D81" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="D81" s="11" t="s">
+      <c r="E81" s="11" t="s">
         <v>451</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>452</v>
       </c>
       <c r="F81" s="14">
         <v>1</v>
@@ -4465,16 +4465,16 @@
     </row>
     <row r="82" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A82" s="32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B82" s="35" t="s">
+        <v>452</v>
+      </c>
+      <c r="C82" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="D82" s="11" t="s">
         <v>454</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>455</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>149</v>
@@ -4485,19 +4485,19 @@
     </row>
     <row r="83" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B83" s="35" t="s">
+        <v>455</v>
+      </c>
+      <c r="C83" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="D83" s="25" t="s">
         <v>457</v>
       </c>
-      <c r="D83" s="25" t="s">
+      <c r="E83" s="11" t="s">
         <v>458</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>459</v>
       </c>
       <c r="F83" s="14">
         <v>1</v>
@@ -4505,16 +4505,16 @@
     </row>
     <row r="84" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A84" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B84" s="35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C84" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="D84" s="11" t="s">
         <v>460</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>461</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>44</v>
@@ -4525,32 +4525,32 @@
     </row>
     <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="32" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B85" s="34" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C85" s="39" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D85" s="40"/>
       <c r="E85" s="41"/>
       <c r="F85" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A86" s="32" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B86" s="36" t="s">
+        <v>462</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>464</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>465</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>44</v>
@@ -4561,16 +4561,16 @@
     </row>
     <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="32" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B87" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="C87" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="D87" s="21" t="s">
         <v>467</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>468</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>149</v>
@@ -4581,19 +4581,19 @@
     </row>
     <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="32" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B88" s="36" t="s">
+        <v>468</v>
+      </c>
+      <c r="C88" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="D88" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="D88" s="11" t="s">
+      <c r="E88" s="11" t="s">
         <v>471</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>472</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>47</v>
@@ -4601,16 +4601,16 @@
     </row>
     <row r="89" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A89" s="32" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B89" s="36" t="s">
+        <v>472</v>
+      </c>
+      <c r="C89" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="D89" s="11" t="s">
         <v>474</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>475</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>149</v>
@@ -4621,19 +4621,19 @@
     </row>
     <row r="90" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A90" s="32" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B90" s="36" t="s">
+        <v>475</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="D90" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="D90" s="11" t="s">
+      <c r="E90" s="11" t="s">
         <v>478</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>479</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>47</v>
@@ -4641,16 +4641,16 @@
     </row>
     <row r="91" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="32" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B91" s="35" t="s">
+        <v>479</v>
+      </c>
+      <c r="C91" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="D91" s="11" t="s">
         <v>481</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>482</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>149</v>
@@ -4661,19 +4661,19 @@
     </row>
     <row r="92" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A92" s="32" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B92" s="35" t="s">
+        <v>482</v>
+      </c>
+      <c r="C92" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="D92" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="D92" s="11" t="s">
-        <v>485</v>
-      </c>
       <c r="E92" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>47</v>
@@ -4681,16 +4681,16 @@
     </row>
     <row r="93" spans="1:6" ht="104" x14ac:dyDescent="0.15">
       <c r="A93" s="32" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B93" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="C93" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="D93" s="11" t="s">
         <v>487</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>488</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>149</v>
@@ -4701,19 +4701,19 @@
     </row>
     <row r="94" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="32" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B94" s="35" t="s">
+        <v>488</v>
+      </c>
+      <c r="C94" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="D94" s="26" t="s">
         <v>490</v>
       </c>
-      <c r="D94" s="26" t="s">
+      <c r="E94" s="11" t="s">
         <v>491</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>492</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>47</v>
@@ -4721,16 +4721,16 @@
     </row>
     <row r="95" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="32" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B95" s="35" t="s">
+        <v>492</v>
+      </c>
+      <c r="C95" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="D95" s="11" t="s">
         <v>494</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>495</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>44</v>
@@ -4741,19 +4741,19 @@
     </row>
     <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A96" s="32" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B96" s="35" t="s">
+        <v>495</v>
+      </c>
+      <c r="C96" s="11" t="s">
         <v>496</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="D96" s="21" t="s">
         <v>497</v>
       </c>
-      <c r="D96" s="21" t="s">
-        <v>498</v>
-      </c>
       <c r="E96" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>47</v>
@@ -4761,16 +4761,16 @@
     </row>
     <row r="97" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A97" s="32" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B97" s="35" t="s">
+        <v>498</v>
+      </c>
+      <c r="C97" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="D97" s="11" t="s">
         <v>500</v>
-      </c>
-      <c r="D97" s="11" t="s">
-        <v>501</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>149</v>
@@ -4826,7 +4826,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>1</v>
@@ -4838,7 +4838,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>5</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>7</v>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B4" s="43" t="s">
         <v>65</v>
@@ -4879,13 +4879,13 @@
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>95</v>
@@ -4896,13 +4896,13 @@
     </row>
     <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>105</v>
@@ -4913,7 +4913,7 @@
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>108</v>
@@ -4930,13 +4930,13 @@
     </row>
     <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>115</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>131</v>
@@ -4947,7 +4947,7 @@
     </row>
     <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>134</v>
@@ -4964,7 +4964,7 @@
     </row>
     <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>138</v>
@@ -4981,7 +4981,7 @@
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>141</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>143</v>
@@ -5015,7 +5015,7 @@
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>146</v>
@@ -5032,7 +5032,7 @@
     </row>
     <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>152</v>
@@ -5049,13 +5049,13 @@
     </row>
     <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>155</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>156</v>
@@ -5066,13 +5066,13 @@
     </row>
     <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>157</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>156</v>
@@ -5083,13 +5083,13 @@
     </row>
     <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>158</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>156</v>
@@ -5100,7 +5100,7 @@
     </row>
     <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>159</v>
@@ -5117,13 +5117,13 @@
     </row>
     <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>162</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>163</v>
@@ -5134,7 +5134,7 @@
     </row>
     <row r="20" spans="1:5" ht="65" x14ac:dyDescent="0.15">
       <c r="A20" s="32" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>164</v>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="21" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B21" s="31" t="s">
         <v>171</v>
@@ -5168,7 +5168,7 @@
     </row>
     <row r="22" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>177</v>
@@ -5185,7 +5185,7 @@
     </row>
     <row r="23" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>181</v>
@@ -5202,7 +5202,7 @@
     </row>
     <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B24" s="43" t="s">
         <v>185</v>
@@ -5213,7 +5213,7 @@
     </row>
     <row r="25" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>191</v>
@@ -5230,13 +5230,13 @@
     </row>
     <row r="26" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>195</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>196</v>
@@ -5247,13 +5247,13 @@
     </row>
     <row r="27" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>197</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>198</v>
@@ -5264,13 +5264,13 @@
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="32" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>199</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>201</v>
@@ -5281,13 +5281,13 @@
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="32" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B29" s="31" t="s">
         <v>202</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>204</v>
@@ -5298,7 +5298,7 @@
     </row>
     <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="32" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B30" s="31" t="s">
         <v>205</v>
@@ -5315,7 +5315,7 @@
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A31" s="32" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>216</v>
@@ -5332,7 +5332,7 @@
     </row>
     <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="32" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>221</v>
@@ -5347,7 +5347,7 @@
     </row>
     <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A33" s="32" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B33" s="31" t="s">
         <v>225</v>
@@ -5364,7 +5364,7 @@
     </row>
     <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A34" s="32" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>230</v>
@@ -5381,7 +5381,7 @@
     </row>
     <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="32" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>234</v>
@@ -5398,7 +5398,7 @@
     </row>
     <row r="36" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A36" s="32" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>237</v>
@@ -5415,13 +5415,13 @@
     </row>
     <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="32" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B37" s="31" t="s">
         <v>240</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>241</v>
@@ -5432,7 +5432,7 @@
     </row>
     <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="32" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>242</v>
@@ -5449,7 +5449,7 @@
     </row>
     <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="32" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B39" s="43" t="s">
         <v>244</v>
@@ -5460,7 +5460,7 @@
     </row>
     <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="32" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B40" s="31" t="s">
         <v>245</v>
@@ -5477,7 +5477,7 @@
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" s="32" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B41" s="31" t="s">
         <v>249</v>
@@ -5494,7 +5494,7 @@
     </row>
     <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A42" s="32" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B42" s="31" t="s">
         <v>253</v>
@@ -5511,7 +5511,7 @@
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" s="32" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B43" s="31" t="s">
         <v>260</v>
@@ -5528,7 +5528,7 @@
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A44" s="32" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B44" s="31" t="s">
         <v>262</v>
@@ -5545,7 +5545,7 @@
     </row>
     <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" s="32" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B45" s="31" t="s">
         <v>264</v>
@@ -5562,7 +5562,7 @@
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="32" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B46" s="31" t="s">
         <v>269</v>
@@ -5579,7 +5579,7 @@
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A47" s="32" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B47" s="31" t="s">
         <v>272</v>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A48" s="32" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B48" s="31" t="s">
         <v>277</v>
@@ -5613,7 +5613,7 @@
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A49" s="32" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B49" s="31" t="s">
         <v>280</v>
@@ -5664,7 +5664,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="32" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B1" s="48" t="s">
         <v>2</v>
@@ -5675,7 +5675,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>4</v>
@@ -5708,7 +5708,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>12</v>
@@ -5747,7 +5747,7 @@
     </row>
     <row r="4" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="32" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>15</v>
@@ -5764,7 +5764,7 @@
     </row>
     <row r="5" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>23</v>
@@ -5781,7 +5781,7 @@
     </row>
     <row r="6" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="32" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>27</v>
@@ -5798,7 +5798,7 @@
     </row>
     <row r="7" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="32" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B7" s="31" t="s">
         <v>30</v>
@@ -5815,7 +5815,7 @@
     </row>
     <row r="8" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="32" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B8" s="31" t="s">
         <v>33</v>
@@ -5832,7 +5832,7 @@
     </row>
     <row r="9" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>37</v>
@@ -5849,7 +5849,7 @@
     </row>
     <row r="10" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A10" s="32" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>41</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="11" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="32" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B11" s="31" t="s">
         <v>48</v>
@@ -5883,7 +5883,7 @@
     </row>
     <row r="12" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="32" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>52</v>
@@ -5900,7 +5900,7 @@
     </row>
     <row r="13" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B13" s="31" t="s">
         <v>56</v>
@@ -5917,7 +5917,7 @@
     </row>
     <row r="14" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A14" s="32" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B14" s="31" t="s">
         <v>60</v>
@@ -5934,7 +5934,7 @@
     </row>
     <row r="15" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A15" s="32" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>64</v>
@@ -5951,7 +5951,7 @@
     </row>
     <row r="16" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="32" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>69</v>
@@ -5968,7 +5968,7 @@
     </row>
     <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="32" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B17" s="31" t="s">
         <v>73</v>
@@ -5985,7 +5985,7 @@
     </row>
     <row r="18" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A18" s="32" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>78</v>
@@ -6002,7 +6002,7 @@
     </row>
     <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A19" s="32" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B19" s="31" t="s">
         <v>82</v>
@@ -6019,7 +6019,7 @@
     </row>
     <row r="20" spans="1:5" ht="112" x14ac:dyDescent="0.15">
       <c r="A20" s="32" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B20" s="31" t="s">
         <v>86</v>
@@ -6036,7 +6036,7 @@
     </row>
     <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="32" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B21" s="31" t="s">
         <v>90</v>
@@ -6053,7 +6053,7 @@
     </row>
     <row r="22" spans="1:5" ht="84" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B22" s="31" t="s">
         <v>94</v>
@@ -6070,7 +6070,7 @@
     </row>
     <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>100</v>
@@ -6087,7 +6087,7 @@
     </row>
     <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>106</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="25" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>113</v>
@@ -6121,7 +6121,7 @@
     </row>
     <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>118</v>
@@ -6138,7 +6138,7 @@
     </row>
     <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>122</v>
@@ -6155,7 +6155,7 @@
     </row>
     <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="32" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B28" s="31" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Corrections of typos, spaces between value and unit, examples in separate lines (close #38)
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hania/Code/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6CE3238-1A14-EE47-A199-6A59D43FE0CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9A5E1F4B-D17B-BE4A-BC2F-CEA508A308F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="460" windowWidth="22920" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="720">
   <si>
     <t>MIAPPE</t>
   </si>
@@ -656,9 +656,6 @@
     <t>higher-level landform; land element and position; slope; ....</t>
   </si>
   <si>
-    <t>EBI:12345678, http://phenome-fppn.fr/maugio/2013/t2351</t>
-  </si>
-  <si>
     <t>Crop Ontology:'CO_715:0000058'</t>
   </si>
   <si>
@@ -707,9 +704,6 @@
     <t>pH</t>
   </si>
   <si>
-    <t>2002-04-04; 2006-09-27T10:23:21+00:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">Value of soil pH, separated by a colon, the depth (cm) from where soil sample was taken. Multiple values are separated by semicolon. </t>
   </si>
   <si>
@@ -908,12 +902,6 @@
     <t>Geographic location (altitude)</t>
   </si>
   <si>
-    <t>100m</t>
-  </si>
-  <si>
-    <t>Lines were repeated twice at each location using a complete block design. In order to limit competition effects, each block was organized into four sub-blocks corresponding to earliness groups based on a priori information. https://urgi.versailles.inra.fr/files/ephesis/181000503/181000503_plan.xls</t>
-  </si>
-  <si>
     <t>CO_715:0000145</t>
   </si>
   <si>
@@ -966,9 +954,6 @@
   </si>
   <si>
     <t>Representation of the experimental design.</t>
-  </si>
-  <si>
-    <t>gis or excel file</t>
   </si>
   <si>
     <t>Person</t>
@@ -1102,18 +1087,12 @@
     <t>Genus name for the organism under study, according to standard scientific nomenclature.</t>
   </si>
   <si>
-    <t>Zea; Solanum</t>
-  </si>
-  <si>
     <t>Genus name</t>
   </si>
   <si>
     <t>Species</t>
   </si>
   <si>
-    <t>mays; lycosperium x pennellii</t>
-  </si>
-  <si>
     <t>Species name</t>
   </si>
   <si>
@@ -1135,27 +1114,18 @@
     <t>Biological material altitude</t>
   </si>
   <si>
-    <t>10m</t>
-  </si>
-  <si>
     <t>Biological material coordinates uncertainty</t>
   </si>
   <si>
     <t>Circular uncertainty of the coordinates, preferably provided in meters (m). [Alternative identifier for in situ material]</t>
   </si>
   <si>
-    <t>200m</t>
-  </si>
-  <si>
     <t>Biological material preprocessing</t>
   </si>
   <si>
     <t>Description of any process or treatment applied uniformely to the biological material, prior to the study itself. Can be provided as free text or as an accession number from a suitable controlled vocabulary.</t>
   </si>
   <si>
-    <t>EO:0007210 - PVY(NTN); transplanted from study http://phenome-fppn.fr/maugio/2013/t2351 observation unit ID : pot:894</t>
-  </si>
-  <si>
     <t>Plant Environment Ontology and/or free text</t>
   </si>
   <si>
@@ -1165,9 +1135,6 @@
     <t>An identifier for the source of the biological material, in the form of a key-value pair comprising the name/identifer of the repository from which the material was sourced plus the accession number of the repository for that material. Where an accession number has not been assigned, but the material has been derived from the crossing of known accessions, the material can be defined as follows: "mother_accession X father_accession", or, if father is unknown, as "mother_accession X UNKNOWN". For in situ material, the region of provenance may be used when an accession is not available.</t>
   </si>
   <si>
-    <t>INRA:W95115_inra; ICNF:PNB-RPI .</t>
-  </si>
-  <si>
     <t>Material source DOI</t>
   </si>
   <si>
@@ -1199,9 +1166,6 @@
   </si>
   <si>
     <t>Description of the material source</t>
-  </si>
-  <si>
-    <t>Branches were collected from a 10-year-old tree growing in a progeny trial established in a loamy brown earth soil</t>
   </si>
   <si>
     <t>0-1 per study</t>
@@ -1256,18 +1220,9 @@
     <t>Short name of the event.</t>
   </si>
   <si>
-    <t>Planting; Watering; Fertilizing; Herbicide</t>
-  </si>
-  <si>
     <t>Event acession number</t>
   </si>
   <si>
-    <t>Accession number of the event type in a suitable controlled vocabulary (Crop Ontology) if available.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO_715:0000011; CO_715:0000007 </t>
-  </si>
-  <si>
     <t>Crop Ontology term (subclass of CO_715:0000006)</t>
   </si>
   <si>
@@ -1277,22 +1232,12 @@
     <t xml:space="preserve">Description of the event, including details such as amount applied and possibly duration of the event. </t>
   </si>
   <si>
-    <t xml:space="preserve">Grafting; 
-Fertilizer application, Ammonium nitrate at 3 kg/m2; 
-sowing </t>
-  </si>
-  <si>
     <t>Event date</t>
   </si>
   <si>
     <t>Date and time of the event.</t>
   </si>
   <si>
-    <t>2006-09-27T10:23:21+00:00;
-2006-10-27T10:23:21+00:00;
-2006-02-13T10:23:21+00:00</t>
-  </si>
-  <si>
     <t>Observation Unit</t>
   </si>
   <si>
@@ -1314,21 +1259,12 @@
     <t>Observation unit type</t>
   </si>
   <si>
-    <t>Type of observation unit in textual form.</t>
-  </si>
-  <si>
-    <t>block, sub-lock, plot, plant, trial, sample, pot, replication or replicate, individual, virtual_trial, unit-parcel</t>
-  </si>
-  <si>
     <t>External ID</t>
   </si>
   <si>
     <t xml:space="preserve">Identifier for the observation unit in a persistant repository, comprises the name of the repository and the identifier of the observation unit therein. The EBI Biosamples repository is recommended. </t>
   </si>
   <si>
-    <t>Biosamples: SAMEA4202911</t>
-  </si>
-  <si>
     <t>Spatial distribution</t>
   </si>
   <si>
@@ -1374,10 +1310,6 @@
     <t>The stage in the life of a plant structure during which the sample was taken, in the form of an accession number to a suitable controlled vocabulary (Plant Ontology, BBCH scale)</t>
   </si>
   <si>
-    <t>PO:0025094;
-BBCH-17</t>
-  </si>
-  <si>
     <t>Plant Ontology term (subclass or PO:0009012) or BBCH scale term</t>
   </si>
   <si>
@@ -1385,10 +1317,6 @@
   </si>
   <si>
     <t>A description of  the plant part (e.g. leaf) or the plant product (e.g. resin) from which the sample was taken, in the form of an accession number to a suitable controlled vocabulary (Plant Ontology).</t>
-  </si>
-  <si>
-    <t>PO:0000003;
-PO:0025161</t>
   </si>
   <si>
     <t xml:space="preserve">Plant Ontology term (subclass of PO:0025131)
@@ -1401,9 +1329,6 @@
     <t>Any information not captured by the other sample fields, including quantification, sample treatments and processing.</t>
   </si>
   <si>
-    <t>Distal part of the leaf ; 100mg of roots taken from 10 roots at 20°C, conserved in vacuum at 20mM NaCl salinity, stored at -60 °C to -85 °C.</t>
-  </si>
-  <si>
     <t>Collection date</t>
   </si>
   <si>
@@ -1446,9 +1371,6 @@
     <t>Variable accession number</t>
   </si>
   <si>
-    <t>Accession number of the variable in the Crop Ontology (if available)</t>
-  </si>
-  <si>
     <t>CO_322:0000794</t>
   </si>
   <si>
@@ -1461,16 +1383,10 @@
     <t>Name of the (plant or environmental) trait under observation</t>
   </si>
   <si>
-    <t>Anthesis time; reproductive growth time</t>
-  </si>
-  <si>
     <t>Trait accession number</t>
   </si>
   <si>
     <t>Accession number of the trait in a suitable controlled vocabulary (Crop Ontology, Trait Ontology).</t>
-  </si>
-  <si>
-    <t>CO_322:0000030, TO:0000366</t>
   </si>
   <si>
     <t>Term from Plant Trait Ontology, 
@@ -1541,10 +1457,6 @@
     <t>Name of the scale or unit of time with which observations of this type were recorded in the data file (for time series studies).</t>
   </si>
   <si>
-    <t>Date/Time;
-Growing degree day (GDD) </t>
-  </si>
-  <si>
     <t>Observation unit level hierarchy</t>
   </si>
   <si>
@@ -2077,28 +1989,6 @@
   </si>
   <si>
     <t>Infraspecific name</t>
-  </si>
-  <si>
-    <t>Free text, or key value pair list, or MCPD compliant format</t>
-  </si>
-  <si>
-    <t>Name of any subtaxa level, including variety, crossing name, etc....  It can be used to store any additional taxonomic identifier. 
-For Key value pair list format, the Key is the name of the rank)and the valueis the valueof  the rank. Ranks can be among the following terms: subspecies, cultivar, variety, subvariety, convariety, group, subgroup, hybrid, line, form, subform.
-For MCPD compliant format, the following abbreviations are allowed: ‘subsp.’ (subspecies); ‘convar.’ (convariety); ‘var.’ ( variety); ‘f.’ (form); ‘Group’ (cultivar group).).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free text: vinifera Pinot noir | B73
-Key value pair list: subspecies:vinifera ; cultivar:Pinot noir | var:B73
-MCPD: subsp. vinifera var Pinot Noir | var. B73, </t>
-  </si>
-  <si>
-    <t>SSpecies name (formally species epithet) for the organism under study, according to standard scientific nomenclature.</t>
-  </si>
-  <si>
-    <t>Observation units consisted in individual plots themselves consisting of a row of 15 plants at a density of approximately six plants per square meter | NA</t>
-  </si>
-  <si>
-    <t>field environment condition | NA</t>
   </si>
   <si>
     <t>Altitude of the experimental site, provided in metres (m).</t>
@@ -2206,6 +2096,126 @@
   </si>
   <si>
     <t>Link to the data file (or digital object) in a public database or in a persistant institutional repository; or identifier of the data file when submitted together with the MIAPPE submission.</t>
+  </si>
+  <si>
+    <t>2002-04-04
+2006-09-27T10:23:21+00:00</t>
+  </si>
+  <si>
+    <t>EBI:12345678
+http://phenome-fppn.fr/maugio/2013/t2351</t>
+  </si>
+  <si>
+    <t>100 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lines were repeated twice at each location using a complete block design. In order to limit competition effects, each block was organized into four sub-blocks corresponding to earliness groups based on a priori information. </t>
+  </si>
+  <si>
+    <t>https://urgi.versailles.inra.fr/files/ephesis/181000503/181000503_plan.xls</t>
+  </si>
+  <si>
+    <t>Observation units consisted in individual plots themselves consisting of a row of 15 plants at a density of approximately six plants per square meter.
+NA</t>
+  </si>
+  <si>
+    <t>field environment condition
+NA</t>
+  </si>
+  <si>
+    <t>URL or File name (of gis or excel file)</t>
+  </si>
+  <si>
+    <t>Zea
+Solanum</t>
+  </si>
+  <si>
+    <t>mays
+lycosperium x pennellii</t>
+  </si>
+  <si>
+    <t>Species name (formally: specific epithet) for the organism under study, according to standard scientific nomenclature.</t>
+  </si>
+  <si>
+    <t>Free text, or key-value pair list, or MCPD-compliant format</t>
+  </si>
+  <si>
+    <t>Name of any subtaxa level, including variety, crossing name, etc. It can be used to store any additional taxonomic identifier. Either free text description or key-value pair list format (the key is the name of the rank and the value is the value of  the rank). Ranks can be among the following terms: subspecies, cultivar, variety, subvariety, convariety, group, subgroup, hybrid, line, form, subform. For MCPD compliance, the following abbreviations are allowed: ‘subsp.’ (subspecies); ‘convar.’ (convariety); ‘var.’ (variety); ‘f.’ (form); ‘Group’ (cultivar group).</t>
+  </si>
+  <si>
+    <t>10 m</t>
+  </si>
+  <si>
+    <t>200 m</t>
+  </si>
+  <si>
+    <t>INRA:W95115_inra
+ICNF:PNB-RPI</t>
+  </si>
+  <si>
+    <t>Accession number of the event type in a suitable controlled vocabulary (Crop Ontology).</t>
+  </si>
+  <si>
+    <t>Planting
+Fertilizing</t>
+  </si>
+  <si>
+    <t>CO_715:0000007
+CO_715:0000011</t>
+  </si>
+  <si>
+    <t>2006-09-27T10:23:21+00:00;
+2006-10-27; 2006-11-13; 2016-11-21</t>
+  </si>
+  <si>
+    <t>Type of observation unit in textual form, usually on of the following: block, sub-lock, plot, plant, trial, sample, pot, replication or replicate, individual, virtual_trial, unit-parcel</t>
+  </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>PO:0025094
+BBCH-17</t>
+  </si>
+  <si>
+    <t>PO:0000003
+PO:0025161</t>
+  </si>
+  <si>
+    <t>Distal part of the leaf ; 100 mg of roots taken from 10 roots at 20°C, conserved in vacuum at 20 mM NaCl salinity, stored at -60 °C to -85 °C.</t>
+  </si>
+  <si>
+    <t>Accession number of the variable in the Crop Ontology</t>
+  </si>
+  <si>
+    <t>CO_322:0000030
+TO:0000366</t>
+  </si>
+  <si>
+    <t>Anthesis time
+Reproductive growth time</t>
+  </si>
+  <si>
+    <t>Growing degree day (GDD)
+Date/Time</t>
+  </si>
+  <si>
+    <t>Sowing using seed drill 
+Fertilizer application: Ammonium nitrate at 3 kg/m2</t>
+  </si>
+  <si>
+    <t>Branches were collected from a 10-year-old tree growing in a progeny trial established in a loamy brown earth soil.</t>
+  </si>
+  <si>
+    <t>vinifera Pinot noir
+B73
+subspecies:vinifera ; cultivar:Pinot noir
+var:B73
+subsp. vinifera var. Pinot Noir
+var. B73</t>
+  </si>
+  <si>
+    <t>EO:0007210 - PVY(NTN); transplanted from study http://phenome-fppn.fr/maugio/2013/t2351 observation unit ID: pot:894</t>
   </si>
 </sst>
 </file>
@@ -2215,7 +2225,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2303,6 +2313,19 @@
       <u/>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2420,10 +2443,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2507,9 +2531,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2561,8 +2582,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2881,9 +2909,8 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1380" topLeftCell="A27" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2897,19 +2924,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="32" t="s">
-        <v>503</v>
-      </c>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="31" t="s">
+        <v>476</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2926,26 +2953,26 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="32" t="s">
-        <v>504</v>
-      </c>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="31" t="s">
+        <v>477</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A4" s="32" t="s">
-        <v>505</v>
-      </c>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="31" t="s">
+        <v>478</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -2962,10 +2989,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="52" x14ac:dyDescent="0.15">
-      <c r="A5" s="32" t="s">
-        <v>506</v>
-      </c>
-      <c r="B5" s="35" t="s">
+      <c r="A5" s="31" t="s">
+        <v>479</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>127</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -2982,10 +3009,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="91" x14ac:dyDescent="0.15">
-      <c r="A6" s="32" t="s">
-        <v>507</v>
-      </c>
-      <c r="B6" s="35" t="s">
+      <c r="A6" s="31" t="s">
+        <v>480</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>133</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -3002,10 +3029,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A7" s="32" t="s">
-        <v>508</v>
-      </c>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="31" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>150</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3022,10 +3049,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A8" s="32" t="s">
-        <v>509</v>
-      </c>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="31" t="s">
+        <v>482</v>
+      </c>
+      <c r="B8" s="34" t="s">
         <v>166</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -3042,17 +3069,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A9" s="32" t="s">
-        <v>510</v>
-      </c>
-      <c r="B9" s="35" t="s">
+      <c r="A9" s="31" t="s">
+        <v>483</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>173</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>174</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>674</v>
+        <v>647</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>44</v>
@@ -3062,30 +3089,30 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="32" t="s">
-        <v>511</v>
-      </c>
-      <c r="B10" s="35" t="s">
+      <c r="A10" s="31" t="s">
+        <v>484</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>175</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>176</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>675</v>
+        <v>648</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>676</v>
+        <v>649</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A11" s="32" t="s">
-        <v>512</v>
-      </c>
-      <c r="B11" s="35" t="s">
+      <c r="A11" s="31" t="s">
+        <v>485</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>182</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -3102,33 +3129,33 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.15">
-      <c r="A12" s="32" t="s">
-        <v>513</v>
-      </c>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="31" t="s">
+        <v>486</v>
+      </c>
+      <c r="B12" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="6" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A13" s="32" t="s">
-        <v>514</v>
-      </c>
-      <c r="B13" s="35" t="s">
+      <c r="A13" s="31" t="s">
+        <v>487</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>203</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>206</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>209</v>
+        <v>688</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>44</v>
@@ -3138,17 +3165,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A14" s="32" t="s">
-        <v>515</v>
-      </c>
-      <c r="B14" s="35" t="s">
+      <c r="A14" s="31" t="s">
+        <v>488</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>212</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>213</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>130</v>
@@ -3158,17 +3185,17 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
-      <c r="A15" s="32" t="s">
-        <v>516</v>
-      </c>
-      <c r="B15" s="35" t="s">
+      <c r="A15" s="31" t="s">
+        <v>489</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>215</v>
-      </c>
       <c r="D15" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>149</v>
@@ -3178,17 +3205,17 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A16" s="32" t="s">
-        <v>517</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>222</v>
+      <c r="A16" s="31" t="s">
+        <v>490</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>221</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>226</v>
+        <v>687</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>165</v>
@@ -3198,14 +3225,14 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A17" s="32" t="s">
-        <v>518</v>
-      </c>
-      <c r="B17" s="35" t="s">
+      <c r="A17" s="31" t="s">
+        <v>491</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>231</v>
       </c>
       <c r="D17" s="19">
         <v>37587</v>
@@ -3218,17 +3245,17 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A18" s="32" t="s">
-        <v>519</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>254</v>
+      <c r="A18" s="31" t="s">
+        <v>492</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>252</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>259</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>130</v>
@@ -3238,37 +3265,37 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A19" s="32" t="s">
-        <v>520</v>
-      </c>
-      <c r="B19" s="35" t="s">
+      <c r="A19" s="31" t="s">
+        <v>493</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>267</v>
-      </c>
       <c r="E19" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F19" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A20" s="32" t="s">
-        <v>521</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>273</v>
+      <c r="A20" s="31" t="s">
+        <v>494</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>271</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>276</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>278</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>130</v>
@@ -3278,77 +3305,77 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A21" s="32" t="s">
-        <v>522</v>
-      </c>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="31" t="s">
+        <v>495</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="F21" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="E21" s="11" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A22" s="31" t="s">
+        <v>496</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>286</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="C22" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A22" s="32" t="s">
-        <v>523</v>
-      </c>
-      <c r="B22" s="35" t="s">
+      <c r="D22" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="E22" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="D22" s="20" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="B23" s="34" t="s">
         <v>290</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A23" s="32" t="s">
-        <v>524</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>292</v>
-      </c>
       <c r="C23" s="11" t="s">
-        <v>685</v>
+        <v>652</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>293</v>
+        <v>689</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>686</v>
+        <v>653</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="91" x14ac:dyDescent="0.15">
-      <c r="A24" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>701</v>
+    <row r="24" spans="1:6" ht="65" x14ac:dyDescent="0.15">
+      <c r="A24" s="31" t="s">
+        <v>498</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>668</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>691</v>
+        <v>658</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>294</v>
+        <v>690</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>149</v>
@@ -3358,57 +3385,57 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A25" s="32" t="s">
-        <v>526</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>690</v>
+      <c r="A25" s="31" t="s">
+        <v>499</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>657</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>692</v>
+        <v>659</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A26" s="32" t="s">
-        <v>527</v>
-      </c>
-      <c r="B26" s="35" t="s">
-        <v>501</v>
+      <c r="A26" s="31" t="s">
+        <v>500</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>474</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A27" s="32" t="s">
-        <v>528</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>300</v>
+    <row r="27" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+      <c r="A27" s="31" t="s">
+        <v>501</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>296</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>683</v>
+        <v>692</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>149</v>
@@ -3417,18 +3444,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A28" s="32" t="s">
-        <v>529</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>302</v>
+    <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A28" s="31" t="s">
+        <v>502</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>298</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>130</v>
@@ -3438,37 +3465,37 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A29" s="32" t="s">
-        <v>530</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>304</v>
+      <c r="A29" s="31" t="s">
+        <v>503</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>300</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F29" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A30" s="32" t="s">
-        <v>531</v>
-      </c>
-      <c r="B30" s="35" t="s">
-        <v>308</v>
+      <c r="A30" s="31" t="s">
+        <v>504</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>304</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>149</v>
@@ -3477,92 +3504,94 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A31" s="32" t="s">
-        <v>532</v>
-      </c>
-      <c r="B31" s="35" t="s">
-        <v>311</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="D31" s="29"/>
+    <row r="31" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+      <c r="A31" s="31" t="s">
+        <v>505</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>308</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>691</v>
+      </c>
       <c r="E31" s="28" t="s">
-        <v>313</v>
+        <v>694</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A32" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="B32" s="34" t="s">
+      <c r="A32" s="31" t="s">
+        <v>506</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="D32" s="39"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="6" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A33" s="31" t="s">
+        <v>507</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>314</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="6" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A33" s="32" t="s">
-        <v>534</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>316</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>318</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>319</v>
       </c>
       <c r="F33" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A34" s="32" t="s">
-        <v>535</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>320</v>
+      <c r="A34" s="31" t="s">
+        <v>508</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>315</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A35" s="32" t="s">
-        <v>536</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>324</v>
+      <c r="A35" s="31" t="s">
+        <v>509</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>319</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>44</v>
@@ -3572,93 +3601,93 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A36" s="32" t="s">
-        <v>537</v>
-      </c>
-      <c r="B36" s="35" t="s">
-        <v>327</v>
+      <c r="A36" s="31" t="s">
+        <v>510</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>322</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>130</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A37" s="32" t="s">
-        <v>538</v>
-      </c>
-      <c r="B37" s="35" t="s">
-        <v>330</v>
+      <c r="A37" s="31" t="s">
+        <v>511</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>325</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>130</v>
       </c>
       <c r="F37" s="14" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+      <c r="A38" s="31" t="s">
+        <v>512</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>329</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>330</v>
+      </c>
+      <c r="D38" s="39"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A39" s="31" t="s">
+        <v>513</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>686</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.15">
-      <c r="A38" s="32" t="s">
-        <v>539</v>
-      </c>
-      <c r="B38" s="34" t="s">
+      <c r="E39" s="11" t="s">
         <v>334</v>
-      </c>
-      <c r="C38" s="39" t="s">
-        <v>335</v>
-      </c>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A39" s="32" t="s">
-        <v>540</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>337</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>719</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>338</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>339</v>
       </c>
       <c r="F39" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A40" s="32" t="s">
-        <v>541</v>
-      </c>
-      <c r="B40" s="35" t="s">
-        <v>340</v>
+      <c r="A40" s="31" t="s">
+        <v>514</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>335</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>130</v>
@@ -3668,17 +3697,17 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A41" s="32" t="s">
-        <v>542</v>
-      </c>
-      <c r="B41" s="35" t="s">
-        <v>343</v>
+      <c r="A41" s="31" t="s">
+        <v>515</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>338</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>180</v>
@@ -3688,33 +3717,33 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A42" s="32" t="s">
-        <v>543</v>
-      </c>
-      <c r="B42" s="34" t="s">
+      <c r="A42" s="31" t="s">
+        <v>516</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="D42" s="39"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A43" s="31" t="s">
+        <v>517</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>346</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>347</v>
-      </c>
-      <c r="D42" s="40"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="6" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A43" s="32" t="s">
-        <v>544</v>
-      </c>
-      <c r="B43" s="35" t="s">
-        <v>349</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>351</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>44</v>
@@ -3724,17 +3753,17 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A44" s="32" t="s">
-        <v>545</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>352</v>
+      <c r="A44" s="31" t="s">
+        <v>518</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>347</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>44</v>
@@ -3744,137 +3773,137 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A45" s="32" t="s">
-        <v>546</v>
-      </c>
-      <c r="B45" s="35" t="s">
-        <v>355</v>
+      <c r="A45" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>350</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>357</v>
+        <v>695</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A46" s="32" t="s">
-        <v>547</v>
-      </c>
-      <c r="B46" s="35" t="s">
-        <v>359</v>
+      <c r="A46" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>353</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>682</v>
+        <v>697</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>360</v>
+        <v>696</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="117" x14ac:dyDescent="0.15">
-      <c r="A47" s="32" t="s">
-        <v>677</v>
-      </c>
-      <c r="B47" s="35" t="s">
-        <v>678</v>
+    <row r="47" spans="1:6" ht="104" x14ac:dyDescent="0.15">
+      <c r="A47" s="31" t="s">
+        <v>650</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>651</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>680</v>
+        <v>699</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>681</v>
+        <v>718</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>679</v>
+        <v>698</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A48" s="32" t="s">
-        <v>548</v>
-      </c>
-      <c r="B48" s="35" t="s">
-        <v>362</v>
+      <c r="A48" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>355</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A49" s="32" t="s">
-        <v>549</v>
-      </c>
-      <c r="B49" s="35" t="s">
-        <v>365</v>
+      <c r="A49" s="31" t="s">
+        <v>522</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>358</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="D49" s="14">
         <v>-8.73</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A50" s="32" t="s">
-        <v>550</v>
-      </c>
-      <c r="B50" s="35" t="s">
-        <v>367</v>
+      <c r="A50" s="31" t="s">
+        <v>523</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>360</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>687</v>
+        <v>654</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>368</v>
+        <v>700</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>686</v>
+        <v>653</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="A51" s="32" t="s">
-        <v>551</v>
-      </c>
-      <c r="B51" s="35" t="s">
-        <v>369</v>
+      <c r="A51" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>361</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>371</v>
+        <v>701</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>98</v>
@@ -3884,37 +3913,37 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A52" s="32" t="s">
-        <v>552</v>
-      </c>
-      <c r="B52" s="35" t="s">
-        <v>372</v>
+      <c r="A52" s="31" t="s">
+        <v>525</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>363</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>374</v>
+        <v>719</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="117" x14ac:dyDescent="0.15">
-      <c r="A53" s="32" t="s">
-        <v>553</v>
-      </c>
-      <c r="B53" s="35" t="s">
-        <v>376</v>
+      <c r="A53" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>366</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>378</v>
+        <v>702</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>44</v>
@@ -3924,17 +3953,17 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A54" s="32" t="s">
-        <v>554</v>
-      </c>
-      <c r="B54" s="35" t="s">
-        <v>379</v>
+      <c r="A54" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>368</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>187</v>
@@ -3944,97 +3973,97 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A55" s="32" t="s">
-        <v>555</v>
-      </c>
-      <c r="B55" s="35" t="s">
-        <v>382</v>
+      <c r="A55" s="31" t="s">
+        <v>528</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>371</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A56" s="32" t="s">
-        <v>556</v>
-      </c>
-      <c r="B56" s="35" t="s">
-        <v>384</v>
+      <c r="A56" s="31" t="s">
+        <v>529</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>373</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="D56" s="14">
         <v>-8.73</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A57" s="32" t="s">
-        <v>557</v>
-      </c>
-      <c r="B57" s="35" t="s">
-        <v>386</v>
+      <c r="A57" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>375</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>688</v>
+        <v>655</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>368</v>
+        <v>700</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>686</v>
+        <v>653</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="A58" s="32" t="s">
-        <v>558</v>
-      </c>
-      <c r="B58" s="35" t="s">
-        <v>387</v>
+      <c r="A58" s="31" t="s">
+        <v>531</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>376</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>689</v>
+        <v>656</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>371</v>
+        <v>701</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>686</v>
+        <v>653</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A59" s="32" t="s">
-        <v>559</v>
-      </c>
-      <c r="B59" s="35" t="s">
-        <v>388</v>
+      <c r="A59" s="31" t="s">
+        <v>532</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>377</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>390</v>
+        <v>717</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>149</v>
@@ -4044,109 +4073,109 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="32" t="s">
-        <v>560</v>
-      </c>
-      <c r="B60" s="34" t="s">
+      <c r="A60" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="B60" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="39" t="s">
-        <v>714</v>
-      </c>
-      <c r="D60" s="40"/>
-      <c r="E60" s="41"/>
+      <c r="C60" s="38" t="s">
+        <v>681</v>
+      </c>
+      <c r="D60" s="39"/>
+      <c r="E60" s="40"/>
       <c r="F60" s="6" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A61" s="32" t="s">
-        <v>561</v>
-      </c>
-      <c r="B61" s="35" t="s">
-        <v>392</v>
+      <c r="A61" s="31" t="s">
+        <v>534</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>380</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>715</v>
+        <v>682</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>717</v>
+        <v>684</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A62" s="32" t="s">
-        <v>562</v>
-      </c>
-      <c r="B62" s="35" t="s">
-        <v>394</v>
+      <c r="A62" s="31" t="s">
+        <v>535</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>382</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>716</v>
+        <v>683</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>718</v>
+        <v>685</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="32" t="s">
-        <v>563</v>
-      </c>
-      <c r="B63" s="34" t="s">
-        <v>693</v>
-      </c>
-      <c r="C63" s="39" t="s">
-        <v>699</v>
-      </c>
-      <c r="D63" s="40"/>
-      <c r="E63" s="41"/>
+      <c r="A63" s="31" t="s">
+        <v>536</v>
+      </c>
+      <c r="B63" s="33" t="s">
+        <v>660</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>666</v>
+      </c>
+      <c r="D63" s="39"/>
+      <c r="E63" s="40"/>
       <c r="F63" s="6" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A64" s="32" t="s">
-        <v>564</v>
-      </c>
-      <c r="B64" s="35" t="s">
-        <v>694</v>
+      <c r="A64" s="31" t="s">
+        <v>537</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>661</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>697</v>
+        <v>664</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="F64" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A65" s="32" t="s">
-        <v>565</v>
-      </c>
-      <c r="B65" s="35" t="s">
-        <v>695</v>
+      <c r="A65" s="31" t="s">
+        <v>538</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>662</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>698</v>
+        <v>665</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>149</v>
@@ -4156,53 +4185,53 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A66" s="32" t="s">
-        <v>566</v>
-      </c>
-      <c r="B66" s="35" t="s">
-        <v>696</v>
+      <c r="A66" s="31" t="s">
+        <v>539</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>663</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="32" t="s">
-        <v>567</v>
-      </c>
-      <c r="B67" s="34" t="s">
-        <v>403</v>
-      </c>
-      <c r="C67" s="39" t="s">
-        <v>404</v>
-      </c>
-      <c r="D67" s="40"/>
-      <c r="E67" s="41"/>
+      <c r="A67" s="31" t="s">
+        <v>540</v>
+      </c>
+      <c r="B67" s="33" t="s">
+        <v>391</v>
+      </c>
+      <c r="C67" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="D67" s="39"/>
+      <c r="E67" s="40"/>
       <c r="F67" s="6" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A68" s="32" t="s">
-        <v>568</v>
-      </c>
-      <c r="B68" s="35" t="s">
-        <v>406</v>
+        <v>393</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A68" s="31" t="s">
+        <v>541</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>394</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>408</v>
+        <v>704</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>130</v>
@@ -4212,37 +4241,37 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A69" s="32" t="s">
-        <v>569</v>
-      </c>
-      <c r="B69" s="35" t="s">
-        <v>409</v>
+      <c r="A69" s="31" t="s">
+        <v>542</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>396</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>410</v>
+        <v>703</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>411</v>
+        <v>705</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A70" s="32" t="s">
-        <v>570</v>
-      </c>
-      <c r="B70" s="35" t="s">
-        <v>413</v>
+    <row r="70" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A70" s="31" t="s">
+        <v>543</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>398</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>415</v>
+        <v>716</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>149</v>
@@ -4251,54 +4280,54 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A71" s="32" t="s">
-        <v>571</v>
-      </c>
-      <c r="B71" s="35" t="s">
-        <v>416</v>
+    <row r="71" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A71" s="31" t="s">
+        <v>544</v>
+      </c>
+      <c r="B71" s="34" t="s">
+        <v>400</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>418</v>
+        <v>706</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>165</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="19" x14ac:dyDescent="0.15">
-      <c r="A72" s="32" t="s">
-        <v>572</v>
-      </c>
-      <c r="B72" s="34" t="s">
-        <v>419</v>
-      </c>
-      <c r="C72" s="39" t="s">
-        <v>420</v>
-      </c>
-      <c r="D72" s="40"/>
-      <c r="E72" s="41"/>
+      <c r="A72" s="31" t="s">
+        <v>545</v>
+      </c>
+      <c r="B72" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="C72" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="D72" s="39"/>
+      <c r="E72" s="40"/>
       <c r="F72" s="6" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A73" s="32" t="s">
-        <v>573</v>
-      </c>
-      <c r="B73" s="35" t="s">
-        <v>422</v>
+      <c r="A73" s="31" t="s">
+        <v>546</v>
+      </c>
+      <c r="B73" s="34" t="s">
+        <v>405</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>44</v>
@@ -4307,18 +4336,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A74" s="32" t="s">
-        <v>574</v>
-      </c>
-      <c r="B74" s="35" t="s">
-        <v>425</v>
+    <row r="74" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A74" s="31" t="s">
+        <v>547</v>
+      </c>
+      <c r="B74" s="34" t="s">
+        <v>408</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>426</v>
+        <v>707</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>427</v>
+        <v>708</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>149</v>
@@ -4328,17 +4357,17 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A75" s="32" t="s">
-        <v>575</v>
-      </c>
-      <c r="B75" s="35" t="s">
-        <v>428</v>
+      <c r="A75" s="31" t="s">
+        <v>548</v>
+      </c>
+      <c r="B75" s="34" t="s">
+        <v>409</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>44</v>
@@ -4348,37 +4377,37 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="52" x14ac:dyDescent="0.15">
-      <c r="A76" s="32" t="s">
-        <v>576</v>
-      </c>
-      <c r="B76" s="35" t="s">
-        <v>431</v>
+      <c r="A76" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="B76" s="34" t="s">
+        <v>411</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A77" s="32" t="s">
-        <v>577</v>
-      </c>
-      <c r="B77" s="35" t="s">
-        <v>435</v>
+      <c r="A77" s="31" t="s">
+        <v>550</v>
+      </c>
+      <c r="B77" s="34" t="s">
+        <v>415</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>436</v>
+        <v>416</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>437</v>
+        <v>417</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>149</v>
@@ -4388,33 +4417,33 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="19" x14ac:dyDescent="0.15">
-      <c r="A78" s="32" t="s">
-        <v>578</v>
-      </c>
-      <c r="B78" s="34" t="s">
-        <v>438</v>
-      </c>
-      <c r="C78" s="39" t="s">
-        <v>439</v>
-      </c>
-      <c r="D78" s="40"/>
-      <c r="E78" s="41"/>
+      <c r="A78" s="31" t="s">
+        <v>551</v>
+      </c>
+      <c r="B78" s="33" t="s">
+        <v>418</v>
+      </c>
+      <c r="C78" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="D78" s="39"/>
+      <c r="E78" s="40"/>
       <c r="F78" s="6" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A79" s="32" t="s">
-        <v>579</v>
-      </c>
-      <c r="B79" s="35" t="s">
-        <v>441</v>
+      <c r="A79" s="31" t="s">
+        <v>552</v>
+      </c>
+      <c r="B79" s="34" t="s">
+        <v>421</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>44</v>
@@ -4424,57 +4453,57 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A80" s="32" t="s">
-        <v>580</v>
-      </c>
-      <c r="B80" s="35" t="s">
-        <v>444</v>
+      <c r="A80" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>424</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>446</v>
+        <v>709</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A81" s="32" t="s">
-        <v>581</v>
-      </c>
-      <c r="B81" s="35" t="s">
-        <v>448</v>
+      <c r="A81" s="31" t="s">
+        <v>554</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>427</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>450</v>
+        <v>710</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>451</v>
+        <v>429</v>
       </c>
       <c r="F81" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A82" s="32" t="s">
-        <v>582</v>
-      </c>
-      <c r="B82" s="35" t="s">
-        <v>452</v>
+      <c r="A82" s="31" t="s">
+        <v>555</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>430</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>453</v>
+        <v>431</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>454</v>
+        <v>711</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>149</v>
@@ -4484,37 +4513,37 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A83" s="32" t="s">
-        <v>583</v>
-      </c>
-      <c r="B83" s="35" t="s">
-        <v>455</v>
+      <c r="A83" s="31" t="s">
+        <v>556</v>
+      </c>
+      <c r="B83" s="34" t="s">
+        <v>432</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="F83" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="52" x14ac:dyDescent="0.15">
-      <c r="A84" s="32" t="s">
-        <v>584</v>
-      </c>
-      <c r="B84" s="35" t="s">
-        <v>428</v>
+      <c r="A84" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="B84" s="34" t="s">
+        <v>409</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>44</v>
@@ -4524,33 +4553,33 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="32" t="s">
-        <v>585</v>
-      </c>
-      <c r="B85" s="34" t="s">
-        <v>461</v>
-      </c>
-      <c r="C85" s="39" t="s">
-        <v>700</v>
-      </c>
-      <c r="D85" s="40"/>
-      <c r="E85" s="41"/>
+      <c r="A85" s="31" t="s">
+        <v>558</v>
+      </c>
+      <c r="B85" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="C85" s="38" t="s">
+        <v>667</v>
+      </c>
+      <c r="D85" s="39"/>
+      <c r="E85" s="40"/>
       <c r="F85" s="6" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="65" x14ac:dyDescent="0.15">
-      <c r="A86" s="32" t="s">
-        <v>586</v>
-      </c>
-      <c r="B86" s="36" t="s">
-        <v>462</v>
+      <c r="A86" s="31" t="s">
+        <v>559</v>
+      </c>
+      <c r="B86" s="35" t="s">
+        <v>439</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>44</v>
@@ -4560,17 +4589,17 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A87" s="32" t="s">
-        <v>587</v>
-      </c>
-      <c r="B87" s="35" t="s">
-        <v>465</v>
+      <c r="A87" s="31" t="s">
+        <v>560</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>442</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>149</v>
@@ -4580,37 +4609,37 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A88" s="32" t="s">
-        <v>588</v>
-      </c>
-      <c r="B88" s="36" t="s">
-        <v>468</v>
+      <c r="A88" s="31" t="s">
+        <v>561</v>
+      </c>
+      <c r="B88" s="35" t="s">
+        <v>445</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>469</v>
+        <v>712</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A89" s="32" t="s">
-        <v>589</v>
-      </c>
-      <c r="B89" s="36" t="s">
-        <v>472</v>
+    <row r="89" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A89" s="31" t="s">
+        <v>562</v>
+      </c>
+      <c r="B89" s="35" t="s">
+        <v>448</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>474</v>
+        <v>714</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>149</v>
@@ -4620,37 +4649,37 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A90" s="32" t="s">
-        <v>590</v>
-      </c>
-      <c r="B90" s="36" t="s">
-        <v>475</v>
+      <c r="A90" s="31" t="s">
+        <v>563</v>
+      </c>
+      <c r="B90" s="35" t="s">
+        <v>450</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>477</v>
+        <v>713</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A91" s="32" t="s">
-        <v>591</v>
-      </c>
-      <c r="B91" s="35" t="s">
-        <v>479</v>
+      <c r="A91" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="B91" s="34" t="s">
+        <v>453</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>149</v>
@@ -4660,37 +4689,37 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A92" s="32" t="s">
-        <v>592</v>
-      </c>
-      <c r="B92" s="35" t="s">
-        <v>482</v>
+      <c r="A92" s="31" t="s">
+        <v>565</v>
+      </c>
+      <c r="B92" s="34" t="s">
+        <v>456</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>484</v>
+        <v>458</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="104" x14ac:dyDescent="0.15">
-      <c r="A93" s="32" t="s">
-        <v>593</v>
-      </c>
-      <c r="B93" s="37" t="s">
-        <v>485</v>
+      <c r="A93" s="31" t="s">
+        <v>566</v>
+      </c>
+      <c r="B93" s="36" t="s">
+        <v>459</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>149</v>
@@ -4700,37 +4729,37 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A94" s="32" t="s">
-        <v>594</v>
-      </c>
-      <c r="B94" s="35" t="s">
-        <v>488</v>
+      <c r="A94" s="31" t="s">
+        <v>567</v>
+      </c>
+      <c r="B94" s="34" t="s">
+        <v>462</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>490</v>
+        <v>464</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A95" s="32" t="s">
-        <v>595</v>
-      </c>
-      <c r="B95" s="35" t="s">
-        <v>492</v>
+      <c r="A95" s="31" t="s">
+        <v>568</v>
+      </c>
+      <c r="B95" s="34" t="s">
+        <v>466</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>494</v>
+        <v>468</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>44</v>
@@ -4740,37 +4769,37 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A96" s="32" t="s">
-        <v>596</v>
-      </c>
-      <c r="B96" s="35" t="s">
-        <v>495</v>
+      <c r="A96" s="31" t="s">
+        <v>569</v>
+      </c>
+      <c r="B96" s="34" t="s">
+        <v>469</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>496</v>
+        <v>470</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A97" s="32" t="s">
-        <v>597</v>
-      </c>
-      <c r="B97" s="35" t="s">
-        <v>498</v>
+      <c r="A97" s="31" t="s">
+        <v>570</v>
+      </c>
+      <c r="B97" s="34" t="s">
+        <v>472</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>500</v>
+        <v>715</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>149</v>
@@ -4796,6 +4825,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D94" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D31" r:id="rId2" xr:uid="{02460488-3DB6-824C-B87B-023C2082D683}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4825,34 +4855,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
-        <v>598</v>
-      </c>
-      <c r="B1" s="46" t="s">
+      <c r="A1" s="31" t="s">
+        <v>571</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="32" t="s">
-        <v>599</v>
-      </c>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="31" t="s">
+        <v>572</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="32" t="s">
-        <v>600</v>
-      </c>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="31" t="s">
+        <v>573</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -4867,25 +4897,25 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="32" t="s">
-        <v>601</v>
-      </c>
-      <c r="B4" s="43" t="s">
+      <c r="A4" s="31" t="s">
+        <v>574</v>
+      </c>
+      <c r="B4" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="32" t="s">
-        <v>602</v>
-      </c>
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="31" t="s">
+        <v>575</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>702</v>
+        <v>669</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>95</v>
@@ -4895,14 +4925,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A6" s="32" t="s">
-        <v>603</v>
-      </c>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="31" t="s">
+        <v>576</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>703</v>
+        <v>670</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>105</v>
@@ -4912,10 +4942,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A7" s="32" t="s">
-        <v>604</v>
-      </c>
-      <c r="B7" s="31" t="s">
+      <c r="A7" s="31" t="s">
+        <v>577</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>108</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4929,14 +4959,14 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.15">
-      <c r="A8" s="32" t="s">
-        <v>605</v>
-      </c>
-      <c r="B8" s="31" t="s">
+      <c r="A8" s="31" t="s">
+        <v>578</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="38" t="s">
-        <v>704</v>
+      <c r="C8" s="37" t="s">
+        <v>671</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>131</v>
@@ -4946,10 +4976,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="32" t="s">
-        <v>606</v>
-      </c>
-      <c r="B9" s="31" t="s">
+      <c r="A9" s="31" t="s">
+        <v>579</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>134</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -4963,10 +4993,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="32" t="s">
-        <v>607</v>
-      </c>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="31" t="s">
+        <v>580</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>138</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -4980,10 +5010,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="32" t="s">
-        <v>608</v>
-      </c>
-      <c r="B11" s="31" t="s">
+      <c r="A11" s="31" t="s">
+        <v>581</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>141</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -4997,10 +5027,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
-      <c r="A12" s="32" t="s">
-        <v>609</v>
-      </c>
-      <c r="B12" s="31" t="s">
+      <c r="A12" s="31" t="s">
+        <v>582</v>
+      </c>
+      <c r="B12" s="30" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -5014,10 +5044,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A13" s="32" t="s">
-        <v>610</v>
-      </c>
-      <c r="B13" s="31" t="s">
+      <c r="A13" s="31" t="s">
+        <v>583</v>
+      </c>
+      <c r="B13" s="30" t="s">
         <v>146</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -5031,10 +5061,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="32" t="s">
-        <v>611</v>
-      </c>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="31" t="s">
+        <v>584</v>
+      </c>
+      <c r="B14" s="30" t="s">
         <v>152</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -5048,14 +5078,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="32" t="s">
-        <v>612</v>
-      </c>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="31" t="s">
+        <v>585</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>155</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>705</v>
+        <v>672</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>156</v>
@@ -5065,14 +5095,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="32" t="s">
-        <v>613</v>
-      </c>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="31" t="s">
+        <v>586</v>
+      </c>
+      <c r="B16" s="30" t="s">
         <v>157</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>706</v>
+        <v>673</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>156</v>
@@ -5082,14 +5112,14 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A17" s="32" t="s">
-        <v>614</v>
-      </c>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="31" t="s">
+        <v>587</v>
+      </c>
+      <c r="B17" s="30" t="s">
         <v>158</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>707</v>
+        <v>674</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>156</v>
@@ -5099,10 +5129,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A18" s="32" t="s">
-        <v>615</v>
-      </c>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="31" t="s">
+        <v>588</v>
+      </c>
+      <c r="B18" s="30" t="s">
         <v>159</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -5116,14 +5146,14 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A19" s="32" t="s">
-        <v>616</v>
-      </c>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="31" t="s">
+        <v>589</v>
+      </c>
+      <c r="B19" s="30" t="s">
         <v>162</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>708</v>
+        <v>675</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>163</v>
@@ -5133,8 +5163,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="65" x14ac:dyDescent="0.15">
-      <c r="A20" s="32" t="s">
-        <v>617</v>
+      <c r="A20" s="31" t="s">
+        <v>590</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>164</v>
@@ -5150,10 +5180,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="52" x14ac:dyDescent="0.15">
-      <c r="A21" s="32" t="s">
-        <v>618</v>
-      </c>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="31" t="s">
+        <v>591</v>
+      </c>
+      <c r="B21" s="30" t="s">
         <v>171</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -5167,10 +5197,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="52" x14ac:dyDescent="0.15">
-      <c r="A22" s="32" t="s">
-        <v>619</v>
-      </c>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="31" t="s">
+        <v>592</v>
+      </c>
+      <c r="B22" s="30" t="s">
         <v>177</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -5184,10 +5214,10 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="52" x14ac:dyDescent="0.15">
-      <c r="A23" s="32" t="s">
-        <v>620</v>
-      </c>
-      <c r="B23" s="31" t="s">
+      <c r="A23" s="31" t="s">
+        <v>593</v>
+      </c>
+      <c r="B23" s="30" t="s">
         <v>181</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -5201,21 +5231,21 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="32" t="s">
-        <v>621</v>
-      </c>
-      <c r="B24" s="43" t="s">
+      <c r="A24" s="31" t="s">
+        <v>594</v>
+      </c>
+      <c r="B24" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="45"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
     </row>
     <row r="25" spans="1:5" ht="52" x14ac:dyDescent="0.15">
-      <c r="A25" s="32" t="s">
-        <v>622</v>
-      </c>
-      <c r="B25" s="31" t="s">
+      <c r="A25" s="31" t="s">
+        <v>595</v>
+      </c>
+      <c r="B25" s="30" t="s">
         <v>191</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5229,14 +5259,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A26" s="32" t="s">
-        <v>623</v>
-      </c>
-      <c r="B26" s="31" t="s">
+      <c r="A26" s="31" t="s">
+        <v>596</v>
+      </c>
+      <c r="B26" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>709</v>
+        <v>676</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>196</v>
@@ -5246,14 +5276,14 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A27" s="32" t="s">
-        <v>624</v>
-      </c>
-      <c r="B27" s="31" t="s">
+      <c r="A27" s="31" t="s">
+        <v>597</v>
+      </c>
+      <c r="B27" s="30" t="s">
         <v>197</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>710</v>
+        <v>677</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>198</v>
@@ -5263,14 +5293,14 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
-      <c r="A28" s="32" t="s">
-        <v>625</v>
-      </c>
-      <c r="B28" s="31" t="s">
+      <c r="A28" s="31" t="s">
+        <v>598</v>
+      </c>
+      <c r="B28" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>711</v>
+        <v>678</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>201</v>
@@ -5280,14 +5310,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.15">
-      <c r="A29" s="32" t="s">
-        <v>626</v>
-      </c>
-      <c r="B29" s="31" t="s">
+      <c r="A29" s="31" t="s">
+        <v>599</v>
+      </c>
+      <c r="B29" s="30" t="s">
         <v>202</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>712</v>
+        <v>679</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>204</v>
@@ -5297,10 +5327,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A30" s="32" t="s">
-        <v>627</v>
-      </c>
-      <c r="B30" s="31" t="s">
+      <c r="A30" s="31" t="s">
+        <v>600</v>
+      </c>
+      <c r="B30" s="30" t="s">
         <v>205</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -5310,35 +5340,35 @@
         <v>208</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
-      <c r="A31" s="32" t="s">
-        <v>628</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>216</v>
+      <c r="A31" s="31" t="s">
+        <v>601</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>215</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="E31" s="18" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+      <c r="A32" s="31" t="s">
+        <v>602</v>
+      </c>
+      <c r="B32" s="30" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A32" s="32" t="s">
-        <v>629</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>221</v>
-      </c>
       <c r="C32" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="10" t="s">
@@ -5346,212 +5376,212 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.15">
-      <c r="A33" s="32" t="s">
-        <v>630</v>
-      </c>
-      <c r="B33" s="31" t="s">
+      <c r="A33" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="D33" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.15">
-      <c r="A34" s="32" t="s">
-        <v>631</v>
-      </c>
-      <c r="B34" s="31" t="s">
+      <c r="A34" s="31" t="s">
+        <v>604</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>232</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A35" s="32" t="s">
-        <v>632</v>
-      </c>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="31" t="s">
+        <v>605</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>236</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="52" x14ac:dyDescent="0.15">
-      <c r="A36" s="32" t="s">
-        <v>633</v>
-      </c>
-      <c r="B36" s="31" t="s">
+      <c r="A36" s="31" t="s">
+        <v>606</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.15">
-      <c r="A37" s="32" t="s">
-        <v>634</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>240</v>
+      <c r="A37" s="31" t="s">
+        <v>607</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>238</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>713</v>
+        <v>680</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="32" t="s">
-        <v>635</v>
-      </c>
-      <c r="B38" s="31" t="s">
-        <v>242</v>
+      <c r="A38" s="31" t="s">
+        <v>608</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>240</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="32" t="s">
-        <v>636</v>
-      </c>
-      <c r="B39" s="43" t="s">
+      <c r="A39" s="31" t="s">
+        <v>609</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="44"/>
+    </row>
+    <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A40" s="31" t="s">
+        <v>610</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>243</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="45"/>
-    </row>
-    <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A40" s="32" t="s">
-        <v>637</v>
-      </c>
-      <c r="B40" s="31" t="s">
+      <c r="D40" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="E40" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="D40" s="18" t="s">
+    </row>
+    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A41" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="B41" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="C41" s="18" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.15">
-      <c r="A41" s="32" t="s">
-        <v>638</v>
-      </c>
-      <c r="B41" s="31" t="s">
+      <c r="D41" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="E41" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="D41" s="18" t="s">
+    </row>
+    <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A42" s="31" t="s">
+        <v>612</v>
+      </c>
+      <c r="B42" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A42" s="32" t="s">
-        <v>639</v>
-      </c>
-      <c r="B42" s="31" t="s">
+      <c r="C42" s="18" t="s">
         <v>253</v>
       </c>
-      <c r="C42" s="18" t="s">
-        <v>255</v>
-      </c>
       <c r="D42" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="E42" s="10" t="s">
+    </row>
+    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A43" s="31" t="s">
+        <v>613</v>
+      </c>
+      <c r="B43" s="30" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.15">
-      <c r="A43" s="32" t="s">
-        <v>640</v>
-      </c>
-      <c r="B43" s="31" t="s">
+      <c r="C43" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A44" s="31" t="s">
+        <v>614</v>
+      </c>
+      <c r="B44" s="30" t="s">
         <v>260</v>
       </c>
-      <c r="C43" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.15">
-      <c r="A44" s="32" t="s">
-        <v>641</v>
-      </c>
-      <c r="B44" s="31" t="s">
+      <c r="C44" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A45" s="31" t="s">
+        <v>615</v>
+      </c>
+      <c r="B45" s="30" t="s">
         <v>262</v>
       </c>
-      <c r="C44" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A45" s="32" t="s">
-        <v>642</v>
-      </c>
-      <c r="B45" s="31" t="s">
+      <c r="C45" s="15" t="s">
         <v>264</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>266</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>198</v>
@@ -5561,68 +5591,68 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
-      <c r="A46" s="32" t="s">
-        <v>643</v>
-      </c>
-      <c r="B46" s="31" t="s">
+      <c r="A46" s="31" t="s">
+        <v>616</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>269</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>271</v>
       </c>
       <c r="E46" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.15">
-      <c r="A47" s="32" t="s">
-        <v>644</v>
-      </c>
-      <c r="B47" s="31" t="s">
+      <c r="A47" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="C47" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="C47" s="18" t="s">
-        <v>274</v>
-      </c>
       <c r="D47" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E47" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.15">
-      <c r="A48" s="32" t="s">
-        <v>645</v>
-      </c>
-      <c r="B48" s="31" t="s">
+      <c r="A48" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="D48" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+      <c r="A49" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C49" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.15">
-      <c r="A49" s="32" t="s">
-        <v>646</v>
-      </c>
-      <c r="B49" s="31" t="s">
+      <c r="D49" s="18" t="s">
         <v>280</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>282</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>98</v>
@@ -5663,26 +5693,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
-        <v>503</v>
-      </c>
-      <c r="B1" s="48" t="s">
+      <c r="A1" s="31" t="s">
+        <v>476</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="32" t="s">
-        <v>647</v>
-      </c>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="31" t="s">
+        <v>620</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5707,10 +5737,10 @@
       <c r="AA2" s="4"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="32" t="s">
-        <v>648</v>
-      </c>
-      <c r="B3" s="33" t="s">
+      <c r="A3" s="31" t="s">
+        <v>621</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -5746,10 +5776,10 @@
       <c r="AA3" s="4"/>
     </row>
     <row r="4" spans="1:27" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="32" t="s">
-        <v>649</v>
-      </c>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -5763,10 +5793,10 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A5" s="32" t="s">
-        <v>650</v>
-      </c>
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="31" t="s">
+        <v>623</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -5780,10 +5810,10 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A6" s="32" t="s">
-        <v>651</v>
-      </c>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="31" t="s">
+        <v>624</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -5797,10 +5827,10 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A7" s="32" t="s">
-        <v>652</v>
-      </c>
-      <c r="B7" s="31" t="s">
+      <c r="A7" s="31" t="s">
+        <v>625</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -5814,10 +5844,10 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="28" x14ac:dyDescent="0.15">
-      <c r="A8" s="32" t="s">
-        <v>653</v>
-      </c>
-      <c r="B8" s="31" t="s">
+      <c r="A8" s="31" t="s">
+        <v>626</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -5831,10 +5861,10 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="28" x14ac:dyDescent="0.15">
-      <c r="A9" s="32" t="s">
-        <v>654</v>
-      </c>
-      <c r="B9" s="31" t="s">
+      <c r="A9" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -5848,10 +5878,10 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A10" s="32" t="s">
-        <v>655</v>
-      </c>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="31" t="s">
+        <v>628</v>
+      </c>
+      <c r="B10" s="30" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -5865,10 +5895,10 @@
       </c>
     </row>
     <row r="11" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A11" s="32" t="s">
-        <v>656</v>
-      </c>
-      <c r="B11" s="31" t="s">
+      <c r="A11" s="31" t="s">
+        <v>629</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -5882,10 +5912,10 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A12" s="32" t="s">
-        <v>657</v>
-      </c>
-      <c r="B12" s="31" t="s">
+      <c r="A12" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="B12" s="30" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -5899,10 +5929,10 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="28" x14ac:dyDescent="0.15">
-      <c r="A13" s="32" t="s">
-        <v>658</v>
-      </c>
-      <c r="B13" s="31" t="s">
+      <c r="A13" s="31" t="s">
+        <v>631</v>
+      </c>
+      <c r="B13" s="30" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -5916,10 +5946,10 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A14" s="32" t="s">
-        <v>659</v>
-      </c>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="31" t="s">
+        <v>632</v>
+      </c>
+      <c r="B14" s="30" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -5933,10 +5963,10 @@
       </c>
     </row>
     <row r="15" spans="1:27" ht="56" x14ac:dyDescent="0.15">
-      <c r="A15" s="32" t="s">
-        <v>660</v>
-      </c>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="31" t="s">
+        <v>633</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -5950,10 +5980,10 @@
       </c>
     </row>
     <row r="16" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A16" s="32" t="s">
-        <v>661</v>
-      </c>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="31" t="s">
+        <v>634</v>
+      </c>
+      <c r="B16" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -5967,10 +5997,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A17" s="32" t="s">
-        <v>662</v>
-      </c>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="31" t="s">
+        <v>635</v>
+      </c>
+      <c r="B17" s="30" t="s">
         <v>73</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -5984,10 +6014,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="56" x14ac:dyDescent="0.15">
-      <c r="A18" s="32" t="s">
-        <v>663</v>
-      </c>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="31" t="s">
+        <v>636</v>
+      </c>
+      <c r="B18" s="30" t="s">
         <v>78</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -6001,10 +6031,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A19" s="32" t="s">
-        <v>664</v>
-      </c>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="31" t="s">
+        <v>637</v>
+      </c>
+      <c r="B19" s="30" t="s">
         <v>82</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -6018,10 +6048,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="112" x14ac:dyDescent="0.15">
-      <c r="A20" s="32" t="s">
-        <v>665</v>
-      </c>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="31" t="s">
+        <v>638</v>
+      </c>
+      <c r="B20" s="30" t="s">
         <v>86</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -6035,10 +6065,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A21" s="32" t="s">
-        <v>666</v>
-      </c>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="31" t="s">
+        <v>639</v>
+      </c>
+      <c r="B21" s="30" t="s">
         <v>90</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -6052,10 +6082,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="84" x14ac:dyDescent="0.15">
-      <c r="A22" s="32" t="s">
-        <v>667</v>
-      </c>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="31" t="s">
+        <v>640</v>
+      </c>
+      <c r="B22" s="30" t="s">
         <v>94</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -6069,10 +6099,10 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A23" s="32" t="s">
-        <v>668</v>
-      </c>
-      <c r="B23" s="31" t="s">
+      <c r="A23" s="31" t="s">
+        <v>641</v>
+      </c>
+      <c r="B23" s="30" t="s">
         <v>100</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -6086,10 +6116,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A24" s="32" t="s">
-        <v>669</v>
-      </c>
-      <c r="B24" s="31" t="s">
+      <c r="A24" s="31" t="s">
+        <v>642</v>
+      </c>
+      <c r="B24" s="30" t="s">
         <v>106</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -6103,10 +6133,10 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="56" x14ac:dyDescent="0.15">
-      <c r="A25" s="32" t="s">
-        <v>670</v>
-      </c>
-      <c r="B25" s="31" t="s">
+      <c r="A25" s="31" t="s">
+        <v>643</v>
+      </c>
+      <c r="B25" s="30" t="s">
         <v>113</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -6120,10 +6150,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.15">
-      <c r="A26" s="32" t="s">
-        <v>671</v>
-      </c>
-      <c r="B26" s="31" t="s">
+      <c r="A26" s="31" t="s">
+        <v>644</v>
+      </c>
+      <c r="B26" s="30" t="s">
         <v>118</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -6137,10 +6167,10 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A27" s="32" t="s">
-        <v>672</v>
-      </c>
-      <c r="B27" s="31" t="s">
+      <c r="A27" s="31" t="s">
+        <v>645</v>
+      </c>
+      <c r="B27" s="30" t="s">
         <v>122</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -6154,10 +6184,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A28" s="32" t="s">
-        <v>673</v>
-      </c>
-      <c r="B28" s="31" t="s">
+      <c r="A28" s="31" t="s">
+        <v>646</v>
+      </c>
+      <c r="B28" s="30" t="s">
         <v>126</v>
       </c>
       <c r="C28" s="12"/>

</xml_diff>

<commit_message>
Close #30 (Add GRID ID to examples for affiliated institution)
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hania/Code/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE\MIAPPE_Checklist-Data-Model-v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9A5E1F4B-D17B-BE4A-BC2F-CEA508A308F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -1011,9 +1010,6 @@
     <t>The institution the person belongs to</t>
   </si>
   <si>
-    <t>ITQB, Portugal</t>
-  </si>
-  <si>
     <t>1+</t>
   </si>
   <si>
@@ -2217,11 +2213,15 @@
   <si>
     <t>EO:0007210 - PVY(NTN); transplanted from study http://phenome-fppn.fr/maugio/2013/t2351 observation unit ID: pot:894</t>
   </si>
+  <si>
+    <t>ITQB, Portugal;
+grid.10772.33</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -2556,6 +2556,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2581,12 +2587,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2902,39 +2902,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="51.83203125" customWidth="1"/>
-    <col min="4" max="4" width="41.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>3</v>
@@ -2952,25 +2952,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>18</v>
@@ -2988,9 +2988,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>127</v>
@@ -3008,9 +3008,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="91" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>133</v>
@@ -3028,9 +3028,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>150</v>
@@ -3048,9 +3048,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>166</v>
@@ -3068,9 +3068,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>173</v>
@@ -3079,7 +3079,7 @@
         <v>174</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>44</v>
@@ -3088,9 +3088,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>175</v>
@@ -3099,18 +3099,18 @@
         <v>176</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>647</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>648</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>649</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>182</v>
@@ -3128,25 +3128,25 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>203</v>
@@ -3155,7 +3155,7 @@
         <v>206</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>44</v>
@@ -3164,9 +3164,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>210</v>
@@ -3184,9 +3184,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>213</v>
@@ -3204,9 +3204,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>221</v>
@@ -3215,7 +3215,7 @@
         <v>223</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>165</v>
@@ -3224,9 +3224,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>227</v>
@@ -3244,9 +3244,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>252</v>
@@ -3264,9 +3264,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>261</v>
@@ -3284,9 +3284,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>271</v>
@@ -3304,9 +3304,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B21" s="34" t="s">
         <v>281</v>
@@ -3324,9 +3324,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>286</v>
@@ -3344,38 +3344,38 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>290</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>651</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>688</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>652</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>689</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>653</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="65" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>149</v>
@@ -3384,15 +3384,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>291</v>
@@ -3404,12 +3404,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>293</v>
@@ -3424,9 +3424,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>296</v>
@@ -3435,7 +3435,7 @@
         <v>297</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>149</v>
@@ -3444,9 +3444,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B28" s="34" t="s">
         <v>298</v>
@@ -3455,7 +3455,7 @@
         <v>299</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>130</v>
@@ -3464,9 +3464,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>300</v>
@@ -3484,9 +3484,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>304</v>
@@ -3504,45 +3504,45 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="D31" s="49" t="s">
-        <v>691</v>
+      <c r="D31" s="39" t="s">
+        <v>690</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B32" s="33" t="s">
         <v>309</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="40"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="31" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>311</v>
@@ -3560,9 +3560,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>315</v>
@@ -3580,9 +3580,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>319</v>
@@ -3600,9 +3600,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="31" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>322</v>
@@ -3617,12 +3617,12 @@
         <v>130</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B37" s="34" t="s">
         <v>325</v>
@@ -3631,63 +3631,63 @@
         <v>326</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>327</v>
+        <v>719</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>130</v>
       </c>
       <c r="F37" s="14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="31" t="s">
+        <v>511</v>
+      </c>
+      <c r="B38" s="33" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.15">
-      <c r="A38" s="31" t="s">
+      <c r="C38" s="40" t="s">
+        <v>329</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+      <c r="A39" s="31" t="s">
         <v>512</v>
       </c>
-      <c r="B38" s="33" t="s">
-        <v>329</v>
-      </c>
-      <c r="C38" s="38" t="s">
-        <v>330</v>
-      </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="6" t="s">
+      <c r="B39" s="34" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A39" s="31" t="s">
-        <v>513</v>
-      </c>
-      <c r="B39" s="34" t="s">
+      <c r="C39" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>686</v>
-      </c>
-      <c r="D39" s="22" t="s">
+      <c r="E39" s="11" t="s">
         <v>333</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>334</v>
       </c>
       <c r="F39" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A40" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B40" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>335</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="D40" s="21" t="s">
         <v>336</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>337</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>130</v>
@@ -3696,18 +3696,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="31" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B41" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="23" t="s">
         <v>339</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>340</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>180</v>
@@ -3716,34 +3716,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="31" t="s">
+        <v>515</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>340</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>341</v>
+      </c>
+      <c r="D42" s="41"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+      <c r="A43" s="31" t="s">
         <v>516</v>
       </c>
-      <c r="B42" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>342</v>
-      </c>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="6" t="s">
+      <c r="B43" s="34" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A43" s="31" t="s">
-        <v>517</v>
-      </c>
-      <c r="B43" s="34" t="s">
+      <c r="C43" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>345</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>346</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>44</v>
@@ -3752,18 +3752,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B44" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="21" t="s">
         <v>348</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>349</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>44</v>
@@ -3772,78 +3772,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
+        <v>694</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>351</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>695</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>352</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A46" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B46" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>696</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>695</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>353</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>697</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>696</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>354</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="104" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" ht="108" x14ac:dyDescent="0.2">
       <c r="A47" s="31" t="s">
+        <v>649</v>
+      </c>
+      <c r="B47" s="34" t="s">
         <v>650</v>
       </c>
-      <c r="B47" s="34" t="s">
-        <v>651</v>
-      </c>
       <c r="C47" s="11" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B48" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="20" t="s">
         <v>356</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>357</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>284</v>
@@ -3852,15 +3852,15 @@
         <v>285</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B49" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>358</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>359</v>
       </c>
       <c r="D49" s="14">
         <v>-8.73</v>
@@ -3872,38 +3872,38 @@
         <v>289</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B51" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>362</v>
-      </c>
       <c r="D51" s="14" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>98</v>
@@ -3912,38 +3912,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B52" s="34" t="s">
+        <v>362</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="24" t="s">
+        <v>718</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>364</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>719</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>365</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="117" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" ht="132" x14ac:dyDescent="0.2">
       <c r="A53" s="31" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B53" s="34" t="s">
+        <v>365</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>367</v>
-      </c>
       <c r="D53" s="14" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>44</v>
@@ -3952,18 +3952,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="31" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B54" s="34" t="s">
+        <v>367</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="14" t="s">
         <v>369</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>370</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>187</v>
@@ -3972,18 +3972,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A55" s="31" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B55" s="34" t="s">
+        <v>370</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>371</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>372</v>
-      </c>
       <c r="D55" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>284</v>
@@ -3992,15 +3992,15 @@
         <v>285</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B56" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>373</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>374</v>
       </c>
       <c r="D56" s="14">
         <v>-8.73</v>
@@ -4012,58 +4012,58 @@
         <v>289</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B59" s="34" t="s">
+        <v>376</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>378</v>
-      </c>
       <c r="D59" s="21" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>149</v>
@@ -4072,110 +4072,110 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B60" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="38" t="s">
+      <c r="C60" s="40" t="s">
+        <v>680</v>
+      </c>
+      <c r="D60" s="41"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A61" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>379</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="D60" s="39"/>
-      <c r="E60" s="40"/>
-      <c r="F60" s="6" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A61" s="31" t="s">
+      <c r="D61" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A62" s="31" t="s">
         <v>534</v>
       </c>
-      <c r="B61" s="34" t="s">
-        <v>380</v>
-      </c>
-      <c r="C61" s="11" t="s">
+      <c r="B62" s="34" t="s">
+        <v>381</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>682</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D62" s="11" t="s">
         <v>684</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A62" s="31" t="s">
-        <v>535</v>
-      </c>
-      <c r="B62" s="34" t="s">
-        <v>382</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>685</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="11" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="31" t="s">
+        <v>535</v>
+      </c>
+      <c r="B63" s="33" t="s">
+        <v>659</v>
+      </c>
+      <c r="C63" s="40" t="s">
+        <v>665</v>
+      </c>
+      <c r="D63" s="41"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="6" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="31" t="s">
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="31" t="s">
         <v>536</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B64" s="34" t="s">
         <v>660</v>
       </c>
-      <c r="C63" s="38" t="s">
-        <v>666</v>
-      </c>
-      <c r="D63" s="39"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="6" t="s">
+      <c r="C64" s="21" t="s">
+        <v>663</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A64" s="31" t="s">
-        <v>537</v>
-      </c>
-      <c r="B64" s="34" t="s">
-        <v>661</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>664</v>
-      </c>
-      <c r="D64" s="11" t="s">
+      <c r="E64" s="11" t="s">
         <v>385</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>386</v>
       </c>
       <c r="F64" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="31" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>149</v>
@@ -4184,54 +4184,54 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="31" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C66" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="D66" s="11" t="s">
         <v>388</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>389</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F66" s="11" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="31" t="s">
+        <v>539</v>
+      </c>
+      <c r="B67" s="33" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="31" t="s">
+      <c r="C67" s="40" t="s">
+        <v>391</v>
+      </c>
+      <c r="D67" s="41"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A68" s="31" t="s">
         <v>540</v>
       </c>
-      <c r="B67" s="33" t="s">
-        <v>391</v>
-      </c>
-      <c r="C67" s="38" t="s">
-        <v>392</v>
-      </c>
-      <c r="D67" s="39"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="6" t="s">
+      <c r="B68" s="34" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A68" s="31" t="s">
-        <v>541</v>
-      </c>
-      <c r="B68" s="34" t="s">
+      <c r="C68" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="C68" s="11" t="s">
-        <v>395</v>
-      </c>
       <c r="D68" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>130</v>
@@ -4240,38 +4240,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="31" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B69" s="34" t="s">
+        <v>395</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>702</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>704</v>
+      </c>
+      <c r="E69" s="11" t="s">
         <v>396</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>703</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>705</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>397</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="31" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B70" s="34" t="s">
+        <v>397</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>399</v>
-      </c>
       <c r="D70" s="11" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>149</v>
@@ -4280,54 +4280,54 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A71" s="31" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B71" s="34" t="s">
+        <v>399</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="C71" s="11" t="s">
-        <v>401</v>
-      </c>
       <c r="D71" s="11" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>165</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="31" t="s">
+        <v>544</v>
+      </c>
+      <c r="B72" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="C72" s="40" t="s">
+        <v>402</v>
+      </c>
+      <c r="D72" s="41"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+      <c r="A73" s="31" t="s">
         <v>545</v>
       </c>
-      <c r="B72" s="33" t="s">
-        <v>402</v>
-      </c>
-      <c r="C72" s="38" t="s">
-        <v>403</v>
-      </c>
-      <c r="D72" s="39"/>
-      <c r="E72" s="40"/>
-      <c r="F72" s="6" t="s">
+      <c r="B73" s="34" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A73" s="31" t="s">
-        <v>546</v>
-      </c>
-      <c r="B73" s="34" t="s">
+      <c r="C73" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="D73" s="11" t="s">
         <v>406</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>407</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>44</v>
@@ -4336,18 +4336,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A74" s="31" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B74" s="34" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C74" s="11" t="s">
+        <v>706</v>
+      </c>
+      <c r="D74" s="11" t="s">
         <v>707</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>708</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>149</v>
@@ -4356,18 +4356,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="31" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B75" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="C75" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C75" s="11" t="s">
-        <v>410</v>
-      </c>
       <c r="D75" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>44</v>
@@ -4376,38 +4376,38 @@
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="31" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B76" s="34" t="s">
+        <v>410</v>
+      </c>
+      <c r="C76" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="D76" s="21" t="s">
         <v>412</v>
       </c>
-      <c r="D76" s="21" t="s">
+      <c r="E76" s="11" t="s">
         <v>413</v>
-      </c>
-      <c r="E76" s="11" t="s">
-        <v>414</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B77" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="D77" s="11" t="s">
         <v>416</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>417</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>149</v>
@@ -4416,34 +4416,34 @@
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="19" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="31" t="s">
+        <v>550</v>
+      </c>
+      <c r="B78" s="33" t="s">
+        <v>417</v>
+      </c>
+      <c r="C78" s="40" t="s">
+        <v>418</v>
+      </c>
+      <c r="D78" s="41"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="31" t="s">
         <v>551</v>
       </c>
-      <c r="B78" s="33" t="s">
-        <v>418</v>
-      </c>
-      <c r="C78" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="D78" s="39"/>
-      <c r="E78" s="40"/>
-      <c r="F78" s="6" t="s">
+      <c r="B79" s="34" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A79" s="31" t="s">
-        <v>552</v>
-      </c>
-      <c r="B79" s="34" t="s">
+      <c r="C79" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="D79" s="11" t="s">
         <v>422</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>423</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>44</v>
@@ -4452,58 +4452,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B80" s="34" t="s">
+        <v>423</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="D80" s="11" t="s">
+        <v>708</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>425</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>709</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>426</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="31" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B81" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="C81" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="D81" s="11" t="s">
+        <v>709</v>
+      </c>
+      <c r="E81" s="11" t="s">
         <v>428</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>710</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>429</v>
       </c>
       <c r="F81" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B82" s="34" t="s">
+        <v>429</v>
+      </c>
+      <c r="C82" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="C82" s="11" t="s">
-        <v>431</v>
-      </c>
       <c r="D82" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>149</v>
@@ -4512,38 +4512,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="31" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B83" s="34" t="s">
+        <v>431</v>
+      </c>
+      <c r="C83" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="D83" s="25" t="s">
         <v>433</v>
       </c>
-      <c r="D83" s="25" t="s">
+      <c r="E83" s="11" t="s">
         <v>434</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>435</v>
       </c>
       <c r="F83" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="31" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C84" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="D84" s="11" t="s">
         <v>436</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>437</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>44</v>
@@ -4552,34 +4552,34 @@
         <v>188</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="B85" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="C85" s="40" t="s">
+        <v>666</v>
+      </c>
+      <c r="D85" s="41"/>
+      <c r="E85" s="42"/>
+      <c r="F85" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.2">
+      <c r="A86" s="31" t="s">
         <v>558</v>
       </c>
-      <c r="B85" s="33" t="s">
+      <c r="B86" s="35" t="s">
         <v>438</v>
       </c>
-      <c r="C85" s="38" t="s">
-        <v>667</v>
-      </c>
-      <c r="D85" s="39"/>
-      <c r="E85" s="40"/>
-      <c r="F85" s="6" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="65" x14ac:dyDescent="0.15">
-      <c r="A86" s="31" t="s">
-        <v>559</v>
-      </c>
-      <c r="B86" s="35" t="s">
+      <c r="C86" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>440</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>441</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>44</v>
@@ -4588,18 +4588,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B87" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="C87" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="D87" s="21" t="s">
         <v>443</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>444</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>149</v>
@@ -4608,38 +4608,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="31" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B88" s="35" t="s">
+        <v>444</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="D88" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="C88" s="11" t="s">
-        <v>712</v>
-      </c>
-      <c r="D88" s="11" t="s">
+      <c r="E88" s="11" t="s">
         <v>446</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>447</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A89" s="31" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B89" s="35" t="s">
+        <v>447</v>
+      </c>
+      <c r="C89" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="C89" s="11" t="s">
-        <v>449</v>
-      </c>
       <c r="D89" s="11" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>149</v>
@@ -4648,38 +4648,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A90" s="31" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B90" s="35" t="s">
+        <v>449</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="D90" s="11" t="s">
+        <v>712</v>
+      </c>
+      <c r="E90" s="11" t="s">
         <v>451</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>713</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>452</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="31" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B91" s="34" t="s">
+        <v>452</v>
+      </c>
+      <c r="C91" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="D91" s="11" t="s">
         <v>454</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>455</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>149</v>
@@ -4688,38 +4688,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A92" s="31" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B92" s="34" t="s">
+        <v>455</v>
+      </c>
+      <c r="C92" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="D92" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="D92" s="11" t="s">
-        <v>458</v>
-      </c>
       <c r="E92" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="104" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:6" ht="108" x14ac:dyDescent="0.2">
       <c r="A93" s="31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B93" s="36" t="s">
+        <v>458</v>
+      </c>
+      <c r="C93" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="D93" s="11" t="s">
         <v>460</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>461</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>149</v>
@@ -4728,38 +4728,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="31" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B94" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="C94" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="D94" s="26" t="s">
         <v>463</v>
       </c>
-      <c r="D94" s="26" t="s">
+      <c r="E94" s="11" t="s">
         <v>464</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>465</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="31" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B95" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="C95" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="D95" s="11" t="s">
         <v>467</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>468</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>44</v>
@@ -4768,38 +4768,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A96" s="31" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B96" s="34" t="s">
+        <v>468</v>
+      </c>
+      <c r="C96" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="D96" s="21" t="s">
         <v>470</v>
       </c>
-      <c r="D96" s="21" t="s">
-        <v>471</v>
-      </c>
       <c r="E96" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A97" s="31" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B97" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="C97" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="C97" s="11" t="s">
-        <v>473</v>
-      </c>
       <c r="D97" s="11" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>149</v>
@@ -4824,8 +4824,8 @@
     <mergeCell ref="C67:E67"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D94" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D31" r:id="rId2" xr:uid="{02460488-3DB6-824C-B87B-023C2082D683}"/>
+    <hyperlink ref="D94" r:id="rId1"/>
+    <hyperlink ref="D31" r:id="rId2"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4834,7 +4834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -4845,42 +4845,42 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
+        <v>570</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
         <v>571</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="31" t="s">
+      <c r="B2" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
         <v>572</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="31" t="s">
-        <v>573</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>7</v>
@@ -4896,26 +4896,26 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
+        <v>573</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
+    </row>
+    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
         <v>574</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="44"/>
-    </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A5" s="31" t="s">
-        <v>575</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>95</v>
@@ -4924,15 +4924,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>105</v>
@@ -4941,9 +4941,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>108</v>
@@ -4958,15 +4958,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>115</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>131</v>
@@ -4975,9 +4975,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>134</v>
@@ -4992,9 +4992,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>138</v>
@@ -5009,9 +5009,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>141</v>
@@ -5026,9 +5026,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>143</v>
@@ -5043,9 +5043,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>146</v>
@@ -5060,9 +5060,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>152</v>
@@ -5077,15 +5077,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>155</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>156</v>
@@ -5094,15 +5094,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>157</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>156</v>
@@ -5111,15 +5111,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>158</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>156</v>
@@ -5128,9 +5128,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>159</v>
@@ -5145,15 +5145,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>162</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>163</v>
@@ -5162,9 +5162,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="65" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>164</v>
@@ -5179,9 +5179,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="52" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>171</v>
@@ -5196,9 +5196,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="52" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>177</v>
@@ -5213,9 +5213,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="52" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>181</v>
@@ -5230,20 +5230,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
+        <v>593</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="46"/>
+    </row>
+    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" s="31" t="s">
         <v>594</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
-    </row>
-    <row r="25" spans="1:5" ht="52" x14ac:dyDescent="0.15">
-      <c r="A25" s="31" t="s">
-        <v>595</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>191</v>
@@ -5258,15 +5258,15 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>196</v>
@@ -5275,15 +5275,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>197</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>198</v>
@@ -5292,15 +5292,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>201</v>
@@ -5309,15 +5309,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>202</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>204</v>
@@ -5326,9 +5326,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>205</v>
@@ -5343,9 +5343,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>215</v>
@@ -5360,9 +5360,9 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B32" s="30" t="s">
         <v>220</v>
@@ -5375,9 +5375,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A33" s="31" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B33" s="30" t="s">
         <v>224</v>
@@ -5392,9 +5392,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="31" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B34" s="30" t="s">
         <v>228</v>
@@ -5409,9 +5409,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B35" s="30" t="s">
         <v>232</v>
@@ -5426,9 +5426,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="52" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A36" s="31" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B36" s="30" t="s">
         <v>235</v>
@@ -5443,15 +5443,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="31" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B37" s="30" t="s">
         <v>238</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>239</v>
@@ -5460,9 +5460,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="31" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B38" s="30" t="s">
         <v>240</v>
@@ -5477,20 +5477,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="31" t="s">
+        <v>608</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="46"/>
+    </row>
+    <row r="40" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="31" t="s">
         <v>609</v>
-      </c>
-      <c r="B39" s="42" t="s">
-        <v>242</v>
-      </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="44"/>
-    </row>
-    <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.15">
-      <c r="A40" s="31" t="s">
-        <v>610</v>
       </c>
       <c r="B40" s="30" t="s">
         <v>243</v>
@@ -5505,9 +5505,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="31" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B41" s="30" t="s">
         <v>247</v>
@@ -5522,9 +5522,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="31" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B42" s="30" t="s">
         <v>251</v>
@@ -5539,9 +5539,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="31" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>258</v>
@@ -5556,9 +5556,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="31" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>260</v>
@@ -5573,9 +5573,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="31" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B45" s="30" t="s">
         <v>262</v>
@@ -5590,9 +5590,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="31" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B46" s="30" t="s">
         <v>267</v>
@@ -5607,9 +5607,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A47" s="31" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>270</v>
@@ -5624,9 +5624,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A48" s="31" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>275</v>
@@ -5641,9 +5641,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A49" s="31" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B49" s="30" t="s">
         <v>278</v>
@@ -5672,7 +5672,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -5683,36 +5683,36 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>476</v>
-      </c>
-      <c r="B1" s="47" t="s">
+        <v>475</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>620</v>
-      </c>
-      <c r="B2" s="46" t="s">
+        <v>619</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5736,9 +5736,9 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>12</v>
@@ -5775,9 +5775,9 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:27" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>15</v>
@@ -5792,9 +5792,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>23</v>
@@ -5809,9 +5809,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>27</v>
@@ -5826,9 +5826,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>30</v>
@@ -5843,9 +5843,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="28" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>33</v>
@@ -5860,9 +5860,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>37</v>
@@ -5877,9 +5877,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="56" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>41</v>
@@ -5894,9 +5894,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>48</v>
@@ -5911,9 +5911,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>52</v>
@@ -5928,9 +5928,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>56</v>
@@ -5945,9 +5945,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>60</v>
@@ -5962,9 +5962,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="56" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>64</v>
@@ -5979,9 +5979,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>69</v>
@@ -5996,9 +5996,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>73</v>
@@ -6013,9 +6013,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>78</v>
@@ -6030,9 +6030,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>82</v>
@@ -6047,9 +6047,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="112" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>86</v>
@@ -6064,9 +6064,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>90</v>
@@ -6081,9 +6081,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>94</v>
@@ -6098,9 +6098,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>100</v>
@@ -6115,9 +6115,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>106</v>
@@ -6132,9 +6132,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>113</v>
@@ -6149,9 +6149,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>118</v>
@@ -6166,9 +6166,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>122</v>
@@ -6183,9 +6183,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>126</v>
@@ -6196,7 +6196,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
Fix #24, #25, #35, #41, #32
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE\MIAPPE_Checklist-Data-Model-v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpommier/src/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DFA3A5-D10A-A24C-BE65-6EAFB0F1C94E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="28800" yWindow="-3060" windowWidth="30260" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -1062,9 +1063,6 @@
     <t>Biological material ID</t>
   </si>
   <si>
-    <t>Code used to identify the biological material in the data file. Should be unique within the Investigation. Can correspond to experimental plant ID, seed lot ID, etc...</t>
-  </si>
-  <si>
     <t>INRA:W95115_inra_2001; INRA:inra_kernel_2351; Rothamsted:rres_GK090847</t>
   </si>
   <si>
@@ -1246,9 +1244,6 @@
     <t>Observation unit ID</t>
   </si>
   <si>
-    <t>Identifier used to identify the observation unit in data files containing the values observed or measured on that unit. Must be locally unique</t>
-  </si>
-  <si>
     <t>plot:894</t>
   </si>
   <si>
@@ -1258,16 +1253,7 @@
     <t>External ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier for the observation unit in a persistant repository, comprises the name of the repository and the identifier of the observation unit therein. The EBI Biosamples repository is recommended. </t>
-  </si>
-  <si>
     <t>Spatial distribution</t>
-  </si>
-  <si>
-    <t>Type and value of a spatial coordinate (georeference or relative) or level of observation (plot 45, subblock 7, block 2) provided as a key-value pair of the form [type] value. Levels of observation must be consistent with those listed in the Study section.</t>
-  </si>
-  <si>
-    <t>[Latitude] +2.341; [row] 4 ; [X] 3; [Y] 6; [Xm] 35; [Ym] 65; [Block] 1; [Plot] 894</t>
   </si>
   <si>
     <t>Formatted text ([Key] value)</t>
@@ -1337,9 +1323,6 @@
     <t>Date/Time</t>
   </si>
   <si>
-    <t>An identifier for the sample in a persistant repository, comprising the name of the repository and the accession number of the observation unit therein. Submission to the EBI Biosamples repository is recommended</t>
-  </si>
-  <si>
     <t>Biosamples:SAMEA4202911</t>
   </si>
   <si>
@@ -2005,9 +1988,6 @@
     <t>Type of experimental design</t>
   </si>
   <si>
-    <t>Short description of the experimental design, possibly including statistical design. Can be simply 'NA' or 'none' when it doesn't make sense anymore, like for data computed from several studies.</t>
-  </si>
-  <si>
     <t>Type of esperimental  design of the study, in the form of an accession number from the Crop Ontology.</t>
   </si>
   <si>
@@ -2081,10 +2061,6 @@
   </si>
   <si>
     <t>Value of the environment parameter (defined above) constant within the experiment.</t>
-  </si>
-  <si>
-    <t>sowing density
-rooting medium composition; pH</t>
   </si>
   <si>
     <t>300 seeds per m2
@@ -2117,9 +2093,6 @@
   <si>
     <t>field environment condition
 NA</t>
-  </si>
-  <si>
-    <t>URL or File name (of gis or excel file)</t>
   </si>
   <si>
     <t>Zea
@@ -2217,15 +2190,43 @@
     <t>ITQB, Portugal;
 grid.10772.33</t>
   </si>
+  <si>
+    <t>sowing density;
+rooting medium composition; pH</t>
+  </si>
+  <si>
+    <t>Short description of the experimental design, possibly including statistical design. In specific cases, e.g. legacy datasets or data computed from several studies, the experimental design can be "unknown"/"NA", "aggregated/reduced data", or simply 'none'.</t>
+  </si>
+  <si>
+    <t>Type and value of a spatial coordinate (georeference or relative) or level of observation (plot 45, subblock 7, block 2) provided as a key-value pair of the form type:value. Levels of observation must be consistent with those listed in the Study section.</t>
+  </si>
+  <si>
+    <t>Latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; Block:1; Plot:894</t>
+  </si>
+  <si>
+    <t>Code used to identify the biological material in the data file. Should be unique within the Investigation. Can correspond to experimental plant ID, seed lot ID, etc… This material identification is different from a BiosampleID which corresponds to Observation Unit or Samples sections below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier used to identify the observation unit in data files containing the values observed or measured on that unit. Must be locally unique. </t>
+  </si>
+  <si>
+    <t>Identifier for the observation unit in a persistant repository, comprises the name of the repository and the identifier of the observation unit therein. The EBI Biosamples repository can be used. URI are recommended when possible.</t>
+  </si>
+  <si>
+    <t>An identifier for the sample in a persistant repository, comprising the name of the repository and the accession number of the observation unit therein. Submission to the EBI Biosamples repository is recommended. URI are recommended when possible.</t>
+  </si>
+  <si>
+    <t>URL or File name (of gis or tabular file like csv or tsv)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2321,13 +2322,6 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2559,9 +2553,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2588,9 +2579,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2902,39 +2896,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="51.83203125" customWidth="1"/>
+    <col min="4" max="4" width="41.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>3</v>
@@ -2952,25 +2946,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>18</v>
@@ -2988,9 +2982,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A5" s="31" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>127</v>
@@ -3008,9 +3002,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="91" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>133</v>
@@ -3028,9 +3022,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>150</v>
@@ -3048,9 +3042,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>166</v>
@@ -3068,9 +3062,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>173</v>
@@ -3079,7 +3073,7 @@
         <v>174</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>44</v>
@@ -3088,9 +3082,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>175</v>
@@ -3099,18 +3093,18 @@
         <v>176</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>182</v>
@@ -3128,25 +3122,25 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A12" s="31" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="39" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="31" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>203</v>
@@ -3155,7 +3149,7 @@
         <v>206</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>44</v>
@@ -3164,9 +3158,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="31" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>210</v>
@@ -3184,9 +3178,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A15" s="31" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>213</v>
@@ -3204,9 +3198,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="31" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>221</v>
@@ -3215,7 +3209,7 @@
         <v>223</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>165</v>
@@ -3224,9 +3218,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="31" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>227</v>
@@ -3244,9 +3238,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="31" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>252</v>
@@ -3264,9 +3258,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="31" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>261</v>
@@ -3284,9 +3278,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>271</v>
@@ -3304,9 +3298,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="B21" s="34" t="s">
         <v>281</v>
@@ -3324,9 +3318,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="31" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>286</v>
@@ -3344,38 +3338,38 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="31" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>290</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A24" s="31" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>657</v>
+        <v>712</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>149</v>
@@ -3384,15 +3378,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A25" s="31" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>291</v>
@@ -3404,12 +3398,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="31" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>293</v>
@@ -3424,9 +3418,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A27" s="31" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>296</v>
@@ -3435,7 +3429,7 @@
         <v>297</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>149</v>
@@ -3444,9 +3438,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A28" s="31" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="B28" s="34" t="s">
         <v>298</v>
@@ -3455,7 +3449,7 @@
         <v>299</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>130</v>
@@ -3464,9 +3458,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="31" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>300</v>
@@ -3484,9 +3478,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="31" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>304</v>
@@ -3504,9 +3498,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A31" s="31" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>307</v>
@@ -3514,35 +3508,35 @@
       <c r="C31" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="D31" s="39" t="s">
-        <v>690</v>
+      <c r="D31" s="49" t="s">
+        <v>682</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>693</v>
+        <v>719</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="31" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="B32" s="33" t="s">
         <v>309</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="39" t="s">
         <v>310</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="6" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A33" s="31" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>311</v>
@@ -3560,9 +3554,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="31" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>315</v>
@@ -3580,9 +3574,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A35" s="31" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>319</v>
@@ -3600,9 +3594,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="31" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>322</v>
@@ -3620,9 +3614,9 @@
         <v>327</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="31" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="B37" s="34" t="s">
         <v>325</v>
@@ -3631,7 +3625,7 @@
         <v>326</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>130</v>
@@ -3640,31 +3634,31 @@
         <v>327</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A38" s="31" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="B38" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="39" t="s">
         <v>329</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="42"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="6" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A39" s="31" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="B39" s="34" t="s">
         <v>331</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>332</v>
@@ -3676,9 +3670,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A40" s="31" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="B40" s="34" t="s">
         <v>334</v>
@@ -3696,9 +3690,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="31" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="B41" s="34" t="s">
         <v>337</v>
@@ -3716,34 +3710,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A42" s="31" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="B42" s="33" t="s">
         <v>340</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="39" t="s">
         <v>341</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="42"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41"/>
       <c r="F42" s="6" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A43" s="31" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="B43" s="34" t="s">
         <v>343</v>
       </c>
       <c r="C43" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>344</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>345</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>44</v>
@@ -3752,18 +3746,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A44" s="31" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B44" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>346</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="21" t="s">
         <v>347</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>348</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>44</v>
@@ -3772,78 +3766,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A45" s="31" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>349</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>350</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>694</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>351</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A46" s="31" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="B46" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>686</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>352</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>696</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>695</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>353</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="108" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="104" x14ac:dyDescent="0.15">
       <c r="A47" s="31" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>698</v>
+        <v>689</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>697</v>
+        <v>688</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A48" s="31" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B48" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>354</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="20" t="s">
         <v>355</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>356</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>284</v>
@@ -3852,15 +3846,15 @@
         <v>285</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A49" s="31" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="B49" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>357</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>358</v>
       </c>
       <c r="D49" s="14">
         <v>-8.73</v>
@@ -3872,38 +3866,38 @@
         <v>289</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A50" s="31" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" s="31" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="B51" s="34" t="s">
+        <v>359</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>361</v>
-      </c>
       <c r="D51" s="14" t="s">
-        <v>700</v>
+        <v>691</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>98</v>
@@ -3912,38 +3906,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A52" s="31" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="B52" s="34" t="s">
+        <v>361</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="24" t="s">
+        <v>709</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>363</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>718</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>364</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="132" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="117" x14ac:dyDescent="0.15">
       <c r="A53" s="31" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="B53" s="34" t="s">
+        <v>364</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>366</v>
-      </c>
       <c r="D53" s="14" t="s">
-        <v>701</v>
+        <v>692</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>44</v>
@@ -3952,18 +3946,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="31" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="B54" s="34" t="s">
+        <v>366</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="14" t="s">
         <v>368</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>369</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>187</v>
@@ -3972,18 +3966,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A55" s="31" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="B55" s="34" t="s">
+        <v>369</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>371</v>
-      </c>
       <c r="D55" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>284</v>
@@ -3992,15 +3986,15 @@
         <v>285</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A56" s="31" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="B56" s="34" t="s">
+        <v>371</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>372</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>373</v>
       </c>
       <c r="D56" s="14">
         <v>-8.73</v>
@@ -4012,58 +4006,58 @@
         <v>289</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A57" s="31" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A58" s="31" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>700</v>
+        <v>691</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A59" s="31" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B59" s="34" t="s">
+        <v>375</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>377</v>
-      </c>
       <c r="D59" s="21" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>149</v>
@@ -4072,110 +4066,110 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="31" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="B60" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="40" t="s">
-        <v>680</v>
-      </c>
-      <c r="D60" s="41"/>
-      <c r="E60" s="42"/>
+      <c r="C60" s="39" t="s">
+        <v>673</v>
+      </c>
+      <c r="D60" s="40"/>
+      <c r="E60" s="41"/>
       <c r="F60" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A61" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="B61" s="34" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A61" s="31" t="s">
-        <v>533</v>
-      </c>
-      <c r="B61" s="34" t="s">
+      <c r="C61" s="11" t="s">
+        <v>674</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>711</v>
+      </c>
+      <c r="E61" s="11" t="s">
         <v>379</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>681</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>380</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A62" s="31" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="11" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="31" t="s">
+        <v>529</v>
+      </c>
+      <c r="B63" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>658</v>
+      </c>
+      <c r="D63" s="40"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="6" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="31" t="s">
-        <v>535</v>
-      </c>
-      <c r="B63" s="33" t="s">
-        <v>659</v>
-      </c>
-      <c r="C63" s="40" t="s">
-        <v>665</v>
-      </c>
-      <c r="D63" s="41"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="6" t="s">
+    <row r="64" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A64" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>653</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>656</v>
+      </c>
+      <c r="D64" s="11" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="31" t="s">
-        <v>536</v>
-      </c>
-      <c r="B64" s="34" t="s">
-        <v>660</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>663</v>
-      </c>
-      <c r="D64" s="11" t="s">
+      <c r="E64" s="11" t="s">
         <v>384</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>385</v>
       </c>
       <c r="F64" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A65" s="31" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>149</v>
@@ -4184,54 +4178,54 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="31" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="C66" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="D66" s="11" t="s">
         <v>387</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>388</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F66" s="11" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="31" t="s">
+        <v>533</v>
+      </c>
+      <c r="B67" s="33" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="31" t="s">
-        <v>539</v>
-      </c>
-      <c r="B67" s="33" t="s">
+      <c r="C67" s="39" t="s">
         <v>390</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="D67" s="40"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="D67" s="41"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="6" t="s">
+    </row>
+    <row r="68" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A68" s="31" t="s">
+        <v>534</v>
+      </c>
+      <c r="B68" s="34" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A68" s="31" t="s">
-        <v>540</v>
-      </c>
-      <c r="B68" s="34" t="s">
+      <c r="C68" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="C68" s="11" t="s">
-        <v>394</v>
-      </c>
       <c r="D68" s="11" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>130</v>
@@ -4240,38 +4234,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A69" s="31" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="B69" s="34" t="s">
+        <v>394</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>693</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>695</v>
+      </c>
+      <c r="E69" s="11" t="s">
         <v>395</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>702</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>704</v>
-      </c>
-      <c r="E69" s="11" t="s">
-        <v>396</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A70" s="31" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="B70" s="34" t="s">
+        <v>396</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>398</v>
-      </c>
       <c r="D70" s="11" t="s">
-        <v>715</v>
+        <v>706</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>149</v>
@@ -4280,18 +4274,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A71" s="31" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="B71" s="34" t="s">
+        <v>398</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="C71" s="11" t="s">
-        <v>400</v>
-      </c>
       <c r="D71" s="11" t="s">
-        <v>705</v>
+        <v>696</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>165</v>
@@ -4300,34 +4294,34 @@
         <v>327</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A72" s="31" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="B72" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="C72" s="39" t="s">
         <v>401</v>
       </c>
-      <c r="C72" s="40" t="s">
+      <c r="D72" s="40"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="D72" s="41"/>
-      <c r="E72" s="42"/>
-      <c r="F72" s="6" t="s">
+    </row>
+    <row r="73" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A73" s="31" t="s">
+        <v>539</v>
+      </c>
+      <c r="B73" s="34" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A73" s="31" t="s">
-        <v>545</v>
-      </c>
-      <c r="B73" s="34" t="s">
+      <c r="C73" s="11" t="s">
+        <v>716</v>
+      </c>
+      <c r="D73" s="11" t="s">
         <v>404</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>406</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>44</v>
@@ -4336,18 +4330,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A74" s="31" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="B74" s="34" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>706</v>
+        <v>697</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>149</v>
@@ -4356,18 +4350,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A75" s="31" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>409</v>
+        <v>717</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>44</v>
@@ -4376,38 +4370,38 @@
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A76" s="31" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>411</v>
+        <v>713</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>412</v>
+        <v>714</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="31" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>149</v>
@@ -4416,34 +4410,34 @@
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A78" s="31" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="B78" s="33" t="s">
+        <v>412</v>
+      </c>
+      <c r="C78" s="39" t="s">
+        <v>413</v>
+      </c>
+      <c r="D78" s="40"/>
+      <c r="E78" s="41"/>
+      <c r="F78" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A79" s="31" t="s">
+        <v>545</v>
+      </c>
+      <c r="B79" s="34" t="s">
+        <v>415</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="D79" s="11" t="s">
         <v>417</v>
-      </c>
-      <c r="C78" s="40" t="s">
-        <v>418</v>
-      </c>
-      <c r="D78" s="41"/>
-      <c r="E78" s="42"/>
-      <c r="F78" s="6" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="31" t="s">
-        <v>551</v>
-      </c>
-      <c r="B79" s="34" t="s">
-        <v>420</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>422</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>44</v>
@@ -4452,58 +4446,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A80" s="31" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="B80" s="34" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>708</v>
+        <v>699</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A81" s="31" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>709</v>
+        <v>700</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F81" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A82" s="31" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>149</v>
@@ -4512,38 +4506,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="31" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B83" s="34" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D83" s="25" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F83" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A84" s="31" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>435</v>
+        <v>718</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>44</v>
@@ -4552,34 +4546,34 @@
         <v>188</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="31" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="B85" s="33" t="s">
-        <v>437</v>
-      </c>
-      <c r="C85" s="40" t="s">
-        <v>666</v>
-      </c>
-      <c r="D85" s="41"/>
-      <c r="E85" s="42"/>
+        <v>431</v>
+      </c>
+      <c r="C85" s="39" t="s">
+        <v>659</v>
+      </c>
+      <c r="D85" s="40"/>
+      <c r="E85" s="41"/>
       <c r="F85" s="6" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A86" s="31" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>44</v>
@@ -4588,18 +4582,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="31" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>149</v>
@@ -4608,38 +4602,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="31" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A89" s="31" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="B89" s="35" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>149</v>
@@ -4648,38 +4642,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A90" s="31" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="B90" s="35" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="31" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>149</v>
@@ -4688,38 +4682,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A92" s="31" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="B92" s="34" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="108" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="104" x14ac:dyDescent="0.15">
       <c r="A93" s="31" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="B93" s="36" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>149</v>
@@ -4728,38 +4722,38 @@
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="31" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="B94" s="34" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="31" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="B95" s="34" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>44</v>
@@ -4768,38 +4762,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A96" s="31" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="B96" s="34" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A97" s="31" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="B97" s="34" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>149</v>
@@ -4824,8 +4818,8 @@
     <mergeCell ref="C67:E67"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D94" r:id="rId1"/>
-    <hyperlink ref="D31" r:id="rId2"/>
+    <hyperlink ref="D94" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D31" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4834,53 +4828,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
-        <v>570</v>
-      </c>
-      <c r="B1" s="47" t="s">
+        <v>564</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
-        <v>571</v>
-      </c>
-      <c r="B2" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>7</v>
@@ -4896,26 +4890,26 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>573</v>
-      </c>
-      <c r="B4" s="44" t="s">
+        <v>567</v>
+      </c>
+      <c r="B4" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+    </row>
+    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="31" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>95</v>
@@ -4924,15 +4918,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>105</v>
@@ -4941,9 +4935,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>108</v>
@@ -4958,15 +4952,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>115</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>131</v>
@@ -4975,9 +4969,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>134</v>
@@ -4992,9 +4986,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>138</v>
@@ -5009,9 +5003,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>141</v>
@@ -5026,9 +5020,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="31" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>143</v>
@@ -5043,9 +5037,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="31" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>146</v>
@@ -5060,9 +5054,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="31" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>152</v>
@@ -5077,15 +5071,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="31" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>155</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>156</v>
@@ -5094,15 +5088,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="31" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>157</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>156</v>
@@ -5111,15 +5105,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="31" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>158</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>156</v>
@@ -5128,9 +5122,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="31" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>159</v>
@@ -5145,15 +5139,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="31" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>162</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>163</v>
@@ -5162,9 +5156,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="65" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>164</v>
@@ -5179,9 +5173,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>171</v>
@@ -5196,9 +5190,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A22" s="31" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>177</v>
@@ -5213,9 +5207,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A23" s="31" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>181</v>
@@ -5230,20 +5224,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="31" t="s">
-        <v>593</v>
-      </c>
-      <c r="B24" s="44" t="s">
+        <v>587</v>
+      </c>
+      <c r="B24" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
-    </row>
-    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
+    </row>
+    <row r="25" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A25" s="31" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>191</v>
@@ -5258,15 +5252,15 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="31" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>196</v>
@@ -5275,15 +5269,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="31" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>197</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>198</v>
@@ -5292,15 +5286,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="31" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>201</v>
@@ -5309,15 +5303,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="31" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>202</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>204</v>
@@ -5326,9 +5320,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="31" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>205</v>
@@ -5343,9 +5337,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A31" s="31" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>215</v>
@@ -5360,9 +5354,9 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="31" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B32" s="30" t="s">
         <v>220</v>
@@ -5375,9 +5369,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A33" s="31" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="B33" s="30" t="s">
         <v>224</v>
@@ -5392,9 +5386,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A34" s="31" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B34" s="30" t="s">
         <v>228</v>
@@ -5409,9 +5403,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="31" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="B35" s="30" t="s">
         <v>232</v>
@@ -5426,9 +5420,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A36" s="31" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B36" s="30" t="s">
         <v>235</v>
@@ -5443,15 +5437,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="31" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="B37" s="30" t="s">
         <v>238</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>239</v>
@@ -5460,9 +5454,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="31" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="B38" s="30" t="s">
         <v>240</v>
@@ -5477,20 +5471,20 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="31" t="s">
-        <v>608</v>
-      </c>
-      <c r="B39" s="44" t="s">
+        <v>602</v>
+      </c>
+      <c r="B39" s="43" t="s">
         <v>242</v>
       </c>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
-    </row>
-    <row r="40" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="45"/>
+    </row>
+    <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="31" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="B40" s="30" t="s">
         <v>243</v>
@@ -5505,9 +5499,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" s="31" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="B41" s="30" t="s">
         <v>247</v>
@@ -5522,9 +5516,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A42" s="31" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="B42" s="30" t="s">
         <v>251</v>
@@ -5539,9 +5533,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" s="31" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>258</v>
@@ -5556,9 +5550,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A44" s="31" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>260</v>
@@ -5573,9 +5567,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" s="31" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="B45" s="30" t="s">
         <v>262</v>
@@ -5590,9 +5584,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="31" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="B46" s="30" t="s">
         <v>267</v>
@@ -5607,9 +5601,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A47" s="31" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>270</v>
@@ -5624,9 +5618,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A48" s="31" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>275</v>
@@ -5641,9 +5635,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A49" s="31" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B49" s="30" t="s">
         <v>278</v>
@@ -5672,7 +5666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
@@ -5683,36 +5677,36 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
-        <v>475</v>
-      </c>
-      <c r="B1" s="49" t="s">
+        <v>469</v>
+      </c>
+      <c r="B1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="B2" s="48" t="s">
+        <v>613</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5736,9 +5730,9 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>12</v>
@@ -5775,9 +5769,9 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>15</v>
@@ -5792,9 +5786,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="31" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>23</v>
@@ -5809,9 +5803,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>27</v>
@@ -5826,9 +5820,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>30</v>
@@ -5843,9 +5837,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>33</v>
@@ -5860,9 +5854,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>37</v>
@@ -5877,9 +5871,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>41</v>
@@ -5894,9 +5888,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>48</v>
@@ -5911,9 +5905,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="31" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>52</v>
@@ -5928,9 +5922,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="31" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>56</v>
@@ -5945,9 +5939,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A14" s="31" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>60</v>
@@ -5962,9 +5956,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A15" s="31" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>64</v>
@@ -5979,9 +5973,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="31" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>69</v>
@@ -5996,9 +5990,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="31" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>73</v>
@@ -6013,9 +6007,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A18" s="31" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>78</v>
@@ -6030,9 +6024,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A19" s="31" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>82</v>
@@ -6047,9 +6041,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="112" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>86</v>
@@ -6064,9 +6058,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>90</v>
@@ -6081,9 +6075,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="84" x14ac:dyDescent="0.15">
       <c r="A22" s="31" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>94</v>
@@ -6098,9 +6092,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="31" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>100</v>
@@ -6115,9 +6109,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="31" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>106</v>
@@ -6132,9 +6126,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A25" s="31" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>113</v>
@@ -6149,9 +6143,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="31" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>118</v>
@@ -6166,9 +6160,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="31" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>122</v>
@@ -6183,9 +6177,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="31" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>126</v>
@@ -6196,7 +6190,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
Correct DM-73 Format (after #41) and some typos
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpommier/src/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hania/Code/MIAPPE/MIAPPE-checklist/MIAPPE_Checklist-Data-Model-v1.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DFA3A5-D10A-A24C-BE65-6EAFB0F1C94E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC18F93-52AD-1241-A46A-F717CE600FFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3060" windowWidth="30260" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="8660" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -1038,9 +1038,6 @@
     <t>Description of the format of the data file. May be a standard file format name, or a description of organization of the data in a tabular file.</t>
   </si>
   <si>
-    <t>FASTA; tab-delineated, column headers headers: 1. A 2. B 3. C</t>
-  </si>
-  <si>
     <t>Data file version</t>
   </si>
   <si>
@@ -1187,9 +1184,6 @@
     <t>Free text (see Appendix II)</t>
   </si>
   <si>
-    <t xml:space="preserve">Daily watering 1L per plant. </t>
-  </si>
-  <si>
     <t>List of possible values for the factor.</t>
   </si>
   <si>
@@ -1254,9 +1248,6 @@
   </si>
   <si>
     <t>Spatial distribution</t>
-  </si>
-  <si>
-    <t>Formatted text ([Key] value)</t>
   </si>
   <si>
     <t>Observation Unit factor value</t>
@@ -1368,10 +1359,6 @@
     <t>Accession number of the trait in a suitable controlled vocabulary (Crop Ontology, Trait Ontology).</t>
   </si>
   <si>
-    <t>Term from Plant Trait Ontology, 
-Crop Ontology, or XML Environment Ontology</t>
-  </si>
-  <si>
     <t>Method</t>
   </si>
   <si>
@@ -1396,10 +1383,6 @@
     <t>Textual description of the method, which may extend a method defined in an external reference with specific parameters, e.g. growth stage, inoculation precise organ (leaf number)</t>
   </si>
   <si>
-    <t>1/ Days to anthesis for male flowering was measured in thermal time (GDD: growing degree-days) according to Ritchie J, NeSmith D (1991;Temperature and crop development. Modeling plant a nd soil systems American Society of Agronomy Madison, Wisconsin USA) with TBASE=8°C and T0=30°C.
-2/ Plant height was measured at 5 years with a ruler, one year after Botritis inoculation. </t>
-  </si>
-  <si>
     <t>Reference associated to the method</t>
   </si>
   <si>
@@ -2010,9 +1993,6 @@
   </si>
   <si>
     <t xml:space="preserve">The object of a study is to ascertain the impact of one or more factors on the biological material. Thus, a factor is, by definition a condition that varies between observation units, which may be biotic (pest, disease interaction) or abiotic (treatment and cultural practice) in nature. Depending on the level of the data, an experimental factor can be either  "what is the factor applied to the plant" (ie Unwatered), or the "environmental characterisation" (ie if no rain on unwatered plant : Drought ;  if rain on unwatered plant: Irrigated) </t>
-  </si>
-  <si>
-    <t>An observed variable describe how a measurement has been made. It typically takes the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement.</t>
   </si>
   <si>
     <t>Description of the experimental design</t>
@@ -2131,13 +2111,6 @@
   <si>
     <t>CO_715:0000007
 CO_715:0000011</t>
-  </si>
-  <si>
-    <t>2006-09-27T10:23:21+00:00;
-2006-10-27; 2006-11-13; 2016-11-21</t>
-  </si>
-  <si>
-    <t>Type of observation unit in textual form, usually on of the following: block, sub-lock, plot, plant, trial, sample, pot, replication or replicate, individual, virtual_trial, unit-parcel</t>
   </si>
   <si>
     <t>plot</t>
@@ -2191,32 +2164,60 @@
 grid.10772.33</t>
   </si>
   <si>
-    <t>sowing density;
+    <t>Short description of the experimental design, possibly including statistical design. In specific cases, e.g. legacy datasets or data computed from several studies, the experimental design can be "unknown"/"NA", "aggregated/reduced data", or simply 'none'.</t>
+  </si>
+  <si>
+    <t>Type and value of a spatial coordinate (georeference or relative) or level of observation (plot 45, subblock 7, block 2) provided as a key-value pair of the form type:value. Levels of observation must be consistent with those listed in the Study section.</t>
+  </si>
+  <si>
+    <t>Latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; Block:1; Plot:894</t>
+  </si>
+  <si>
+    <t>Code used to identify the biological material in the data file. Should be unique within the Investigation. Can correspond to experimental plant ID, seed lot ID, etc… This material identification is different from a BiosampleID which corresponds to Observation Unit or Samples sections below.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier used to identify the observation unit in data files containing the values observed or measured on that unit. Must be locally unique. </t>
+  </si>
+  <si>
+    <t>Identifier for the observation unit in a persistant repository, comprises the name of the repository and the identifier of the observation unit therein. The EBI Biosamples repository can be used. URI are recommended when possible.</t>
+  </si>
+  <si>
+    <t>An identifier for the sample in a persistant repository, comprising the name of the repository and the accession number of the observation unit therein. Submission to the EBI Biosamples repository is recommended. URI are recommended when possible.</t>
+  </si>
+  <si>
+    <t>URL or File name (of gis or tabular file like csv or tsv)</t>
+  </si>
+  <si>
+    <t>An observed variable describes how a measurement has been made. It typically takes the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement.</t>
+  </si>
+  <si>
+    <t>Formatted text (Key:value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily watering 1 L per plant. </t>
+  </si>
+  <si>
+    <t>FASTA
+tab-delimited
+column headers headers: 1. A 2. B 3. C</t>
+  </si>
+  <si>
+    <t>sowing density
 rooting medium composition; pH</t>
   </si>
   <si>
-    <t>Short description of the experimental design, possibly including statistical design. In specific cases, e.g. legacy datasets or data computed from several studies, the experimental design can be "unknown"/"NA", "aggregated/reduced data", or simply 'none'.</t>
-  </si>
-  <si>
-    <t>Type and value of a spatial coordinate (georeference or relative) or level of observation (plot 45, subblock 7, block 2) provided as a key-value pair of the form type:value. Levels of observation must be consistent with those listed in the Study section.</t>
-  </si>
-  <si>
-    <t>Latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; Block:1; Plot:894</t>
-  </si>
-  <si>
-    <t>Code used to identify the biological material in the data file. Should be unique within the Investigation. Can correspond to experimental plant ID, seed lot ID, etc… This material identification is different from a BiosampleID which corresponds to Observation Unit or Samples sections below.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier used to identify the observation unit in data files containing the values observed or measured on that unit. Must be locally unique. </t>
-  </si>
-  <si>
-    <t>Identifier for the observation unit in a persistant repository, comprises the name of the repository and the identifier of the observation unit therein. The EBI Biosamples repository can be used. URI are recommended when possible.</t>
-  </si>
-  <si>
-    <t>An identifier for the sample in a persistant repository, comprising the name of the repository and the accession number of the observation unit therein. Submission to the EBI Biosamples repository is recommended. URI are recommended when possible.</t>
-  </si>
-  <si>
-    <t>URL or File name (of gis or tabular file like csv or tsv)</t>
+    <t>2006-09-27T10:23:21+00:00
+2006-10-27; 2006-11-13; 2016-11-21</t>
+  </si>
+  <si>
+    <t>Type of observation unit in textual form, usually one of the following: block, sub-block, plot, plant, trial, sample, pot, replication or replicate, individual, virtual_trial, unit-parcel</t>
+  </si>
+  <si>
+    <t>Days to anthesis for male flowering was measured in thermal time (GDD: growing degree-days) according to Ritchie J, NeSmith D (1991;Temperature and crop development. Modeling plant a nd soil systems American Society of Agronomy Madison, Wisconsin USA) with TBASE=8°C and T0=30°C.
+Plant height was measured at 5 years with a ruler, one year after Botritis inoculation.</t>
+  </si>
+  <si>
+    <t>Term from Plant Trait Ontology, Crop Ontology, or XML Environment Ontology</t>
   </si>
 </sst>
 </file>
@@ -2322,6 +2323,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2553,6 +2555,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2579,12 +2584,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2903,8 +2905,8 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2918,17 +2920,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>3</v>
@@ -2948,23 +2950,23 @@
     </row>
     <row r="3" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>18</v>
@@ -2984,7 +2986,7 @@
     </row>
     <row r="5" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A5" s="31" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>127</v>
@@ -3004,7 +3006,7 @@
     </row>
     <row r="6" spans="1:6" ht="91" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>133</v>
@@ -3024,7 +3026,7 @@
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>150</v>
@@ -3044,7 +3046,7 @@
     </row>
     <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>166</v>
@@ -3064,7 +3066,7 @@
     </row>
     <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>173</v>
@@ -3073,7 +3075,7 @@
         <v>174</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>44</v>
@@ -3084,7 +3086,7 @@
     </row>
     <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>175</v>
@@ -3093,10 +3095,10 @@
         <v>176</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
@@ -3104,7 +3106,7 @@
     </row>
     <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>182</v>
@@ -3124,23 +3126,23 @@
     </row>
     <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A12" s="31" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="6" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="31" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>203</v>
@@ -3149,7 +3151,7 @@
         <v>206</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>44</v>
@@ -3160,7 +3162,7 @@
     </row>
     <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="31" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>210</v>
@@ -3180,7 +3182,7 @@
     </row>
     <row r="15" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A15" s="31" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>213</v>
@@ -3200,7 +3202,7 @@
     </row>
     <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="31" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>221</v>
@@ -3209,7 +3211,7 @@
         <v>223</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>165</v>
@@ -3220,7 +3222,7 @@
     </row>
     <row r="17" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="31" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>227</v>
@@ -3240,7 +3242,7 @@
     </row>
     <row r="18" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="31" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>252</v>
@@ -3260,7 +3262,7 @@
     </row>
     <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="31" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>261</v>
@@ -3280,7 +3282,7 @@
     </row>
     <row r="20" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>271</v>
@@ -3300,7 +3302,7 @@
     </row>
     <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B21" s="34" t="s">
         <v>281</v>
@@ -3320,7 +3322,7 @@
     </row>
     <row r="22" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="31" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>286</v>
@@ -3340,19 +3342,19 @@
     </row>
     <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="31" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>290</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>47</v>
@@ -3360,16 +3362,16 @@
     </row>
     <row r="24" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A24" s="31" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>149</v>
@@ -3380,13 +3382,13 @@
     </row>
     <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A25" s="31" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>291</v>
@@ -3400,10 +3402,10 @@
     </row>
     <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="31" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>293</v>
@@ -3420,7 +3422,7 @@
     </row>
     <row r="27" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A27" s="31" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>296</v>
@@ -3429,7 +3431,7 @@
         <v>297</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>149</v>
@@ -3440,7 +3442,7 @@
     </row>
     <row r="28" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A28" s="31" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="B28" s="34" t="s">
         <v>298</v>
@@ -3449,7 +3451,7 @@
         <v>299</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>130</v>
@@ -3460,7 +3462,7 @@
     </row>
     <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="31" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>300</v>
@@ -3480,7 +3482,7 @@
     </row>
     <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="31" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>304</v>
@@ -3500,7 +3502,7 @@
     </row>
     <row r="31" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A31" s="31" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>307</v>
@@ -3508,11 +3510,11 @@
       <c r="C31" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="D31" s="49" t="s">
-        <v>682</v>
+      <c r="D31" s="39" t="s">
+        <v>676</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>719</v>
+        <v>710</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>188</v>
@@ -3520,23 +3522,23 @@
     </row>
     <row r="32" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="31" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B32" s="33" t="s">
         <v>309</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="D32" s="40"/>
-      <c r="E32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="6" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A33" s="31" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>311</v>
@@ -3556,7 +3558,7 @@
     </row>
     <row r="34" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="31" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>315</v>
@@ -3576,7 +3578,7 @@
     </row>
     <row r="35" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A35" s="31" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="B35" s="34" t="s">
         <v>319</v>
@@ -3596,7 +3598,7 @@
     </row>
     <row r="36" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="31" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>322</v>
@@ -3616,7 +3618,7 @@
     </row>
     <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="31" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="B37" s="34" t="s">
         <v>325</v>
@@ -3625,7 +3627,7 @@
         <v>326</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>130</v>
@@ -3636,29 +3638,29 @@
     </row>
     <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A38" s="31" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="B38" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="40" t="s">
         <v>329</v>
       </c>
-      <c r="D38" s="40"/>
-      <c r="E38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="6" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A39" s="31" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B39" s="34" t="s">
         <v>331</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>332</v>
@@ -3670,9 +3672,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A40" s="31" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B40" s="34" t="s">
         <v>334</v>
@@ -3681,7 +3683,7 @@
         <v>335</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>336</v>
+        <v>714</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>130</v>
@@ -3692,16 +3694,16 @@
     </row>
     <row r="41" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="31" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="B41" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="23" t="s">
         <v>338</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>339</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>180</v>
@@ -3712,32 +3714,32 @@
     </row>
     <row r="42" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A42" s="31" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="B42" s="33" t="s">
+        <v>339</v>
+      </c>
+      <c r="C42" s="40" t="s">
         <v>340</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="D42" s="41"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="6" t="s">
         <v>341</v>
-      </c>
-      <c r="D42" s="40"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="6" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A43" s="31" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="B43" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>706</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>343</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>715</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>344</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>44</v>
@@ -3748,16 +3750,16 @@
     </row>
     <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A44" s="31" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="B44" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="21" t="s">
         <v>346</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>347</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>44</v>
@@ -3768,19 +3770,19 @@
     </row>
     <row r="45" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A45" s="31" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
+        <v>679</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>349</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>685</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>350</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>47</v>
@@ -3788,19 +3790,19 @@
     </row>
     <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A46" s="31" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="B46" s="34" t="s">
+        <v>350</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>681</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>680</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>351</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>687</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>686</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>352</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>47</v>
@@ -3808,19 +3810,19 @@
     </row>
     <row r="47" spans="1:6" ht="104" x14ac:dyDescent="0.15">
       <c r="A47" s="31" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>47</v>
@@ -3828,16 +3830,16 @@
     </row>
     <row r="48" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A48" s="31" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B48" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="20" t="s">
         <v>354</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>355</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>284</v>
@@ -3848,13 +3850,13 @@
     </row>
     <row r="49" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A49" s="31" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B49" s="34" t="s">
+        <v>355</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>356</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>357</v>
       </c>
       <c r="D49" s="14">
         <v>-8.73</v>
@@ -3868,19 +3870,19 @@
     </row>
     <row r="50" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A50" s="31" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B50" s="34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>47</v>
@@ -3888,16 +3890,16 @@
     </row>
     <row r="51" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" s="31" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="B51" s="34" t="s">
+        <v>358</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>359</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="D51" s="14" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>98</v>
@@ -3908,19 +3910,19 @@
     </row>
     <row r="52" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A52" s="31" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="B52" s="34" t="s">
+        <v>360</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>362</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>709</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>363</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>188</v>
@@ -3928,16 +3930,16 @@
     </row>
     <row r="53" spans="1:6" ht="117" x14ac:dyDescent="0.15">
       <c r="A53" s="31" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B53" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>365</v>
-      </c>
       <c r="D53" s="14" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>44</v>
@@ -3948,16 +3950,16 @@
     </row>
     <row r="54" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="31" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="B54" s="34" t="s">
+        <v>365</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>366</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>368</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>187</v>
@@ -3968,16 +3970,16 @@
     </row>
     <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A55" s="31" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B55" s="34" t="s">
+        <v>368</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>370</v>
-      </c>
       <c r="D55" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>284</v>
@@ -3988,13 +3990,13 @@
     </row>
     <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A56" s="31" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B56" s="34" t="s">
+        <v>370</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>371</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>372</v>
       </c>
       <c r="D56" s="14">
         <v>-8.73</v>
@@ -4008,19 +4010,19 @@
     </row>
     <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A57" s="31" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>47</v>
@@ -4028,19 +4030,19 @@
     </row>
     <row r="58" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A58" s="31" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>47</v>
@@ -4048,16 +4050,16 @@
     </row>
     <row r="59" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A59" s="31" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="B59" s="34" t="s">
+        <v>374</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>376</v>
-      </c>
       <c r="D59" s="21" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>149</v>
@@ -4068,35 +4070,35 @@
     </row>
     <row r="60" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="31" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="B60" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="39" t="s">
-        <v>673</v>
-      </c>
-      <c r="D60" s="40"/>
-      <c r="E60" s="41"/>
+      <c r="C60" s="40" t="s">
+        <v>667</v>
+      </c>
+      <c r="D60" s="41"/>
+      <c r="E60" s="42"/>
       <c r="F60" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A61" s="31" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B61" s="34" t="s">
+        <v>377</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>668</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="E61" s="11" t="s">
         <v>378</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>674</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>711</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>379</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>327</v>
@@ -4104,55 +4106,55 @@
     </row>
     <row r="62" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A62" s="31" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="B62" s="34" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="31" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>652</v>
-      </c>
-      <c r="C63" s="39" t="s">
-        <v>658</v>
-      </c>
-      <c r="D63" s="40"/>
-      <c r="E63" s="41"/>
+        <v>647</v>
+      </c>
+      <c r="C63" s="40" t="s">
+        <v>653</v>
+      </c>
+      <c r="D63" s="41"/>
+      <c r="E63" s="42"/>
       <c r="F63" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="31" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="B64" s="34" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D64" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="E64" s="11" t="s">
         <v>383</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>384</v>
       </c>
       <c r="F64" s="14">
         <v>1</v>
@@ -4160,16 +4162,16 @@
     </row>
     <row r="65" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A65" s="31" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="B65" s="34" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>385</v>
+        <v>713</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>149</v>
@@ -4180,52 +4182,52 @@
     </row>
     <row r="66" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="31" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="B66" s="34" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="31" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="B67" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="C67" s="40" t="s">
+        <v>388</v>
+      </c>
+      <c r="D67" s="41"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="6" t="s">
         <v>389</v>
-      </c>
-      <c r="C67" s="39" t="s">
-        <v>390</v>
-      </c>
-      <c r="D67" s="40"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="6" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A68" s="31" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="B68" s="34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>130</v>
@@ -4236,19 +4238,19 @@
     </row>
     <row r="69" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A69" s="31" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="B69" s="34" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>47</v>
@@ -4256,16 +4258,16 @@
     </row>
     <row r="70" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A70" s="31" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B70" s="34" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>149</v>
@@ -4276,16 +4278,16 @@
     </row>
     <row r="71" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A71" s="31" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B71" s="34" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>696</v>
+        <v>716</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>165</v>
@@ -4296,32 +4298,32 @@
     </row>
     <row r="72" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A72" s="31" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="B72" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="C72" s="40" t="s">
+        <v>399</v>
+      </c>
+      <c r="D72" s="41"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="6" t="s">
         <v>400</v>
-      </c>
-      <c r="C72" s="39" t="s">
-        <v>401</v>
-      </c>
-      <c r="D72" s="40"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="6" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A73" s="31" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="B73" s="34" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>716</v>
+        <v>707</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>44</v>
@@ -4332,16 +4334,16 @@
     </row>
     <row r="74" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A74" s="31" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="B74" s="34" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>697</v>
+        <v>717</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>149</v>
@@ -4352,16 +4354,16 @@
     </row>
     <row r="75" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A75" s="31" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B75" s="34" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>717</v>
+        <v>708</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>44</v>
@@ -4372,19 +4374,19 @@
     </row>
     <row r="76" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A76" s="31" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>408</v>
+        <v>712</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>188</v>
@@ -4392,16 +4394,16 @@
     </row>
     <row r="77" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="31" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>149</v>
@@ -4412,32 +4414,32 @@
     </row>
     <row r="78" spans="1:6" ht="19" x14ac:dyDescent="0.15">
       <c r="A78" s="31" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B78" s="33" t="s">
-        <v>412</v>
-      </c>
-      <c r="C78" s="39" t="s">
-        <v>413</v>
-      </c>
-      <c r="D78" s="40"/>
-      <c r="E78" s="41"/>
+        <v>409</v>
+      </c>
+      <c r="C78" s="40" t="s">
+        <v>410</v>
+      </c>
+      <c r="D78" s="41"/>
+      <c r="E78" s="42"/>
       <c r="F78" s="6" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A79" s="31" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="B79" s="34" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>44</v>
@@ -4448,19 +4450,19 @@
     </row>
     <row r="80" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A80" s="31" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="B80" s="34" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>47</v>
@@ -4468,19 +4470,19 @@
     </row>
     <row r="81" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A81" s="31" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B81" s="34" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="F81" s="14">
         <v>1</v>
@@ -4488,16 +4490,16 @@
     </row>
     <row r="82" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A82" s="31" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B82" s="34" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>149</v>
@@ -4508,19 +4510,19 @@
     </row>
     <row r="83" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="31" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="B83" s="34" t="s">
+        <v>423</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="D83" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="E83" s="11" t="s">
         <v>426</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>427</v>
-      </c>
-      <c r="D83" s="25" t="s">
-        <v>428</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>429</v>
       </c>
       <c r="F83" s="14">
         <v>1</v>
@@ -4528,16 +4530,16 @@
     </row>
     <row r="84" spans="1:6" ht="52" x14ac:dyDescent="0.15">
       <c r="A84" s="31" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="B84" s="34" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>718</v>
+        <v>709</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>44</v>
@@ -4548,32 +4550,32 @@
     </row>
     <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="31" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="B85" s="33" t="s">
-        <v>431</v>
-      </c>
-      <c r="C85" s="39" t="s">
-        <v>659</v>
-      </c>
-      <c r="D85" s="40"/>
-      <c r="E85" s="41"/>
+        <v>428</v>
+      </c>
+      <c r="C85" s="40" t="s">
+        <v>711</v>
+      </c>
+      <c r="D85" s="41"/>
+      <c r="E85" s="42"/>
       <c r="F85" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="65" x14ac:dyDescent="0.15">
       <c r="A86" s="31" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>44</v>
@@ -4584,16 +4586,16 @@
     </row>
     <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="31" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B87" s="34" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>149</v>
@@ -4604,19 +4606,19 @@
     </row>
     <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A88" s="31" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="B88" s="35" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>47</v>
@@ -4624,16 +4626,16 @@
     </row>
     <row r="89" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A89" s="31" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B89" s="35" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>149</v>
@@ -4644,19 +4646,19 @@
     </row>
     <row r="90" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A90" s="31" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="B90" s="35" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>445</v>
+        <v>719</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>47</v>
@@ -4664,16 +4666,16 @@
     </row>
     <row r="91" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="31" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="B91" s="34" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>149</v>
@@ -4684,19 +4686,19 @@
     </row>
     <row r="92" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A92" s="31" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="B92" s="34" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>445</v>
+        <v>719</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>47</v>
@@ -4704,16 +4706,16 @@
     </row>
     <row r="93" spans="1:6" ht="104" x14ac:dyDescent="0.15">
       <c r="A93" s="31" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="B93" s="36" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>454</v>
+        <v>718</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>149</v>
@@ -4724,19 +4726,19 @@
     </row>
     <row r="94" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="31" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B94" s="34" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>47</v>
@@ -4744,16 +4746,16 @@
     </row>
     <row r="95" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="31" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="B95" s="34" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>44</v>
@@ -4764,19 +4766,19 @@
     </row>
     <row r="96" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A96" s="31" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="B96" s="34" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>47</v>
@@ -4784,16 +4786,16 @@
     </row>
     <row r="97" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A97" s="31" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="B97" s="34" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>149</v>
@@ -4850,31 +4852,31 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
-        <v>564</v>
-      </c>
-      <c r="B1" s="46" t="s">
+        <v>559</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
-        <v>565</v>
-      </c>
-      <c r="B2" s="47" t="s">
+        <v>560</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>7</v>
@@ -4892,24 +4894,24 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>567</v>
-      </c>
-      <c r="B4" s="43" t="s">
+        <v>562</v>
+      </c>
+      <c r="B4" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
     </row>
     <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="31" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>95</v>
@@ -4920,13 +4922,13 @@
     </row>
     <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>105</v>
@@ -4937,7 +4939,7 @@
     </row>
     <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>108</v>
@@ -4954,13 +4956,13 @@
     </row>
     <row r="8" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>115</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>131</v>
@@ -4971,7 +4973,7 @@
     </row>
     <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>134</v>
@@ -4988,7 +4990,7 @@
     </row>
     <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>138</v>
@@ -5005,7 +5007,7 @@
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>141</v>
@@ -5022,7 +5024,7 @@
     </row>
     <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="31" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>143</v>
@@ -5039,7 +5041,7 @@
     </row>
     <row r="13" spans="1:6" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="31" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>146</v>
@@ -5056,7 +5058,7 @@
     </row>
     <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="31" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>152</v>
@@ -5073,13 +5075,13 @@
     </row>
     <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="31" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>155</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>156</v>
@@ -5090,13 +5092,13 @@
     </row>
     <row r="16" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="31" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>157</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>156</v>
@@ -5107,13 +5109,13 @@
     </row>
     <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="31" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>158</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>156</v>
@@ -5124,7 +5126,7 @@
     </row>
     <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A18" s="31" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>159</v>
@@ -5141,13 +5143,13 @@
     </row>
     <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="31" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>162</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>163</v>
@@ -5158,7 +5160,7 @@
     </row>
     <row r="20" spans="1:5" ht="65" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>164</v>
@@ -5175,7 +5177,7 @@
     </row>
     <row r="21" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>171</v>
@@ -5192,7 +5194,7 @@
     </row>
     <row r="22" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A22" s="31" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>177</v>
@@ -5209,7 +5211,7 @@
     </row>
     <row r="23" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A23" s="31" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>181</v>
@@ -5226,18 +5228,18 @@
     </row>
     <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="31" t="s">
-        <v>587</v>
-      </c>
-      <c r="B24" s="43" t="s">
+        <v>582</v>
+      </c>
+      <c r="B24" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="46"/>
     </row>
     <row r="25" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A25" s="31" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>191</v>
@@ -5254,13 +5256,13 @@
     </row>
     <row r="26" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="31" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>195</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>196</v>
@@ -5271,13 +5273,13 @@
     </row>
     <row r="27" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="31" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>197</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>198</v>
@@ -5288,13 +5290,13 @@
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="31" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>199</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>201</v>
@@ -5305,13 +5307,13 @@
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="31" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="B29" s="30" t="s">
         <v>202</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>204</v>
@@ -5322,7 +5324,7 @@
     </row>
     <row r="30" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A30" s="31" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>205</v>
@@ -5339,7 +5341,7 @@
     </row>
     <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A31" s="31" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>215</v>
@@ -5356,7 +5358,7 @@
     </row>
     <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="31" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="B32" s="30" t="s">
         <v>220</v>
@@ -5371,7 +5373,7 @@
     </row>
     <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A33" s="31" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="B33" s="30" t="s">
         <v>224</v>
@@ -5388,7 +5390,7 @@
     </row>
     <row r="34" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A34" s="31" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="B34" s="30" t="s">
         <v>228</v>
@@ -5405,7 +5407,7 @@
     </row>
     <row r="35" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="31" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="B35" s="30" t="s">
         <v>232</v>
@@ -5422,7 +5424,7 @@
     </row>
     <row r="36" spans="1:5" ht="52" x14ac:dyDescent="0.15">
       <c r="A36" s="31" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="B36" s="30" t="s">
         <v>235</v>
@@ -5439,13 +5441,13 @@
     </row>
     <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="31" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="B37" s="30" t="s">
         <v>238</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>239</v>
@@ -5456,7 +5458,7 @@
     </row>
     <row r="38" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="31" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="B38" s="30" t="s">
         <v>240</v>
@@ -5473,18 +5475,18 @@
     </row>
     <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="31" t="s">
-        <v>602</v>
-      </c>
-      <c r="B39" s="43" t="s">
+        <v>597</v>
+      </c>
+      <c r="B39" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="46"/>
     </row>
     <row r="40" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="31" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="B40" s="30" t="s">
         <v>243</v>
@@ -5501,7 +5503,7 @@
     </row>
     <row r="41" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" s="31" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="B41" s="30" t="s">
         <v>247</v>
@@ -5518,7 +5520,7 @@
     </row>
     <row r="42" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A42" s="31" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B42" s="30" t="s">
         <v>251</v>
@@ -5535,7 +5537,7 @@
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" s="31" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="B43" s="30" t="s">
         <v>258</v>
@@ -5552,7 +5554,7 @@
     </row>
     <row r="44" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A44" s="31" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>260</v>
@@ -5569,7 +5571,7 @@
     </row>
     <row r="45" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" s="31" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="B45" s="30" t="s">
         <v>262</v>
@@ -5586,7 +5588,7 @@
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="31" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="B46" s="30" t="s">
         <v>267</v>
@@ -5603,7 +5605,7 @@
     </row>
     <row r="47" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A47" s="31" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="B47" s="30" t="s">
         <v>270</v>
@@ -5620,7 +5622,7 @@
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A48" s="31" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="B48" s="30" t="s">
         <v>275</v>
@@ -5637,7 +5639,7 @@
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.15">
       <c r="A49" s="31" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="B49" s="30" t="s">
         <v>278</v>
@@ -5688,25 +5690,25 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
-        <v>469</v>
-      </c>
-      <c r="B1" s="48" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
-        <v>613</v>
-      </c>
-      <c r="B2" s="47" t="s">
+        <v>608</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5732,7 +5734,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="31" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>12</v>
@@ -5771,7 +5773,7 @@
     </row>
     <row r="4" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>15</v>
@@ -5788,7 +5790,7 @@
     </row>
     <row r="5" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A5" s="31" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>23</v>
@@ -5805,7 +5807,7 @@
     </row>
     <row r="6" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>27</v>
@@ -5822,7 +5824,7 @@
     </row>
     <row r="7" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A7" s="31" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>30</v>
@@ -5839,7 +5841,7 @@
     </row>
     <row r="8" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="31" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>33</v>
@@ -5856,7 +5858,7 @@
     </row>
     <row r="9" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A9" s="31" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>37</v>
@@ -5873,7 +5875,7 @@
     </row>
     <row r="10" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A10" s="31" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>41</v>
@@ -5890,7 +5892,7 @@
     </row>
     <row r="11" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="31" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>48</v>
@@ -5907,7 +5909,7 @@
     </row>
     <row r="12" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="31" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="B12" s="30" t="s">
         <v>52</v>
@@ -5924,7 +5926,7 @@
     </row>
     <row r="13" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="31" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>56</v>
@@ -5941,7 +5943,7 @@
     </row>
     <row r="14" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A14" s="31" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>60</v>
@@ -5958,7 +5960,7 @@
     </row>
     <row r="15" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A15" s="31" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>64</v>
@@ -5975,7 +5977,7 @@
     </row>
     <row r="16" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="31" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>69</v>
@@ -5992,7 +5994,7 @@
     </row>
     <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="31" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>73</v>
@@ -6009,7 +6011,7 @@
     </row>
     <row r="18" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A18" s="31" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>78</v>
@@ -6026,7 +6028,7 @@
     </row>
     <row r="19" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A19" s="31" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>82</v>
@@ -6043,7 +6045,7 @@
     </row>
     <row r="20" spans="1:5" ht="112" x14ac:dyDescent="0.15">
       <c r="A20" s="31" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>86</v>
@@ -6060,7 +6062,7 @@
     </row>
     <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>90</v>
@@ -6077,7 +6079,7 @@
     </row>
     <row r="22" spans="1:5" ht="84" x14ac:dyDescent="0.15">
       <c r="A22" s="31" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>94</v>
@@ -6094,7 +6096,7 @@
     </row>
     <row r="23" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="31" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>100</v>
@@ -6111,7 +6113,7 @@
     </row>
     <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="31" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>106</v>
@@ -6128,7 +6130,7 @@
     </row>
     <row r="25" spans="1:5" ht="56" x14ac:dyDescent="0.15">
       <c r="A25" s="31" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>113</v>
@@ -6145,7 +6147,7 @@
     </row>
     <row r="26" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A26" s="31" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>118</v>
@@ -6162,7 +6164,7 @@
     </row>
     <row r="27" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="31" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>122</v>
@@ -6179,7 +6181,7 @@
     </row>
     <row r="28" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="31" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Add clarifications for sub-plant observations
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -2127,9 +2127,6 @@
     <t>URL or File name (of gis or tabular file like csv or tsv)</t>
   </si>
   <si>
-    <t>An observed variable describes how a measurement has been made. It typically takes the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement.</t>
-  </si>
-  <si>
     <t>Formatted text (Key:value)</t>
   </si>
   <si>
@@ -2152,12 +2149,6 @@
     <t>Term from Plant Trait Ontology, Crop Ontology, or XML Environment Ontology</t>
   </si>
   <si>
-    <t>Type of observation unit in textual form, usually one of the following: block, sub-block, plot, plant, trial, pot, replication or replicate, individual, virtual_trial, unit-parcel</t>
-  </si>
-  <si>
-    <t>A sample is a portion of plant tissue extracted from an observation unit for the purpose of sub-plant observations and/or molecular studies. A sample must be used when there is a physical sample that needs to be stored and traced. Otherwise, you can use directly variables on the Observation unit (Berry sugar content, Fruit weight, Grain Protein content)</t>
-  </si>
-  <si>
     <t>Experimental Factors</t>
   </si>
   <si>
@@ -2177,9 +2168,6 @@
   </si>
   <si>
     <t>Event accession number</t>
-  </si>
-  <si>
-    <t>Observation units are objects that are subject to particular instances of observation and measurement. An observation unit comprises one or more plants, and their environment. Synonym : Experimental unit.</t>
   </si>
   <si>
     <t>Identifier for the observation unit in a persistent repository, comprises the name of the repository and the identifier of the observation unit therein. The EBI Biosamples repository can be used. URI are recommended when possible.</t>
@@ -2217,6 +2205,21 @@
   </si>
   <si>
     <t>Medium composition</t>
+  </si>
+  <si>
+    <t>Observation units are objects that are subject to particular instances of observation and measurement. An observation unit comprises one or more plants, and/or their environment. There can be pure environment observation units with no plants. 
+Synonym: Experimental unit.</t>
+  </si>
+  <si>
+    <t>A sample is a portion of plant tissue harvested, non-harvested or extracted from an observation unit for the purpose of sub-plant observations and/or molecular studies. A sample must be used when there is a physical sample that needs to be stored and traced. Otherwise, variables may be used (Berry sugar content, Fruit weight, Grain Protein content, Leaf 1 width, Leaf 2 width, Leaf 2 length) directly on the observation unit for sub-plant level observations.</t>
+  </si>
+  <si>
+    <t>An observed variable describes how a measurement has been made. It typically takes the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement. Multiple variables with the same combination of trait, method and scale can be used in association with different plant parts (leaf 1, leaf 2), when this distinction is necessary for observations referring to different parts of the same observation unit.</t>
+  </si>
+  <si>
+    <t>Type of observation unit in textual form, usually one of the following: block, sub-block, plot, plant, study, pot, replication or replicate, individual, virtual_trial, unit-parcel. Use of other observation unit types is possible but not recommended. 
+The observation unit type cannot be used to indicate sub-plant levels. However, observations can still be made on the sub-plant level, as long as the details are indicated in the associated observed variable (see observed variables).
+Alternatively, it is possible to use samples for more detailed tracing of sub-plant units, attaching the observations to them instead.</t>
   </si>
 </sst>
 </file>
@@ -2442,7 +2445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2523,9 +2526,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2551,20 +2551,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2582,6 +2570,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2904,8 +2913,8 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2919,19 +2928,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="48" t="s">
         <v>451</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2948,26 +2958,26 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="48" t="s">
         <v>452</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
       <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="48" t="s">
         <v>453</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -2984,10 +2994,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="48" t="s">
         <v>454</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>123</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -3004,17 +3014,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="48" t="s">
         <v>455</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>129</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>132</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>143</v>
@@ -3024,10 +3034,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="48" t="s">
         <v>456</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>144</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -3044,10 +3054,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="48" t="s">
         <v>457</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>160</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -3064,10 +3074,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="48" t="s">
         <v>458</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>167</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -3084,10 +3094,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="48" t="s">
         <v>459</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>169</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -3104,10 +3114,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="48" t="s">
         <v>460</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -3124,26 +3134,26 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="48" t="s">
         <v>461</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="6" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="48" t="s">
         <v>462</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>197</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3160,10 +3170,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="48" t="s">
         <v>463</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>204</v>
       </c>
       <c r="C14" s="11" t="s">
@@ -3180,10 +3190,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="48" t="s">
         <v>464</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>207</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -3200,10 +3210,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="48" t="s">
         <v>465</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>215</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -3220,10 +3230,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="48" t="s">
         <v>466</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>221</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -3240,10 +3250,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="48" t="s">
         <v>467</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>245</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -3260,10 +3270,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="48" t="s">
         <v>468</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>254</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -3280,10 +3290,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="48" t="s">
         <v>469</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>264</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -3300,10 +3310,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="48" t="s">
         <v>470</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>274</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -3320,14 +3330,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="48" t="s">
         <v>471</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>279</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>280</v>
@@ -3340,10 +3350,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="48" t="s">
         <v>472</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>282</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -3360,10 +3370,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="48" t="s">
         <v>473</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="33" t="s">
         <v>638</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -3380,14 +3390,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="48" t="s">
         <v>474</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="33" t="s">
         <v>632</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>283</v>
@@ -3400,10 +3410,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="48" t="s">
         <v>475</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="33" t="s">
         <v>449</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -3420,10 +3430,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="48" t="s">
         <v>476</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>288</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -3440,10 +3450,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="48" t="s">
         <v>477</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="33" t="s">
         <v>290</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -3460,10 +3470,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="48" t="s">
         <v>478</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="33" t="s">
         <v>292</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -3480,10 +3490,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="48" t="s">
         <v>479</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="33" t="s">
         <v>296</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -3500,19 +3510,19 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="48" t="s">
         <v>480</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="33" t="s">
         <v>299</v>
       </c>
-      <c r="C31" s="38" t="s">
+      <c r="C31" s="49" t="s">
         <v>300</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="50" t="s">
         <v>658</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="51" t="s">
         <v>690</v>
       </c>
       <c r="F31" s="14" t="s">
@@ -3520,26 +3530,26 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="48" t="s">
         <v>481</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="32" t="s">
         <v>301</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="37" t="s">
         <v>302</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="47"/>
       <c r="F32" s="6" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="48" t="s">
         <v>482</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="33" t="s">
         <v>303</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -3556,10 +3566,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="48" t="s">
         <v>483</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="33" t="s">
         <v>307</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -3576,10 +3586,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="48" t="s">
         <v>484</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="33" t="s">
         <v>311</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -3596,10 +3606,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="48" t="s">
         <v>485</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="33" t="s">
         <v>314</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -3616,10 +3626,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="48" t="s">
         <v>486</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="33" t="s">
         <v>317</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -3635,31 +3645,31 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="31" t="s">
+    <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="48" t="s">
         <v>487</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="37" t="s">
         <v>321</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="42"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="6" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="48" t="s">
         <v>488</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="33" t="s">
         <v>323</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>324</v>
@@ -3672,17 +3682,17 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="48" t="s">
         <v>489</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="33" t="s">
         <v>326</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>327</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>126</v>
@@ -3692,10 +3702,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="48" t="s">
         <v>490</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="33" t="s">
         <v>328</v>
       </c>
       <c r="C41" s="11" t="s">
@@ -3712,26 +3722,26 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="48" t="s">
         <v>491</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="32" t="s">
         <v>331</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="37" t="s">
         <v>332</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="42"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="6" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="48" t="s">
         <v>492</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="33" t="s">
         <v>334</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -3748,10 +3758,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="48" t="s">
         <v>493</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="33" t="s">
         <v>336</v>
       </c>
       <c r="C44" s="11" t="s">
@@ -3768,10 +3778,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="48" t="s">
         <v>494</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B45" s="33" t="s">
         <v>339</v>
       </c>
       <c r="C45" s="11" t="s">
@@ -3788,10 +3798,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="48" t="s">
         <v>495</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="33" t="s">
         <v>342</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3808,10 +3818,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="108" x14ac:dyDescent="0.2">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="48" t="s">
         <v>625</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="33" t="s">
         <v>626</v>
       </c>
       <c r="C47" s="11" t="s">
@@ -3828,10 +3838,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="48" t="s">
         <v>496</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="33" t="s">
         <v>344</v>
       </c>
       <c r="C48" s="11" t="s">
@@ -3848,10 +3858,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="48" t="s">
         <v>497</v>
       </c>
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="33" t="s">
         <v>347</v>
       </c>
       <c r="C49" s="11" t="s">
@@ -3868,10 +3878,10 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="48" t="s">
         <v>498</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="33" t="s">
         <v>349</v>
       </c>
       <c r="C50" s="11" t="s">
@@ -3888,10 +3898,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="48" t="s">
         <v>499</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="33" t="s">
         <v>350</v>
       </c>
       <c r="C51" s="11" t="s">
@@ -3908,14 +3918,14 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="48" t="s">
         <v>500</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="33" t="s">
         <v>352</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D52" s="24" t="s">
         <v>683</v>
@@ -3928,14 +3938,14 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="132" x14ac:dyDescent="0.2">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="48" t="s">
         <v>501</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="33" t="s">
         <v>354</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>668</v>
@@ -3948,10 +3958,10 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="48" t="s">
         <v>502</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="33" t="s">
         <v>355</v>
       </c>
       <c r="C54" s="11" t="s">
@@ -3968,10 +3978,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="48" t="s">
         <v>503</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="33" t="s">
         <v>358</v>
       </c>
       <c r="C55" s="11" t="s">
@@ -3988,10 +3998,10 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="48" t="s">
         <v>504</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="33" t="s">
         <v>360</v>
       </c>
       <c r="C56" s="11" t="s">
@@ -4008,10 +4018,10 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="48" t="s">
         <v>505</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="33" t="s">
         <v>362</v>
       </c>
       <c r="C57" s="11" t="s">
@@ -4028,10 +4038,10 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="48" t="s">
         <v>506</v>
       </c>
-      <c r="B58" s="34" t="s">
+      <c r="B58" s="33" t="s">
         <v>363</v>
       </c>
       <c r="C58" s="11" t="s">
@@ -4048,10 +4058,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="48" t="s">
         <v>507</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="33" t="s">
         <v>364</v>
       </c>
       <c r="C59" s="11" t="s">
@@ -4068,33 +4078,33 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="48" t="s">
         <v>508</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="40" t="s">
-        <v>716</v>
-      </c>
-      <c r="D60" s="41"/>
-      <c r="E60" s="42"/>
+      <c r="C60" s="37" t="s">
+        <v>712</v>
+      </c>
+      <c r="D60" s="46"/>
+      <c r="E60" s="47"/>
       <c r="F60" s="6" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="48" t="s">
         <v>509</v>
       </c>
-      <c r="B61" s="34" t="s">
+      <c r="B61" s="33" t="s">
         <v>367</v>
       </c>
       <c r="C61" s="11" t="s">
         <v>651</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>368</v>
@@ -4104,10 +4114,10 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="48" t="s">
         <v>510</v>
       </c>
-      <c r="B62" s="34" t="s">
+      <c r="B62" s="33" t="s">
         <v>369</v>
       </c>
       <c r="C62" s="11" t="s">
@@ -4124,26 +4134,26 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="31" t="s">
+      <c r="A63" s="48" t="s">
         <v>511</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="32" t="s">
         <v>633</v>
       </c>
-      <c r="C63" s="40" t="s">
-        <v>717</v>
-      </c>
-      <c r="D63" s="41"/>
-      <c r="E63" s="42"/>
+      <c r="C63" s="37" t="s">
+        <v>713</v>
+      </c>
+      <c r="D63" s="46"/>
+      <c r="E63" s="47"/>
       <c r="F63" s="6" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="48" t="s">
         <v>512</v>
       </c>
-      <c r="B64" s="34" t="s">
+      <c r="B64" s="33" t="s">
         <v>634</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -4160,17 +4170,17 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A65" s="31" t="s">
+      <c r="A65" s="48" t="s">
         <v>513</v>
       </c>
-      <c r="B65" s="34" t="s">
+      <c r="B65" s="33" t="s">
         <v>635</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>143</v>
@@ -4180,10 +4190,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="48" t="s">
         <v>514</v>
       </c>
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="33" t="s">
         <v>636</v>
       </c>
       <c r="C66" s="11" t="s">
@@ -4200,26 +4210,26 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="48" t="s">
         <v>515</v>
       </c>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="32" t="s">
         <v>377</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="C67" s="37" t="s">
         <v>378</v>
       </c>
-      <c r="D67" s="41"/>
-      <c r="E67" s="42"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="47"/>
       <c r="F67" s="6" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A68" s="31" t="s">
+      <c r="A68" s="48" t="s">
         <v>516</v>
       </c>
-      <c r="B68" s="34" t="s">
+      <c r="B68" s="33" t="s">
         <v>380</v>
       </c>
       <c r="C68" s="11" t="s">
@@ -4236,11 +4246,11 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A69" s="31" t="s">
+      <c r="A69" s="48" t="s">
         <v>517</v>
       </c>
-      <c r="B69" s="34" t="s">
-        <v>706</v>
+      <c r="B69" s="33" t="s">
+        <v>703</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>669</v>
@@ -4256,10 +4266,10 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="48" t="s">
         <v>518</v>
       </c>
-      <c r="B70" s="34" t="s">
+      <c r="B70" s="33" t="s">
         <v>383</v>
       </c>
       <c r="C70" s="11" t="s">
@@ -4276,17 +4286,17 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A71" s="31" t="s">
+      <c r="A71" s="48" t="s">
         <v>519</v>
       </c>
-      <c r="B71" s="34" t="s">
+      <c r="B71" s="33" t="s">
         <v>385</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>386</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>159</v>
@@ -4295,27 +4305,27 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A72" s="31" t="s">
+    <row r="72" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="48" t="s">
         <v>520</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="32" t="s">
         <v>387</v>
       </c>
-      <c r="C72" s="40" t="s">
-        <v>707</v>
-      </c>
-      <c r="D72" s="41"/>
-      <c r="E72" s="42"/>
+      <c r="C72" s="37" t="s">
+        <v>716</v>
+      </c>
+      <c r="D72" s="46"/>
+      <c r="E72" s="47"/>
       <c r="F72" s="6" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A73" s="31" t="s">
+      <c r="A73" s="48" t="s">
         <v>521</v>
       </c>
-      <c r="B73" s="34" t="s">
+      <c r="B73" s="33" t="s">
         <v>389</v>
       </c>
       <c r="C73" s="11" t="s">
@@ -4331,15 +4341,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A74" s="31" t="s">
+    <row r="74" spans="1:6" ht="132" x14ac:dyDescent="0.2">
+      <c r="A74" s="48" t="s">
         <v>522</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="33" t="s">
         <v>391</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>698</v>
+        <v>719</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>672</v>
@@ -4352,14 +4362,14 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="48" t="s">
         <v>523</v>
       </c>
-      <c r="B75" s="34" t="s">
+      <c r="B75" s="33" t="s">
         <v>392</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="D75" s="11" t="s">
         <v>414</v>
@@ -4372,10 +4382,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="48" t="s">
         <v>524</v>
       </c>
-      <c r="B76" s="34" t="s">
+      <c r="B76" s="33" t="s">
         <v>393</v>
       </c>
       <c r="C76" s="11" t="s">
@@ -4385,17 +4395,17 @@
         <v>687</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="31" t="s">
+      <c r="A77" s="48" t="s">
         <v>525</v>
       </c>
-      <c r="B77" s="34" t="s">
+      <c r="B77" s="33" t="s">
         <v>394</v>
       </c>
       <c r="C77" s="11" t="s">
@@ -4412,26 +4422,26 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="31" t="s">
+      <c r="A78" s="48" t="s">
         <v>526</v>
       </c>
-      <c r="B78" s="33" t="s">
+      <c r="B78" s="32" t="s">
         <v>397</v>
       </c>
-      <c r="C78" s="40" t="s">
-        <v>699</v>
-      </c>
-      <c r="D78" s="41"/>
-      <c r="E78" s="42"/>
+      <c r="C78" s="37" t="s">
+        <v>717</v>
+      </c>
+      <c r="D78" s="46"/>
+      <c r="E78" s="47"/>
       <c r="F78" s="6" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="31" t="s">
+      <c r="A79" s="48" t="s">
         <v>527</v>
       </c>
-      <c r="B79" s="34" t="s">
+      <c r="B79" s="33" t="s">
         <v>399</v>
       </c>
       <c r="C79" s="11" t="s">
@@ -4448,10 +4458,10 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A80" s="31" t="s">
+      <c r="A80" s="48" t="s">
         <v>528</v>
       </c>
-      <c r="B80" s="34" t="s">
+      <c r="B80" s="33" t="s">
         <v>402</v>
       </c>
       <c r="C80" s="11" t="s">
@@ -4468,10 +4478,10 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A81" s="31" t="s">
+      <c r="A81" s="48" t="s">
         <v>529</v>
       </c>
-      <c r="B81" s="34" t="s">
+      <c r="B81" s="33" t="s">
         <v>405</v>
       </c>
       <c r="C81" s="11" t="s">
@@ -4488,10 +4498,10 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="48" t="s">
         <v>530</v>
       </c>
-      <c r="B82" s="34" t="s">
+      <c r="B82" s="33" t="s">
         <v>408</v>
       </c>
       <c r="C82" s="11" t="s">
@@ -4508,10 +4518,10 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="31" t="s">
+      <c r="A83" s="48" t="s">
         <v>531</v>
       </c>
-      <c r="B83" s="34" t="s">
+      <c r="B83" s="33" t="s">
         <v>410</v>
       </c>
       <c r="C83" s="11" t="s">
@@ -4528,14 +4538,14 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="60" x14ac:dyDescent="0.2">
-      <c r="A84" s="31" t="s">
+      <c r="A84" s="48" t="s">
         <v>532</v>
       </c>
-      <c r="B84" s="34" t="s">
+      <c r="B84" s="33" t="s">
         <v>392</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D84" s="11" t="s">
         <v>414</v>
@@ -4547,27 +4557,27 @@
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="31" t="s">
+    <row r="85" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="48" t="s">
         <v>533</v>
       </c>
-      <c r="B85" s="33" t="s">
+      <c r="B85" s="32" t="s">
         <v>415</v>
       </c>
-      <c r="C85" s="40" t="s">
-        <v>691</v>
-      </c>
-      <c r="D85" s="41"/>
-      <c r="E85" s="42"/>
+      <c r="C85" s="37" t="s">
+        <v>718</v>
+      </c>
+      <c r="D85" s="46"/>
+      <c r="E85" s="47"/>
       <c r="F85" s="6" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.2">
-      <c r="A86" s="31" t="s">
+      <c r="A86" s="48" t="s">
         <v>534</v>
       </c>
-      <c r="B86" s="35" t="s">
+      <c r="B86" s="34" t="s">
         <v>416</v>
       </c>
       <c r="C86" s="11" t="s">
@@ -4584,10 +4594,10 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="31" t="s">
+      <c r="A87" s="48" t="s">
         <v>535</v>
       </c>
-      <c r="B87" s="34" t="s">
+      <c r="B87" s="33" t="s">
         <v>419</v>
       </c>
       <c r="C87" s="11" t="s">
@@ -4604,10 +4614,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="31" t="s">
+      <c r="A88" s="48" t="s">
         <v>536</v>
       </c>
-      <c r="B88" s="35" t="s">
+      <c r="B88" s="34" t="s">
         <v>422</v>
       </c>
       <c r="C88" s="11" t="s">
@@ -4624,10 +4634,10 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A89" s="31" t="s">
+      <c r="A89" s="48" t="s">
         <v>537</v>
       </c>
-      <c r="B89" s="35" t="s">
+      <c r="B89" s="34" t="s">
         <v>425</v>
       </c>
       <c r="C89" s="11" t="s">
@@ -4644,10 +4654,10 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A90" s="31" t="s">
+      <c r="A90" s="48" t="s">
         <v>538</v>
       </c>
-      <c r="B90" s="35" t="s">
+      <c r="B90" s="34" t="s">
         <v>427</v>
       </c>
       <c r="C90" s="11" t="s">
@@ -4657,17 +4667,17 @@
         <v>677</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="31" t="s">
+      <c r="A91" s="48" t="s">
         <v>539</v>
       </c>
-      <c r="B91" s="34" t="s">
+      <c r="B91" s="33" t="s">
         <v>429</v>
       </c>
       <c r="C91" s="11" t="s">
@@ -4684,10 +4694,10 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A92" s="31" t="s">
+      <c r="A92" s="48" t="s">
         <v>540</v>
       </c>
-      <c r="B92" s="34" t="s">
+      <c r="B92" s="33" t="s">
         <v>432</v>
       </c>
       <c r="C92" s="11" t="s">
@@ -4697,24 +4707,24 @@
         <v>434</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="108" x14ac:dyDescent="0.2">
-      <c r="A93" s="31" t="s">
+      <c r="A93" s="48" t="s">
         <v>541</v>
       </c>
-      <c r="B93" s="36" t="s">
+      <c r="B93" s="35" t="s">
         <v>435</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>436</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>143</v>
@@ -4724,10 +4734,10 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="31" t="s">
+      <c r="A94" s="48" t="s">
         <v>542</v>
       </c>
-      <c r="B94" s="34" t="s">
+      <c r="B94" s="33" t="s">
         <v>437</v>
       </c>
       <c r="C94" s="11" t="s">
@@ -4744,10 +4754,10 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="31" t="s">
+      <c r="A95" s="48" t="s">
         <v>543</v>
       </c>
-      <c r="B95" s="34" t="s">
+      <c r="B95" s="33" t="s">
         <v>441</v>
       </c>
       <c r="C95" s="11" t="s">
@@ -4764,10 +4774,10 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A96" s="31" t="s">
+      <c r="A96" s="48" t="s">
         <v>544</v>
       </c>
-      <c r="B96" s="34" t="s">
+      <c r="B96" s="33" t="s">
         <v>444</v>
       </c>
       <c r="C96" s="11" t="s">
@@ -4784,10 +4794,10 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A97" s="31" t="s">
+      <c r="A97" s="48" t="s">
         <v>545</v>
       </c>
-      <c r="B97" s="34" t="s">
+      <c r="B97" s="33" t="s">
         <v>447</v>
       </c>
       <c r="C97" s="11" t="s">
@@ -4850,34 +4860,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>546</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>547</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>702</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
+      <c r="B2" s="43" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>548</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -4892,21 +4902,21 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>549</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>550</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -4920,10 +4930,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>551</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>97</v>
       </c>
       <c r="C6" s="11" t="s">
@@ -4937,10 +4947,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>552</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>104</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4954,13 +4964,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>553</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="36" t="s">
         <v>641</v>
       </c>
       <c r="D8" s="11" t="s">
@@ -4971,10 +4981,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>554</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>130</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -4988,10 +4998,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>555</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>133</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -5005,10 +5015,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>556</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>136</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -5022,27 +5032,27 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>557</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>138</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>558</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>140</v>
       </c>
       <c r="C13" s="8" t="s">
@@ -5056,10 +5066,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>559</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>146</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -5073,10 +5083,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>560</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>149</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -5090,10 +5100,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>561</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>151</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -5107,10 +5117,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>562</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>152</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -5124,10 +5134,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>563</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>153</v>
       </c>
       <c r="C18" s="8" t="s">
@@ -5141,10 +5151,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>564</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>156</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -5158,7 +5168,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>565</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -5175,10 +5185,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>566</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>165</v>
       </c>
       <c r="C21" s="8" t="s">
@@ -5192,10 +5202,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>567</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>171</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -5209,10 +5219,10 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>568</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>175</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -5226,21 +5236,21 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="30" t="s">
         <v>569</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
     </row>
     <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>570</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>185</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5254,10 +5264,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>571</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>189</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -5271,10 +5281,10 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>572</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>191</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -5288,10 +5298,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="30" t="s">
         <v>573</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="29" t="s">
         <v>193</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -5305,10 +5315,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>574</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="29" t="s">
         <v>196</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -5322,10 +5332,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="36" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>575</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="29" t="s">
         <v>199</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -5339,10 +5349,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>576</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="29" t="s">
         <v>209</v>
       </c>
       <c r="C31" s="8" t="s">
@@ -5356,10 +5366,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>577</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="29" t="s">
         <v>214</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -5371,10 +5381,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="30" t="s">
         <v>578</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="29" t="s">
         <v>218</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -5388,10 +5398,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>579</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="29" t="s">
         <v>222</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -5405,10 +5415,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>580</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="29" t="s">
         <v>226</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -5422,10 +5432,10 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>581</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="29" t="s">
         <v>229</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -5439,10 +5449,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>582</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="29" t="s">
         <v>232</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -5456,10 +5466,10 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.2">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>583</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="29" t="s">
         <v>234</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -5473,22 +5483,22 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>584</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
     </row>
     <row r="40" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>585</v>
       </c>
-      <c r="B40" s="30" t="s">
-        <v>719</v>
+      <c r="B40" s="29" t="s">
+        <v>715</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>237</v>
@@ -5501,10 +5511,10 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>586</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="29" t="s">
         <v>240</v>
       </c>
       <c r="C41" s="18" t="s">
@@ -5518,10 +5528,10 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.2">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="30" t="s">
         <v>587</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="29" t="s">
         <v>244</v>
       </c>
       <c r="C42" s="18" t="s">
@@ -5535,10 +5545,10 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>588</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="29" t="s">
         <v>251</v>
       </c>
       <c r="C43" s="18" t="s">
@@ -5552,10 +5562,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>589</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="29" t="s">
         <v>253</v>
       </c>
       <c r="C44" s="18" t="s">
@@ -5569,10 +5579,10 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="30" t="s">
         <v>590</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="29" t="s">
         <v>255</v>
       </c>
       <c r="C45" s="15" t="s">
@@ -5586,10 +5596,10 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>591</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="29" t="s">
         <v>260</v>
       </c>
       <c r="C46" s="18" t="s">
@@ -5603,10 +5613,10 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>592</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="29" t="s">
         <v>263</v>
       </c>
       <c r="C47" s="18" t="s">
@@ -5620,10 +5630,10 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="30" t="s">
         <v>593</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="29" t="s">
         <v>268</v>
       </c>
       <c r="C48" s="15" t="s">
@@ -5637,10 +5647,10 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.2">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="30" t="s">
         <v>594</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="29" t="s">
         <v>271</v>
       </c>
       <c r="C49" s="18" t="s">
@@ -5688,26 +5698,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>451</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="44" t="s">
+        <v>697</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>595</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>700</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
-        <v>595</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>703</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -5732,10 +5742,10 @@
       <c r="AA2" s="4"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>596</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -5771,10 +5781,10 @@
       <c r="AA3" s="4"/>
     </row>
     <row r="4" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>597</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -5788,10 +5798,10 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>598</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -5805,10 +5815,10 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>599</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -5822,10 +5832,10 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>600</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -5839,10 +5849,10 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>601</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -5856,14 +5866,14 @@
       </c>
     </row>
     <row r="9" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>602</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>35</v>
@@ -5873,10 +5883,10 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>603</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -5890,10 +5900,10 @@
       </c>
     </row>
     <row r="11" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>604</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -5907,10 +5917,10 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="30" t="s">
         <v>605</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -5924,10 +5934,10 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="30" t="s">
         <v>606</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -5941,10 +5951,10 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>607</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -5958,10 +5968,10 @@
       </c>
     </row>
     <row r="15" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="30" t="s">
         <v>608</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -5975,10 +5985,10 @@
       </c>
     </row>
     <row r="16" spans="1:27" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="30" t="s">
         <v>609</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>65</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -5992,10 +6002,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="30" t="s">
         <v>610</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -6009,10 +6019,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="30" t="s">
         <v>611</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -6026,10 +6036,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="30" t="s">
         <v>612</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>78</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -6043,10 +6053,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>613</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="29" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -6060,10 +6070,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>614</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -6077,10 +6087,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="30" t="s">
         <v>615</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>90</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -6094,10 +6104,10 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>616</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>96</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -6111,10 +6121,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="30" t="s">
         <v>617</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>102</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -6128,10 +6138,10 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="30" t="s">
         <v>618</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>109</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -6145,10 +6155,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="30" t="s">
         <v>619</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>114</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -6162,10 +6172,10 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>620</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>118</v>
       </c>
       <c r="C27" s="10" t="s">
@@ -6179,10 +6189,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="30" t="s">
         <v>621</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="29" t="s">
         <v>122</v>
       </c>
       <c r="C28" s="12"/>

</xml_diff>

<commit_message>
Remove virtual_trial, unit parcel from list of recommended observation unit types
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\M12\MIAPPE_Checklist-Data-Model-v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE_v1.1.2\MIAPPE_Checklist-Data-Model-v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{735E197D-C37C-40B0-805D-C93F46F80785}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC36176B-8F09-49C7-A2C4-8AC70398D3FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="28800" windowHeight="17532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIAPPE_Checklist-Data-Model-v1." sheetId="1" r:id="rId1"/>
@@ -2211,16 +2211,16 @@
     <t>An observed variable describes how a measurement has been made. It typically takes the form of a measured characteristic of the observation unit (plant or environmental trait), associated to the method and unit of measurement. Multiple variables with the same combination of trait, method and scale can be used in association with different plant parts (leaf 1, leaf 2), when this distinction is necessary for observations referring to different parts of the same observation unit.</t>
   </si>
   <si>
-    <t>Type of observation unit in textual form, usually one of the following: block, sub-block, plot, plant, study, pot, replication or replicate, individual, virtual_trial, unit-parcel. Use of other observation unit types is possible but not recommended. 
+    <t>A sample is a portion of plant tissue harvested, non-harvested or extracted from an observation unit for the purpose of sub-plant observations and/or molecular studies. A sample must be used when there is a physical sample that needs to be stored and traced. Otherwise, observations made at the sub-plant level should be recorded as plant level observations using the observed variables to characterize the object of the observation (e.g. Berry sugar content, Fruit weight, Grain Protein content, Leaf 1 width, Leaf 2 width, Leaf 2 length).</t>
+  </si>
+  <si>
+    <t>Observation units are objects that are subject to instances of observation and measurement. An observation unit comprises one or more plants, and/or their environment. There can be pure environment observation units with no plants. 
+Synonym: Experimental unit.</t>
+  </si>
+  <si>
+    <t>Type of observation unit in textual form, usually one of the following: block, sub-block, plot, plant, study, pot, replication or replicate, individual. Use of other observation unit types is possible but not recommended. 
 The observation unit type cannot be used to indicate sub-plant levels. However, observations can still be made on the sub-plant level, as long as the details are indicated in the associated observed variable (see observed variables).
 Alternatively, it is possible to use samples for more detailed tracing of sub-plant units, attaching the observations to them instead.</t>
-  </si>
-  <si>
-    <t>A sample is a portion of plant tissue harvested, non-harvested or extracted from an observation unit for the purpose of sub-plant observations and/or molecular studies. A sample must be used when there is a physical sample that needs to be stored and traced. Otherwise, observations made at the sub-plant level should be recorded as plant level observations using the observed variables to characterize the object of the observation (e.g. Berry sugar content, Fruit weight, Grain Protein content, Leaf 1 width, Leaf 2 width, Leaf 2 length).</t>
-  </si>
-  <si>
-    <t>Observation units are objects that are subject to instances of observation and measurement. An observation unit comprises one or more plants, and/or their environment. There can be pure environment observation units with no plants. 
-Synonym: Experimental unit.</t>
   </si>
 </sst>
 </file>
@@ -2915,20 +2915,20 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1"/>
-    <col min="3" max="3" width="51.88671875" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="37"/>
       <c r="B1" s="45" t="s">
         <v>0</v>
@@ -2938,7 +2938,7 @@
       <c r="E1" s="43"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>451</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>452</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>453</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
         <v>454</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="79.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
         <v>455</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
         <v>456</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>457</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
         <v>458</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="38" t="s">
         <v>459</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>460</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>461</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>462</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>463</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>464</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>465</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
         <v>466</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>467</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>468</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>469</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>470</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>471</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
         <v>472</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="38" t="s">
         <v>473</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
         <v>474</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
         <v>475</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
         <v>476</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
         <v>477</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
         <v>478</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
         <v>479</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
         <v>480</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="s">
         <v>481</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="38" t="s">
         <v>482</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
         <v>483</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
         <v>484</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
         <v>485</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
         <v>486</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
         <v>487</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
         <v>488</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A40" s="38" t="s">
         <v>489</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="38" t="s">
         <v>490</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="38" t="s">
         <v>491</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A43" s="38" t="s">
         <v>492</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="38" t="s">
         <v>493</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="38" t="s">
         <v>494</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A46" s="38" t="s">
         <v>495</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="91.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="108" x14ac:dyDescent="0.2">
       <c r="A47" s="38" t="s">
         <v>625</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="38" t="s">
         <v>496</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="38" t="s">
         <v>497</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="38" t="s">
         <v>498</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="38" t="s">
         <v>499</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="38" t="s">
         <v>500</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="102.6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="132" x14ac:dyDescent="0.2">
       <c r="A53" s="38" t="s">
         <v>501</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="38" t="s">
         <v>502</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A55" s="38" t="s">
         <v>503</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="38" t="s">
         <v>504</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="38" t="s">
         <v>505</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="38" t="s">
         <v>506</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A59" s="38" t="s">
         <v>507</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="38" t="s">
         <v>508</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A61" s="38" t="s">
         <v>509</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A62" s="38" t="s">
         <v>510</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
         <v>511</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="38" t="s">
         <v>512</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="38" t="s">
         <v>513</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="38" t="s">
         <v>514</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="38" t="s">
         <v>515</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A68" s="38" t="s">
         <v>516</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="38" t="s">
         <v>517</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="38" t="s">
         <v>518</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A71" s="38" t="s">
         <v>519</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="38" t="s">
         <v>520</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>387</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D72" s="43"/>
       <c r="E72" s="44"/>
@@ -4322,7 +4322,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="38" t="s">
         <v>521</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="114" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="132" x14ac:dyDescent="0.2">
       <c r="A74" s="38" t="s">
         <v>522</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>391</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>672</v>
@@ -4362,7 +4362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="38" t="s">
         <v>523</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="38" t="s">
         <v>524</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="38" t="s">
         <v>525</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="45.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="38" t="s">
         <v>526</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>397</v>
       </c>
       <c r="C78" s="42" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D78" s="43"/>
       <c r="E78" s="44"/>
@@ -4438,7 +4438,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="38" t="s">
         <v>527</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A80" s="38" t="s">
         <v>528</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="38" t="s">
         <v>529</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A82" s="38" t="s">
         <v>530</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="38" t="s">
         <v>531</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A84" s="38" t="s">
         <v>532</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="38" t="s">
         <v>533</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.2">
       <c r="A86" s="38" t="s">
         <v>534</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="38" t="s">
         <v>535</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="38" t="s">
         <v>536</v>
       </c>
@@ -4634,7 +4634,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A89" s="38" t="s">
         <v>537</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A90" s="38" t="s">
         <v>538</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="38" t="s">
         <v>539</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A92" s="38" t="s">
         <v>540</v>
       </c>
@@ -4714,7 +4714,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="91.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="108" x14ac:dyDescent="0.2">
       <c r="A93" s="38" t="s">
         <v>541</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="38" t="s">
         <v>542</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="38" t="s">
         <v>543</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A96" s="38" t="s">
         <v>544</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A97" s="38" t="s">
         <v>545</v>
       </c>
@@ -4851,16 +4851,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>546</v>
       </c>
@@ -4872,7 +4872,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>547</v>
       </c>
@@ -4884,7 +4884,7 @@
       <c r="E2" s="48"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>548</v>
       </c>
@@ -4902,7 +4902,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>549</v>
       </c>
@@ -4913,7 +4913,7 @@
       <c r="D4" s="47"/>
       <c r="E4" s="48"/>
     </row>
-    <row r="5" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>550</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>551</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>552</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>553</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>554</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>555</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>556</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
         <v>557</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
         <v>558</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>559</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>560</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
         <v>561</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
         <v>562</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
         <v>563</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>564</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="57" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>565</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>566</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
         <v>567</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
         <v>568</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>569</v>
       </c>
@@ -5247,7 +5247,7 @@
       <c r="D24" s="47"/>
       <c r="E24" s="48"/>
     </row>
-    <row r="25" spans="1:5" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
         <v>570</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>571</v>
       </c>
@@ -5281,7 +5281,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
         <v>572</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
         <v>573</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>574</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>575</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
         <v>576</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>577</v>
       </c>
@@ -5381,7 +5381,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
         <v>578</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="34.200000000000003" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>579</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="30" t="s">
         <v>580</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
         <v>581</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
         <v>582</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
         <v>583</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
         <v>584</v>
       </c>
@@ -5494,7 +5494,7 @@
       <c r="D39" s="47"/>
       <c r="E39" s="48"/>
     </row>
-    <row r="40" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
         <v>585</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="30" t="s">
         <v>586</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="s">
         <v>587</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
         <v>588</v>
       </c>
@@ -5562,7 +5562,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="30" t="s">
         <v>589</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="30" t="s">
         <v>590</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="30" t="s">
         <v>591</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A47" s="30" t="s">
         <v>592</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A48" s="30" t="s">
         <v>593</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A49" s="30" t="s">
         <v>594</v>
       </c>
@@ -5689,16 +5689,16 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>451</v>
       </c>
@@ -5709,7 +5709,7 @@
       <c r="D1" s="47"/>
       <c r="E1" s="48"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
         <v>595</v>
       </c>
@@ -5742,7 +5742,7 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>596</v>
       </c>
@@ -5781,7 +5781,7 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>597</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
         <v>598</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
         <v>599</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>600</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>601</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
         <v>602</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>603</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>604</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
         <v>605</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
         <v>606</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>607</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
         <v>608</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
         <v>609</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
         <v>610</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
         <v>611</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>612</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="118.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>613</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>614</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
         <v>615</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
         <v>616</v>
       </c>
@@ -6121,7 +6121,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>617</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
         <v>618</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
         <v>619</v>
       </c>
@@ -6172,7 +6172,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
         <v>620</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
         <v>621</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
Adjust recommended observation unit types and add replicate to spatial distribution example
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE_v1.1.2\MIAPPE_Checklist-Data-Model-v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AC36176B-8F09-49C7-A2C4-8AC70398D3FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2CC69939-30DE-4FD1-B276-DD8260DAC3F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2116,9 +2116,6 @@
     <t>Type and value of a spatial coordinate (georeference or relative) or level of observation (plot 45, subblock 7, block 2) provided as a key-value pair of the form type:value. Levels of observation must be consistent with those listed in the Study section.</t>
   </si>
   <si>
-    <t>Latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; Block:1; Plot:894</t>
-  </si>
-  <si>
     <t>Code used to identify the biological material in the data file. Should be unique within the Investigation. Can correspond to experimental plant ID, seed lot ID, etc… This material identification is different from a BiosampleID which corresponds to Observation Unit or Samples sections below.</t>
   </si>
   <si>
@@ -2218,9 +2215,12 @@
 Synonym: Experimental unit.</t>
   </si>
   <si>
-    <t>Type of observation unit in textual form, usually one of the following: block, sub-block, plot, plant, study, pot, replication or replicate, individual. Use of other observation unit types is possible but not recommended. 
+    <t>Type of observation unit in textual form, usually one of the following: study, block, sub-block, plot, sub-plot, pot, whole plant. Use of other observation unit types is possible but not recommended. 
 The observation unit type cannot be used to indicate sub-plant levels. However, observations can still be made on the sub-plant level, as long as the details are indicated in the associated observed variable (see observed variables).
 Alternatively, it is possible to use samples for more detailed tracing of sub-plant units, attaching the observations to them instead.</t>
+  </si>
+  <si>
+    <t>latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; block:1; plot:894; replicate:1</t>
   </si>
 </sst>
 </file>
@@ -2914,8 +2914,8 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="B74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3025,7 +3025,7 @@
         <v>132</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>143</v>
@@ -3338,7 +3338,7 @@
         <v>279</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>280</v>
@@ -3398,7 +3398,7 @@
         <v>632</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>283</v>
@@ -3524,7 +3524,7 @@
         <v>658</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>182</v>
@@ -3670,7 +3670,7 @@
         <v>323</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>324</v>
@@ -3693,7 +3693,7 @@
         <v>327</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>126</v>
@@ -3746,7 +3746,7 @@
         <v>334</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>335</v>
@@ -3926,7 +3926,7 @@
         <v>352</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D52" s="24" t="s">
         <v>683</v>
@@ -3946,7 +3946,7 @@
         <v>354</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>668</v>
@@ -4086,7 +4086,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D60" s="43"/>
       <c r="E60" s="44"/>
@@ -4105,7 +4105,7 @@
         <v>651</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>368</v>
@@ -4142,7 +4142,7 @@
         <v>633</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="44"/>
@@ -4178,10 +4178,10 @@
         <v>635</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>143</v>
@@ -4251,7 +4251,7 @@
         <v>517</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>669</v>
@@ -4297,7 +4297,7 @@
         <v>386</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>159</v>
@@ -4314,7 +4314,7 @@
         <v>387</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D72" s="43"/>
       <c r="E72" s="44"/>
@@ -4330,7 +4330,7 @@
         <v>389</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>390</v>
@@ -4350,7 +4350,7 @@
         <v>391</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>672</v>
@@ -4370,7 +4370,7 @@
         <v>392</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D75" s="11" t="s">
         <v>414</v>
@@ -4393,10 +4393,10 @@
         <v>686</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>687</v>
+        <v>719</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>182</v>
@@ -4430,7 +4430,7 @@
         <v>397</v>
       </c>
       <c r="C78" s="42" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D78" s="43"/>
       <c r="E78" s="44"/>
@@ -4546,7 +4546,7 @@
         <v>392</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D84" s="11" t="s">
         <v>414</v>
@@ -4566,7 +4566,7 @@
         <v>415</v>
       </c>
       <c r="C85" s="42" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D85" s="43"/>
       <c r="E85" s="44"/>
@@ -4668,7 +4668,7 @@
         <v>677</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>43</v>
@@ -4708,7 +4708,7 @@
         <v>434</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>43</v>
@@ -4725,7 +4725,7 @@
         <v>436</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>143</v>
@@ -4877,7 +4877,7 @@
         <v>547</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
@@ -5043,7 +5043,7 @@
         <v>139</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>94</v>
@@ -5499,7 +5499,7 @@
         <v>585</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>237</v>
@@ -5703,7 +5703,7 @@
         <v>451</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
@@ -5714,7 +5714,7 @@
         <v>595</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
@@ -5874,7 +5874,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Change whole plant to plant, in recommended observation unit type list
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE_v1.1.2\MIAPPE_Checklist-Data-Model-v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2CC69939-30DE-4FD1-B276-DD8260DAC3F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BDE8F9E9-8813-4A4D-AE79-DE28AB659F59}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2215,12 +2215,12 @@
 Synonym: Experimental unit.</t>
   </si>
   <si>
-    <t>Type of observation unit in textual form, usually one of the following: study, block, sub-block, plot, sub-plot, pot, whole plant. Use of other observation unit types is possible but not recommended. 
+    <t>latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; block:1; plot:894; replicate:1</t>
+  </si>
+  <si>
+    <t>Type of observation unit in textual form, usually one of the following: study, block, sub-block, plot, sub-plot, pot, plant. Use of other observation unit types is possible but not recommended. 
 The observation unit type cannot be used to indicate sub-plant levels. However, observations can still be made on the sub-plant level, as long as the details are indicated in the associated observed variable (see observed variables).
 Alternatively, it is possible to use samples for more detailed tracing of sub-plant units, attaching the observations to them instead.</t>
-  </si>
-  <si>
-    <t>latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; block:1; plot:894; replicate:1</t>
   </si>
 </sst>
 </file>
@@ -2914,8 +2914,8 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B74" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4350,7 +4350,7 @@
         <v>391</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>672</v>
@@ -4393,7 +4393,7 @@
         <v>686</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>690</v>

</xml_diff>

<commit_message>
Remove replicate from Statistical distribution example
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE_v1.1.2\MIAPPE_Checklist-Data-Model-v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE_dev_15aug\MIAPPE_Checklist-Data-Model-v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BDE8F9E9-8813-4A4D-AE79-DE28AB659F59}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{72BDB4C4-B023-4329-A244-A253801245C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2215,12 +2215,12 @@
 Synonym: Experimental unit.</t>
   </si>
   <si>
-    <t>latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; block:1; plot:894; replicate:1</t>
-  </si>
-  <si>
     <t>Type of observation unit in textual form, usually one of the following: study, block, sub-block, plot, sub-plot, pot, plant. Use of other observation unit types is possible but not recommended. 
 The observation unit type cannot be used to indicate sub-plant levels. However, observations can still be made on the sub-plant level, as long as the details are indicated in the associated observed variable (see observed variables).
 Alternatively, it is possible to use samples for more detailed tracing of sub-plant units, attaching the observations to them instead.</t>
+  </si>
+  <si>
+    <t>latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; block:1; plot:894</t>
   </si>
 </sst>
 </file>
@@ -2915,7 +2915,7 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4350,7 +4350,7 @@
         <v>391</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>672</v>
@@ -4393,7 +4393,7 @@
         <v>686</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>690</v>

</xml_diff>

<commit_message>
Change NCBI prefix to NCBITAXON
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE_dev_15aug\MIAPPE_Checklist-Data-Model-v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papou001\git\MIAPPE_1.1.2\MIAPPE_Checklist-Data-Model-v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{72BDB4C4-B023-4329-A244-A253801245C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E492EFDF-5FB9-44A8-A7AD-D0A15D54D11D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,9 +1045,6 @@
     <t xml:space="preserve">An identifier for the organism at the species level. Use of the NCBI taxon ID is recommended. </t>
   </si>
   <si>
-    <t xml:space="preserve">NCBI:4577 </t>
-  </si>
-  <si>
     <t>Genus</t>
   </si>
   <si>
@@ -2221,6 +2218,9 @@
   </si>
   <si>
     <t>latitude:+2.341; row:4 ; X:3; Y:6; Xm:35; Ym:65; block:1; plot:894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCBITAXON:4577 </t>
   </si>
 </sst>
 </file>
@@ -2914,8 +2914,8 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>2</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="3" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>8</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>15</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>123</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="6" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>129</v>
@@ -3025,7 +3025,7 @@
         <v>132</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>143</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="38" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>144</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>160</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>167</v>
@@ -3085,7 +3085,7 @@
         <v>168</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>40</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>169</v>
@@ -3105,10 +3105,10 @@
         <v>170</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>622</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>623</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>624</v>
       </c>
       <c r="F10" s="14">
         <v>1</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B11" s="33" t="s">
         <v>176</v>
@@ -3136,7 +3136,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>183</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="13" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>197</v>
@@ -3161,7 +3161,7 @@
         <v>200</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>40</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B14" s="33" t="s">
         <v>204</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>207</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B16" s="33" t="s">
         <v>215</v>
@@ -3221,7 +3221,7 @@
         <v>217</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>159</v>
@@ -3232,7 +3232,7 @@
     </row>
     <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B17" s="33" t="s">
         <v>221</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B18" s="33" t="s">
         <v>245</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B19" s="33" t="s">
         <v>254</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="20" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B20" s="33" t="s">
         <v>264</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B21" s="33" t="s">
         <v>274</v>
@@ -3332,13 +3332,13 @@
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B22" s="33" t="s">
         <v>279</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>280</v>
@@ -3352,19 +3352,19 @@
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B23" s="33" t="s">
         <v>282</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>627</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>656</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>628</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>43</v>
@@ -3372,16 +3372,16 @@
     </row>
     <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A24" s="38" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>143</v>
@@ -3392,13 +3392,13 @@
     </row>
     <row r="25" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>283</v>
@@ -3412,10 +3412,10 @@
     </row>
     <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>285</v>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B27" s="33" t="s">
         <v>288</v>
@@ -3441,7 +3441,7 @@
         <v>289</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>143</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="28" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B28" s="33" t="s">
         <v>290</v>
@@ -3461,7 +3461,7 @@
         <v>291</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>126</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B29" s="33" t="s">
         <v>292</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B30" s="33" t="s">
         <v>296</v>
@@ -3512,7 +3512,7 @@
     </row>
     <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B31" s="33" t="s">
         <v>299</v>
@@ -3521,10 +3521,10 @@
         <v>300</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="F31" s="14" t="s">
         <v>182</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B32" s="32" t="s">
         <v>301</v>
@@ -3543,12 +3543,12 @@
       <c r="D32" s="43"/>
       <c r="E32" s="44"/>
       <c r="F32" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="38" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B33" s="33" t="s">
         <v>303</v>
@@ -3568,7 +3568,7 @@
     </row>
     <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B34" s="33" t="s">
         <v>307</v>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="38" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B35" s="33" t="s">
         <v>311</v>
@@ -3608,7 +3608,7 @@
     </row>
     <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B36" s="33" t="s">
         <v>314</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="38" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B37" s="33" t="s">
         <v>317</v>
@@ -3637,7 +3637,7 @@
         <v>318</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>126</v>
@@ -3648,7 +3648,7 @@
     </row>
     <row r="38" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B38" s="32" t="s">
         <v>320</v>
@@ -3664,13 +3664,13 @@
     </row>
     <row r="39" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A39" s="38" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B39" s="33" t="s">
         <v>323</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>324</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A40" s="38" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B40" s="33" t="s">
         <v>326</v>
@@ -3693,7 +3693,7 @@
         <v>327</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>126</v>
@@ -3704,7 +3704,7 @@
     </row>
     <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="38" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B41" s="33" t="s">
         <v>328</v>
@@ -3724,7 +3724,7 @@
     </row>
     <row r="42" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="38" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B42" s="32" t="s">
         <v>331</v>
@@ -3740,13 +3740,13 @@
     </row>
     <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A43" s="38" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B43" s="33" t="s">
         <v>334</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>335</v>
@@ -3760,7 +3760,7 @@
     </row>
     <row r="44" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="38" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B44" s="33" t="s">
         <v>336</v>
@@ -3769,7 +3769,7 @@
         <v>337</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>338</v>
+        <v>719</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>40</v>
@@ -3780,19 +3780,19 @@
     </row>
     <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B45" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
+        <v>660</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>340</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>661</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>341</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>43</v>
@@ -3800,19 +3800,19 @@
     </row>
     <row r="46" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A46" s="38" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B46" s="33" t="s">
+        <v>341</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>662</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>342</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>663</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>662</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>343</v>
       </c>
       <c r="F46" s="14" t="s">
         <v>43</v>
@@ -3820,19 +3820,19 @@
     </row>
     <row r="47" spans="1:6" ht="108" x14ac:dyDescent="0.2">
       <c r="A47" s="38" t="s">
+        <v>624</v>
+      </c>
+      <c r="B47" s="33" t="s">
         <v>625</v>
       </c>
-      <c r="B47" s="33" t="s">
-        <v>626</v>
-      </c>
       <c r="C47" s="11" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>43</v>
@@ -3840,16 +3840,16 @@
     </row>
     <row r="48" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="38" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B48" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>346</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>277</v>
@@ -3860,13 +3860,13 @@
     </row>
     <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="38" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B49" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>347</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>348</v>
       </c>
       <c r="D49" s="14">
         <v>-8.73</v>
@@ -3880,19 +3880,19 @@
     </row>
     <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="38" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F50" s="14" t="s">
         <v>43</v>
@@ -3900,16 +3900,16 @@
     </row>
     <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="38" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B51" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>350</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>351</v>
-      </c>
       <c r="D51" s="14" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>94</v>
@@ -3920,19 +3920,19 @@
     </row>
     <row r="52" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="38" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B52" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>708</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>682</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>352</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>709</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>683</v>
-      </c>
-      <c r="E52" s="11" t="s">
-        <v>353</v>
       </c>
       <c r="F52" s="14" t="s">
         <v>182</v>
@@ -3940,16 +3940,16 @@
     </row>
     <row r="53" spans="1:6" ht="132" x14ac:dyDescent="0.2">
       <c r="A53" s="38" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>40</v>
@@ -3960,16 +3960,16 @@
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="38" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B54" s="33" t="s">
+        <v>354</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="14" t="s">
         <v>356</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>357</v>
       </c>
       <c r="E54" s="11" t="s">
         <v>181</v>
@@ -3980,16 +3980,16 @@
     </row>
     <row r="55" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A55" s="38" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B55" s="33" t="s">
+        <v>357</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>359</v>
-      </c>
       <c r="D55" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E55" s="11" t="s">
         <v>277</v>
@@ -4000,13 +4000,13 @@
     </row>
     <row r="56" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="38" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B56" s="33" t="s">
+        <v>359</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>360</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>361</v>
       </c>
       <c r="D56" s="14">
         <v>-8.73</v>
@@ -4020,19 +4020,19 @@
     </row>
     <row r="57" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="38" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F57" s="14" t="s">
         <v>43</v>
@@ -4040,19 +4040,19 @@
     </row>
     <row r="58" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="38" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B58" s="33" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F58" s="14" t="s">
         <v>43</v>
@@ -4060,16 +4060,16 @@
     </row>
     <row r="59" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A59" s="38" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B59" s="33" t="s">
+        <v>363</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>365</v>
-      </c>
       <c r="D59" s="21" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>143</v>
@@ -4080,35 +4080,35 @@
     </row>
     <row r="60" spans="1:6" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="38" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B60" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D60" s="43"/>
       <c r="E60" s="44"/>
       <c r="F60" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A61" s="38" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B61" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>650</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>692</v>
+      </c>
+      <c r="E61" s="11" t="s">
         <v>367</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>651</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>693</v>
-      </c>
-      <c r="E61" s="11" t="s">
-        <v>368</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>319</v>
@@ -4116,55 +4116,55 @@
     </row>
     <row r="62" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A62" s="38" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B62" s="33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C62" s="11" t="s">
+        <v>651</v>
+      </c>
+      <c r="D62" s="11" t="s">
         <v>652</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>653</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>143</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="38" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="44"/>
       <c r="F63" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="38" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D64" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="E64" s="11" t="s">
         <v>372</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>373</v>
       </c>
       <c r="F64" s="14">
         <v>1</v>
@@ -4172,16 +4172,16 @@
     </row>
     <row r="65" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A65" s="38" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>143</v>
@@ -4192,52 +4192,52 @@
     </row>
     <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="38" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B66" s="33" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C66" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="D66" s="11" t="s">
         <v>374</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>375</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>143</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="38" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B67" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="C67" s="42" t="s">
         <v>377</v>
-      </c>
-      <c r="C67" s="42" t="s">
-        <v>378</v>
       </c>
       <c r="D67" s="43"/>
       <c r="E67" s="44"/>
       <c r="F67" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A68" s="38" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B68" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="C68" s="11" t="s">
-        <v>381</v>
-      </c>
       <c r="D68" s="11" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>126</v>
@@ -4248,19 +4248,19 @@
     </row>
     <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="38" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F69" s="11" t="s">
         <v>43</v>
@@ -4268,16 +4268,16 @@
     </row>
     <row r="70" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A70" s="38" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B70" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>384</v>
-      </c>
       <c r="D70" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>143</v>
@@ -4288,16 +4288,16 @@
     </row>
     <row r="71" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A71" s="38" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B71" s="33" t="s">
+        <v>384</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="C71" s="11" t="s">
-        <v>386</v>
-      </c>
       <c r="D71" s="11" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>159</v>
@@ -4308,32 +4308,32 @@
     </row>
     <row r="72" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="38" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D72" s="43"/>
       <c r="E72" s="44"/>
       <c r="F72" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="38" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B73" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="D73" s="11" t="s">
         <v>389</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>688</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>390</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>40</v>
@@ -4344,16 +4344,16 @@
     </row>
     <row r="74" spans="1:6" ht="132" x14ac:dyDescent="0.2">
       <c r="A74" s="38" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B74" s="33" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>143</v>
@@ -4364,16 +4364,16 @@
     </row>
     <row r="75" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="38" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B75" s="33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>40</v>
@@ -4384,19 +4384,19 @@
     </row>
     <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="38" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B76" s="33" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="F76" s="11" t="s">
         <v>182</v>
@@ -4404,16 +4404,16 @@
     </row>
     <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="38" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B77" s="33" t="s">
+        <v>393</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="D77" s="11" t="s">
         <v>395</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>396</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>143</v>
@@ -4424,32 +4424,32 @@
     </row>
     <row r="78" spans="1:6" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="38" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B78" s="32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C78" s="42" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D78" s="43"/>
       <c r="E78" s="44"/>
       <c r="F78" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="38" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B79" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="D79" s="11" t="s">
         <v>400</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>401</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>40</v>
@@ -4460,19 +4460,19 @@
     </row>
     <row r="80" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A80" s="38" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B80" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="C80" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="D80" s="11" t="s">
+        <v>672</v>
+      </c>
+      <c r="E80" s="11" t="s">
         <v>403</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>673</v>
-      </c>
-      <c r="E80" s="11" t="s">
-        <v>404</v>
       </c>
       <c r="F80" s="14" t="s">
         <v>43</v>
@@ -4480,19 +4480,19 @@
     </row>
     <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="38" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B81" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="C81" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="D81" s="11" t="s">
+        <v>673</v>
+      </c>
+      <c r="E81" s="11" t="s">
         <v>406</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>674</v>
-      </c>
-      <c r="E81" s="11" t="s">
-        <v>407</v>
       </c>
       <c r="F81" s="14">
         <v>1</v>
@@ -4500,16 +4500,16 @@
     </row>
     <row r="82" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A82" s="38" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B82" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="C82" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="C82" s="11" t="s">
-        <v>409</v>
-      </c>
       <c r="D82" s="11" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>143</v>
@@ -4520,19 +4520,19 @@
     </row>
     <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="38" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B83" s="33" t="s">
+        <v>409</v>
+      </c>
+      <c r="C83" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="D83" s="25" t="s">
         <v>411</v>
       </c>
-      <c r="D83" s="25" t="s">
+      <c r="E83" s="11" t="s">
         <v>412</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>413</v>
       </c>
       <c r="F83" s="14">
         <v>1</v>
@@ -4540,16 +4540,16 @@
     </row>
     <row r="84" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A84" s="38" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B84" s="33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>40</v>
@@ -4560,32 +4560,32 @@
     </row>
     <row r="85" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="38" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C85" s="42" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D85" s="43"/>
       <c r="E85" s="44"/>
       <c r="F85" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="72" x14ac:dyDescent="0.2">
       <c r="A86" s="38" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B86" s="34" t="s">
+        <v>415</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>416</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>417</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>418</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>40</v>
@@ -4596,16 +4596,16 @@
     </row>
     <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="38" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B87" s="33" t="s">
+        <v>418</v>
+      </c>
+      <c r="C87" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="D87" s="21" t="s">
         <v>420</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>421</v>
       </c>
       <c r="E87" s="11" t="s">
         <v>143</v>
@@ -4616,19 +4616,19 @@
     </row>
     <row r="88" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="38" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B88" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>675</v>
+      </c>
+      <c r="D88" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="C88" s="11" t="s">
-        <v>676</v>
-      </c>
-      <c r="D88" s="11" t="s">
+      <c r="E88" s="11" t="s">
         <v>423</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>424</v>
       </c>
       <c r="F88" s="14" t="s">
         <v>43</v>
@@ -4636,16 +4636,16 @@
     </row>
     <row r="89" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A89" s="38" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B89" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="C89" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="C89" s="11" t="s">
-        <v>426</v>
-      </c>
       <c r="D89" s="11" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>143</v>
@@ -4656,19 +4656,19 @@
     </row>
     <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A90" s="38" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B90" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="C90" s="11" t="s">
-        <v>428</v>
-      </c>
       <c r="D90" s="11" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F90" s="14" t="s">
         <v>43</v>
@@ -4676,16 +4676,16 @@
     </row>
     <row r="91" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="38" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B91" s="33" t="s">
+        <v>428</v>
+      </c>
+      <c r="C91" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="D91" s="11" t="s">
         <v>430</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>431</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>143</v>
@@ -4696,19 +4696,19 @@
     </row>
     <row r="92" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A92" s="38" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B92" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="C92" s="11" t="s">
         <v>432</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="D92" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="D92" s="11" t="s">
-        <v>434</v>
-      </c>
       <c r="E92" s="11" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F92" s="14" t="s">
         <v>43</v>
@@ -4716,16 +4716,16 @@
     </row>
     <row r="93" spans="1:6" ht="108" x14ac:dyDescent="0.2">
       <c r="A93" s="38" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B93" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="C93" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="C93" s="11" t="s">
-        <v>436</v>
-      </c>
       <c r="D93" s="11" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>143</v>
@@ -4736,19 +4736,19 @@
     </row>
     <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" s="38" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B94" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="C94" s="11" t="s">
         <v>437</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="D94" s="26" t="s">
         <v>438</v>
       </c>
-      <c r="D94" s="26" t="s">
+      <c r="E94" s="11" t="s">
         <v>439</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>440</v>
       </c>
       <c r="F94" s="14" t="s">
         <v>43</v>
@@ -4756,16 +4756,16 @@
     </row>
     <row r="95" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="38" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B95" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="C95" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="D95" s="11" t="s">
         <v>442</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>443</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>40</v>
@@ -4776,19 +4776,19 @@
     </row>
     <row r="96" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A96" s="38" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B96" s="33" t="s">
+        <v>443</v>
+      </c>
+      <c r="C96" s="11" t="s">
         <v>444</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="D96" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="D96" s="21" t="s">
-        <v>446</v>
-      </c>
       <c r="E96" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F96" s="14" t="s">
         <v>43</v>
@@ -4796,16 +4796,16 @@
     </row>
     <row r="97" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A97" s="38" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B97" s="33" t="s">
+        <v>446</v>
+      </c>
+      <c r="C97" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="C97" s="11" t="s">
-        <v>448</v>
-      </c>
       <c r="D97" s="11" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>143</v>
@@ -4862,7 +4862,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B1" s="49" t="s">
         <v>1</v>
@@ -4874,10 +4874,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>4</v>
@@ -4904,7 +4904,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B4" s="46" t="s">
         <v>61</v>
@@ -4915,13 +4915,13 @@
     </row>
     <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>91</v>
@@ -4932,13 +4932,13 @@
     </row>
     <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>97</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>101</v>
@@ -4949,7 +4949,7 @@
     </row>
     <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>104</v>
@@ -4966,13 +4966,13 @@
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>111</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>127</v>
@@ -4983,7 +4983,7 @@
     </row>
     <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>130</v>
@@ -5000,7 +5000,7 @@
     </row>
     <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>133</v>
@@ -5017,7 +5017,7 @@
     </row>
     <row r="11" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>136</v>
@@ -5034,7 +5034,7 @@
     </row>
     <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>138</v>
@@ -5043,7 +5043,7 @@
         <v>139</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>94</v>
@@ -5051,7 +5051,7 @@
     </row>
     <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>140</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>146</v>
@@ -5085,13 +5085,13 @@
     </row>
     <row r="15" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>149</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>150</v>
@@ -5102,13 +5102,13 @@
     </row>
     <row r="16" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>151</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>150</v>
@@ -5119,13 +5119,13 @@
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>152</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>150</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>153</v>
@@ -5153,13 +5153,13 @@
     </row>
     <row r="19" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>156</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>157</v>
@@ -5170,7 +5170,7 @@
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>158</v>
@@ -5187,7 +5187,7 @@
     </row>
     <row r="21" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>165</v>
@@ -5204,7 +5204,7 @@
     </row>
     <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>171</v>
@@ -5221,7 +5221,7 @@
     </row>
     <row r="23" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>175</v>
@@ -5238,7 +5238,7 @@
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>179</v>
@@ -5249,7 +5249,7 @@
     </row>
     <row r="25" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>185</v>
@@ -5266,13 +5266,13 @@
     </row>
     <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>189</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>190</v>
@@ -5283,13 +5283,13 @@
     </row>
     <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>191</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>192</v>
@@ -5300,13 +5300,13 @@
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>193</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>195</v>
@@ -5317,13 +5317,13 @@
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>196</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>198</v>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="30" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>199</v>
@@ -5351,7 +5351,7 @@
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>209</v>
@@ -5368,7 +5368,7 @@
     </row>
     <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>214</v>
@@ -5383,7 +5383,7 @@
     </row>
     <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>218</v>
@@ -5400,7 +5400,7 @@
     </row>
     <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>222</v>
@@ -5417,7 +5417,7 @@
     </row>
     <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="30" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>226</v>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>229</v>
@@ -5451,13 +5451,13 @@
     </row>
     <row r="37" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B37" s="29" t="s">
         <v>232</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>233</v>
@@ -5468,7 +5468,7 @@
     </row>
     <row r="38" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="30" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B38" s="29" t="s">
         <v>234</v>
@@ -5485,7 +5485,7 @@
     </row>
     <row r="39" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="30" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B39" s="46" t="s">
         <v>236</v>
@@ -5496,10 +5496,10 @@
     </row>
     <row r="40" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>237</v>
@@ -5513,7 +5513,7 @@
     </row>
     <row r="41" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="30" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>240</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>244</v>
@@ -5547,7 +5547,7 @@
     </row>
     <row r="43" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>251</v>
@@ -5564,7 +5564,7 @@
     </row>
     <row r="44" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="30" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B44" s="29" t="s">
         <v>253</v>
@@ -5581,7 +5581,7 @@
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="30" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B45" s="29" t="s">
         <v>255</v>
@@ -5598,7 +5598,7 @@
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="30" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B46" s="29" t="s">
         <v>260</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A47" s="30" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B47" s="29" t="s">
         <v>263</v>
@@ -5632,7 +5632,7 @@
     </row>
     <row r="48" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A48" s="30" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B48" s="29" t="s">
         <v>268</v>
@@ -5649,7 +5649,7 @@
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A49" s="30" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B49" s="29" t="s">
         <v>271</v>
@@ -5700,10 +5700,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
@@ -5711,10 +5711,10 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
@@ -5744,7 +5744,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>9</v>
@@ -5783,7 +5783,7 @@
     </row>
     <row r="4" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>12</v>
@@ -5800,7 +5800,7 @@
     </row>
     <row r="5" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>20</v>
@@ -5817,7 +5817,7 @@
     </row>
     <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>24</v>
@@ -5834,7 +5834,7 @@
     </row>
     <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>27</v>
@@ -5851,7 +5851,7 @@
     </row>
     <row r="8" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>30</v>
@@ -5868,13 +5868,13 @@
     </row>
     <row r="9" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>35</v>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="10" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>37</v>
@@ -5902,7 +5902,7 @@
     </row>
     <row r="11" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>44</v>
@@ -5919,7 +5919,7 @@
     </row>
     <row r="12" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>48</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="13" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>52</v>
@@ -5953,7 +5953,7 @@
     </row>
     <row r="14" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>56</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="15" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>60</v>
@@ -5987,7 +5987,7 @@
     </row>
     <row r="16" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>65</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>69</v>
@@ -6021,7 +6021,7 @@
     </row>
     <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>74</v>
@@ -6038,7 +6038,7 @@
     </row>
     <row r="19" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>78</v>
@@ -6055,7 +6055,7 @@
     </row>
     <row r="20" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>82</v>
@@ -6072,7 +6072,7 @@
     </row>
     <row r="21" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>86</v>
@@ -6089,7 +6089,7 @@
     </row>
     <row r="22" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>90</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>96</v>
@@ -6123,7 +6123,7 @@
     </row>
     <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>102</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>109</v>
@@ -6157,7 +6157,7 @@
     </row>
     <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>114</v>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>118</v>
@@ -6191,7 +6191,7 @@
     </row>
     <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B28" s="29" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
Genotypes can be given in the material ID fields #61
</commit_message>
<xml_diff>
--- a/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
+++ b/MIAPPE_Checklist-Data-Model-v1.1/MIAPPE_Checklist-Data-Model-v1.1.xlsx
@@ -744,7 +744,8 @@
     <t xml:space="preserve">Material source ID (Holding institute/stock centre, accession)</t>
   </si>
   <si>
-    <t xml:space="preserve">An identifier for the source of the biological material, in the form of a key-value pair comprising the name/identifier of the repository from which the material was sourced plus the accession number of the repository for that material. Where an accession number has not been assigned, but the material has been derived from the crossing of known accessions, the material can be defined as follows: "mother_accession X father_accession", or, if father is unknown, as "mother_accession X UNKNOWN". For in situ material, the region of provenance may be used when an accession is not available.</t>
+    <t xml:space="preserve">An identifier for the source of the biological material, in the form of a key-value pair comprising the name/identifier of the repository from which the material was sourced plus the accession number of the repository for that material. Where an accession number has not been assigned, but the material has been derived from the crossing of known accessions, the material can be defined as follows: "mother_accession X father_accession", or, if father is unknown, as "mother_accession X UNKNOWN". For in situ material, the region of provenance may be used when an accession is not available. 
+The Material source is commonly called germplasm, accession, genotype and even variety for commercial varieties. For the latest, keep in mind that a variety is commonly ambiguously identified and polysemous</t>
   </si>
   <si>
     <t xml:space="preserve">INRA:W95115_inra
@@ -2449,64 +2450,68 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2514,103 +2519,103 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2694,1903 +2699,1903 @@
   </sheetPr>
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B47" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="41.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="11" t="n">
+      <c r="D7" s="12" t="n">
         <v>41260</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="10" t="n">
+      <c r="F10" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="11" t="n">
+      <c r="D17" s="12" t="n">
         <v>37587</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="10" t="n">
+      <c r="F18" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="10" t="n">
+      <c r="F19" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="10" t="n">
+      <c r="F20" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="F27" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="10" t="n">
+      <c r="F28" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7" t="s">
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="F33" s="10" t="n">
+      <c r="F33" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="11" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="11" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7" t="s">
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="F39" s="10" t="n">
+      <c r="F39" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="10" t="n">
+      <c r="F40" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7" t="s">
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="10" t="n">
+      <c r="F43" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="10" t="n">
+      <c r="F44" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="D49" s="10" t="n">
+      <c r="D49" s="11" t="n">
         <v>-8.73</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+    <row r="53" customFormat="false" ht="136.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E54" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F54" s="10" t="s">
+      <c r="F54" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="D56" s="10" t="n">
+      <c r="D56" s="11" t="n">
         <v>-8.73</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="F57" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E58" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F58" s="10" t="s">
+      <c r="F58" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F59" s="10" t="s">
+      <c r="F59" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7" t="s">
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F61" s="10" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B62" s="8" t="s">
+      <c r="B62" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F62" s="9" t="s">
+      <c r="F62" s="10" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7" t="s">
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="14" t="s">
         <v>275</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D64" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="F64" s="10" t="n">
+      <c r="F64" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D65" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E65" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F65" s="9" t="s">
+      <c r="F65" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="F66" s="10" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7" t="s">
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="8" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B68" s="8" t="s">
+      <c r="B68" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="E68" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F68" s="10" t="n">
+      <c r="F68" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="C69" s="9" t="s">
+      <c r="C69" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D69" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="E69" s="9" t="s">
+      <c r="E69" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="E70" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D71" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="E71" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="10" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7" t="s">
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="C73" s="9" t="s">
+      <c r="C73" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E73" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F73" s="10" t="n">
+      <c r="F73" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D74" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E74" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F74" s="10" t="n">
+      <c r="F74" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C75" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D75" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E75" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F75" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C76" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="D76" s="13" t="s">
+      <c r="D76" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C77" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D77" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F77" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7" t="s">
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="C79" s="9" t="s">
+      <c r="C79" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="E79" s="9" t="s">
+      <c r="E79" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F79" s="10" t="n">
+      <c r="F79" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="C80" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D80" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="E80" s="9" t="s">
+      <c r="E80" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="F80" s="10" t="s">
+      <c r="F80" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D81" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="E81" s="9" t="s">
+      <c r="E81" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="F81" s="10" t="n">
+      <c r="F81" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="D82" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E82" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F82" s="10" t="s">
+      <c r="F82" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C83" s="10" t="s">
         <v>357</v>
       </c>
-      <c r="D83" s="19" t="s">
+      <c r="D83" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="E83" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="F83" s="10" t="n">
+      <c r="F83" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="D84" s="9" t="s">
+      <c r="D84" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="E84" s="9" t="s">
+      <c r="E84" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F84" s="10" t="s">
+      <c r="F84" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B85" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="7" t="s">
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="B86" s="20" t="s">
+      <c r="B86" s="21" t="s">
         <v>366</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C86" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="D86" s="9" t="s">
+      <c r="D86" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="E86" s="9" t="s">
+      <c r="E86" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F86" s="10" t="n">
+      <c r="F86" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="C87" s="9" t="s">
+      <c r="C87" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="D87" s="13" t="s">
+      <c r="D87" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="E87" s="9" t="s">
+      <c r="E87" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F87" s="10" t="s">
+      <c r="F87" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B88" s="21" t="s">
         <v>374</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="D88" s="9" t="s">
+      <c r="D88" s="10" t="s">
         <v>376</v>
       </c>
-      <c r="E88" s="9" t="s">
+      <c r="E88" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="F88" s="10" t="s">
+      <c r="F88" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="B89" s="20" t="s">
+      <c r="B89" s="21" t="s">
         <v>379</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C89" s="10" t="s">
         <v>380</v>
       </c>
-      <c r="D89" s="9" t="s">
+      <c r="D89" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="E89" s="9" t="s">
+      <c r="E89" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F89" s="10" t="n">
+      <c r="F89" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="B90" s="20" t="s">
+      <c r="B90" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="C90" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="D90" s="9" t="s">
+      <c r="D90" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="E90" s="9" t="s">
+      <c r="E90" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="F90" s="10" t="s">
+      <c r="F90" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C91" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="D91" s="9" t="s">
+      <c r="D91" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="E91" s="9" t="s">
+      <c r="E91" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F91" s="10" t="n">
+      <c r="F91" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C92" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="D92" s="9" t="s">
+      <c r="D92" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="E92" s="9" t="s">
+      <c r="E92" s="10" t="s">
         <v>386</v>
       </c>
-      <c r="F92" s="10" t="s">
+      <c r="F92" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="108" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="B93" s="21" t="s">
+      <c r="B93" s="22" t="s">
         <v>396</v>
       </c>
-      <c r="C93" s="9" t="s">
+      <c r="C93" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="D93" s="9" t="s">
+      <c r="D93" s="10" t="s">
         <v>398</v>
       </c>
-      <c r="E93" s="9" t="s">
+      <c r="E93" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F93" s="10" t="s">
+      <c r="F93" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="B94" s="8" t="s">
+      <c r="B94" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="10" t="s">
         <v>401</v>
       </c>
-      <c r="D94" s="22" t="s">
+      <c r="D94" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="E94" s="9" t="s">
+      <c r="E94" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="F94" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="C95" s="9" t="s">
+      <c r="C95" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="D95" s="9" t="s">
+      <c r="D95" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="E95" s="9" t="s">
+      <c r="E95" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F95" s="10" t="n">
+      <c r="F95" s="11" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="B96" s="8" t="s">
+      <c r="B96" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C96" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="D96" s="13" t="s">
+      <c r="D96" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="E96" s="9" t="s">
+      <c r="E96" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="F96" s="10" t="s">
+      <c r="F96" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="B97" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="C97" s="9" t="s">
+      <c r="C97" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="D97" s="9" t="s">
+      <c r="D97" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="E97" s="9" t="s">
+      <c r="E97" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F97" s="10" t="s">
+      <c r="F97" s="11" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4636,814 +4641,814 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>416</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>419</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>422</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>423</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>424</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>425</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="24" t="s">
         <v>428</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="31" t="s">
         <v>429</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>432</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="31" t="s">
         <v>433</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>435</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>436</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>437</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="33" t="s">
         <v>438</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="32" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>441</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="31" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="D9" s="33" t="n">
+      <c r="D9" s="34" t="n">
         <v>16</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="24" t="s">
         <v>444</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="31" t="s">
         <v>445</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>448</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="31" t="s">
         <v>449</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="24" t="s">
         <v>451</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="31" t="s">
         <v>452</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="24" t="s">
         <v>455</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="31" t="s">
         <v>456</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="35" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="24" t="s">
         <v>459</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="31" t="s">
         <v>460</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="24" t="s">
         <v>463</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>464</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="24" t="s">
         <v>467</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="31" t="s">
         <v>468</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="24" t="s">
         <v>470</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="31" t="s">
         <v>471</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>473</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="31" t="s">
         <v>474</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>477</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>478</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="32" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>481</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>482</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>485</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="31" t="s">
         <v>486</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>487</v>
       </c>
-      <c r="D21" s="36" t="n">
+      <c r="D21" s="37" t="n">
         <v>0.3</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>488</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="31" t="s">
         <v>489</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>492</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>493</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D23" s="36" t="n">
+      <c r="D23" s="37" t="n">
         <v>0.33</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="24" t="s">
         <v>495</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>496</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>497</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="31" t="s">
         <v>498</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>499</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="10" t="s">
         <v>500</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="32" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="24" t="s">
         <v>502</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="31" t="s">
         <v>503</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="32" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>506</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="31" t="s">
         <v>507</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="10" t="s">
         <v>508</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="24" t="s">
         <v>510</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="31" t="s">
         <v>511</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="35" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="24" t="s">
         <v>514</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="31" t="s">
         <v>515</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="10" t="s">
         <v>517</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="35" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="24" t="s">
         <v>518</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="31" t="s">
         <v>519</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>520</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="10" t="s">
         <v>521</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="35" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>523</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="31" t="s">
         <v>524</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>525</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="10" t="s">
         <v>526</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="35" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="24" t="s">
         <v>528</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="31" t="s">
         <v>529</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>530</v>
       </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="31" t="s">
+      <c r="D32" s="33"/>
+      <c r="E32" s="32" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="36" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="24" t="s">
         <v>531</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="31" t="s">
         <v>532</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="32" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="24" t="s">
         <v>535</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="31" t="s">
         <v>536</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>537</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="24" t="s">
         <v>539</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="31" t="s">
         <v>540</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>541</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="10" t="s">
         <v>542</v>
       </c>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="31" t="s">
         <v>544</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="10" t="s">
         <v>545</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="24" t="s">
         <v>547</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="31" t="s">
         <v>548</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="10" t="s">
         <v>550</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E37" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="24" t="s">
         <v>551</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="31" t="s">
         <v>552</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="10" t="s">
         <v>553</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="24" t="s">
         <v>554</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="30" t="s">
         <v>555</v>
       </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
     </row>
     <row r="40" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="24" t="s">
         <v>556</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="31" t="s">
         <v>557</v>
       </c>
-      <c r="C40" s="34" t="s">
+      <c r="C40" s="35" t="s">
         <v>558</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="35" t="s">
         <v>559</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="32" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="31" t="s">
         <v>562</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="35" t="s">
         <v>563</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="35" t="s">
         <v>564</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="32" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="24" t="s">
         <v>566</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="31" t="s">
         <v>567</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="35" t="s">
         <v>568</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="35" t="s">
         <v>569</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="32" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="24" t="s">
         <v>571</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="31" t="s">
         <v>572</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="35" t="s">
         <v>573</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="35" t="s">
         <v>559</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="32" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="24" t="s">
         <v>574</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="31" t="s">
         <v>575</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="35" t="s">
         <v>575</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="35" t="s">
         <v>564</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="32" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="24" t="s">
         <v>576</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="31" t="s">
         <v>577</v>
       </c>
-      <c r="C45" s="34" t="s">
+      <c r="C45" s="35" t="s">
         <v>578</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D45" s="35" t="s">
         <v>509</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="31" t="s">
         <v>580</v>
       </c>
-      <c r="C46" s="34" t="s">
+      <c r="C46" s="35" t="s">
         <v>581</v>
       </c>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="35" t="s">
         <v>582</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="32" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="24" t="s">
         <v>583</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="31" t="s">
         <v>584</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="35" t="s">
         <v>585</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="35" t="s">
         <v>586</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="32" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="24" t="s">
         <v>587</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="31" t="s">
         <v>588</v>
       </c>
-      <c r="C48" s="34" t="s">
+      <c r="C48" s="35" t="s">
         <v>589</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="35" t="s">
         <v>559</v>
       </c>
-      <c r="E48" s="31" t="s">
+      <c r="E48" s="32" t="s">
         <v>560</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="24" t="s">
         <v>590</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="31" t="s">
         <v>591</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="35" t="s">
         <v>592</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="35" t="s">
         <v>593</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="32" t="s">
         <v>225</v>
       </c>
     </row>
@@ -5478,514 +5483,514 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>594</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>595</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>596</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>597</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>598</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>599</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
     </row>
     <row r="4" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>600</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="31" t="s">
         <v>601</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="32" t="s">
         <v>602</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="32" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>605</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>606</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="32" t="s">
         <v>607</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>608</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="32" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="24" t="s">
         <v>610</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="31" t="s">
         <v>611</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="32" t="s">
         <v>612</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="32" t="s">
         <v>613</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="32" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>614</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="31" t="s">
         <v>615</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="32" t="s">
         <v>616</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="32" t="s">
         <v>617</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="32" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>618</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>619</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="32" t="s">
         <v>620</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="32" t="s">
         <v>621</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="32" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="24" t="s">
         <v>623</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="31" t="s">
         <v>624</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="32" t="s">
         <v>625</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="32" t="s">
         <v>626</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="32" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="24" t="s">
         <v>628</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="31" t="s">
         <v>629</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="32" t="s">
         <v>630</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="32" t="s">
         <v>631</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="32" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="24" t="s">
         <v>633</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="31" t="s">
         <v>634</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="32" t="s">
         <v>635</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="32" t="s">
         <v>636</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="32" t="s">
         <v>637</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="24" t="s">
         <v>638</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="31" t="s">
         <v>639</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="32" t="s">
         <v>640</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="32" t="s">
         <v>641</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="32" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="24" t="s">
         <v>643</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="31" t="s">
         <v>644</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="32" t="s">
         <v>645</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="32" t="s">
         <v>646</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="32" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="24" t="s">
         <v>648</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="31" t="s">
         <v>649</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="32" t="s">
         <v>650</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="32" t="s">
         <v>651</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="32" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="24" t="s">
         <v>653</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>654</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="32" t="s">
         <v>655</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="32" t="s">
         <v>656</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="32" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="24" t="s">
         <v>658</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="31" t="s">
         <v>659</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="32" t="s">
         <v>660</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="32" t="s">
         <v>661</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="32" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="24" t="s">
         <v>663</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="31" t="s">
         <v>664</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="32" t="s">
         <v>665</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="32" t="s">
         <v>666</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="32" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>668</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="31" t="s">
         <v>669</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="32" t="s">
         <v>670</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="32" t="s">
         <v>671</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="32" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>673</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>674</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="32" t="s">
         <v>675</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="32" t="s">
         <v>676</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="32" t="s">
         <v>677</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>678</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="31" t="s">
         <v>679</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="32" t="s">
         <v>680</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="32" t="s">
         <v>681</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="32" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>683</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="31" t="s">
         <v>684</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="32" t="s">
         <v>685</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="32" t="s">
         <v>686</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="32" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>688</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="31" t="s">
         <v>689</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="32" t="s">
         <v>690</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="32" t="s">
         <v>691</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="32" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>693</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>694</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="32" t="s">
         <v>695</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="32" t="s">
         <v>696</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="32" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="24" t="s">
         <v>698</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="31" t="s">
         <v>699</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="32" t="s">
         <v>700</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="32" t="s">
         <v>701</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="32" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>703</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="31" t="s">
         <v>704</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="32" t="s">
         <v>705</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="32" t="s">
         <v>706</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="32" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="24" t="s">
         <v>708</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="31" t="s">
         <v>709</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="32" t="s">
         <v>710</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="32" t="s">
         <v>711</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="32" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>713</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="31" t="s">
         <v>714</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="32" t="s">
         <v>715</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="32" t="s">
         <v>716</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="32" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="24" t="s">
         <v>718</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="31" t="s">
         <v>719</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="31" t="s">
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="32" t="s">
         <v>440</v>
       </c>
     </row>

</xml_diff>